<commit_message>
Fix minor issues; Improve Randomforest;
</commit_message>
<xml_diff>
--- a/TrainingEminDataSet.xlsx
+++ b/TrainingEminDataSet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
   <si>
     <t xml:space="preserve">Descriptions</t>
   </si>
@@ -185,6 +185,186 @@
   </si>
   <si>
     <t xml:space="preserve">Global Marketing Manager, Zurich Resilience Solutions, 100% Zurich Resilience Solutions helps customers identify, assess, reduce and/or build resilience against cyber, climate and other risks. Do you want to be part of executing an exciting global growth plan for consultancy services in this area? Are you looking for a new challenge? We are looking for a Senior Marketing Manager to join the team.        As the Global Marketing Manager, you will develop and execute the marketing plans and programs to achieve our business goals. Reporting into a ZRS leader, you will lead the development and coordination of our global and local marketing efforts.        What you will do        Some of your key responsibilities include:                      Development and execution of a strategy to increase market awareness of ZRS as a best-in-class consultant of risk management services for traditional as well as emerging risks.                 Works with our global and local business leaders and subject matter experts to develop and implement a comprehensive marketing strategy.                 Identify opportunities (like forum publications, conferences, social media etc.) to increase market awareness of our advisory services.                 Establish and run our external though leadership and education Academy for (potential) customers and partners.                 Web site optimisation and management.                 Identify and recommend alternative marketing and social media opportunities.                 Event planning.                 Customer and stakeholder mapping (internal and external).                 Understanding of our key competitors.                 Co-ordination between the central function and local ZRS Unit activity.             What you bring                    Strong track record of successfully developing and executing global marketing strategies, preferably in the services / consultancy industry.                 Minimum 5 years in a similar global role.                 Experience running large scope projects with cross-over departments and large teams.                 Extensive social media expertise.                 Extensive experience and use of search engine optimization.                 Self-starter and do-er. Strong executor.                 Innovative creator of a new brand (“resilience solutions beyond insurance”).                 Strong analytical skills.                 Strong negotiation and influencing skills.                 Ability to build and maintain strong relationships.             Additional Information           We look forward to receiving your online application.             Zurich wants to attract the best talent and we acknowledge that talents might not always be available full-time. At Zurich we will consider requests for flexible working. Many of our employees work flexibly in a variety of ways. Please talk to us during the interview about the flexibility you may need.             Explore our new Quai Zurich Campus        Information for recruitment agencies             Zurich does not accept any applications from recruitment agencies for this position. We refuse any responsibility for unsolicited applications as well as any associated fees.             Why Zurich             At Zurich, we like to think outside the box and challenge the status quo. We take an optimistic approach by focusing on the positives and constantly asking What can go right?        We are an equal opportunity employer who knows that each employee is unique - that’s what makes our team so great!    Join us as we constantly explore new ways to protect our customers and the planet.           Location(s): CH - Zürich    Remote working:    Schedule: Full Time    Recruiter name: Christopher Parkinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business Intelligence Director Ref: BBBH4772              Location. London     Salary. Bonus, Pension     Type. Permanent           Job Description.    Global BI Director:    We are seeking a Global Business Intelligence Director to shape our future strategy and lead the design and development of core data and reporting applications. Collaborating with the Head of Systems and Integration and the Enterprise Architect, you will identify company needs, build fully automated dashboards, create our first Enterprise Data Warehouse, and execute the full strategy. You will oversee data standards and repositories to support business needs.            5 Days a week on-site in Victoria     up to 20% bonus     £7 a day contributory lunch allowance          Key Responsibilities:            Define solution architecture and delivery for data standards across all company applications, systems, and platforms.     Ensure application software aligns with data standards and reporting strategy.     Understand business processes, systems, tools, regulations, and structure to provide valuable intelligence and reporting services.     Oversee information design for application software and continuous improvement initiatives.     Manage design, coding, verification, testing, documentation, amendments, and refactoring of programs/scripts.     Approve database specifications, maintaining standards and data integrity.     Install and test complex databases and products to meet internal and customer requirements.     Design and select critical storage, data center, and client/server environments in line with industry best practices, and provide third-line escalation for global infrastructure solutions.     Redesign complex software applications or components using agreed standards, patterns, and tools.     Produce specifications for cloud-based or on-premise components for detailed design.     Support change programs or projects with technical plans adhering to enterprise and solution architecture standards, including security.     Evaluate alternative architectures for cost, performance, and scalability.     Monitor emerging technologies to assess potential impacts, threats, and opportunities.     Document and present solutions to stakeholders, including business and technical design authorities.     Evaluate potential risks and defects, analyze specifications, and customize applications.     Define and manage technology governance processes for the Information and Data landscape.     Produce documentation for application architecture, design steps, integration processes, and testing procedures.           Technical Experience required:            Strong knowledge of architecture and data methodologies, principles and frameworks.     A strong familiarity working with data platforms especially SQL server and PowerBI are a must have.           Diversity, equity and inclusion are at the heart of what we value as an organisation. Boston Hale is an equal opportunities employer and all qualified applicants will receive consideration for employment without regard to race, religion, sex, sexual orientation, age, disability or any other status protected by law.    If you are able to operate across the top-level of an organisation, have an enthusiastic and positive attitude and can explain the complicated in simple terms whilst driving a Global Organisation's BI environment towards best in class technologies and Best Practices, then please get in touch ASAP                      David Pynor      Head of Data &amp; Technology      +44 (0)20 3587 7905      dpynor@bostonhale.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linux Cryptography and Security Engineer This is a unique opportunity to use your software engineering and cryptography skills to build and maintain the security foundation that enables Ubuntu and its users to operate securely and remain compliant to international information security standards such as FIPS 140-3 and Common Criteria. You will use your applied cryptography, Linux Security, and coding skills to enhance the Ubuntu distribution and work with organizations such as DISA and CIS to draft and implement security hardening benchmarks for Ubuntu.As a member of the Security Hardening team you will work with and develop automation tooling to audit deployed systems for DISA-STIG and CIS benchmark compliance. You will interact with internal and external stakeholders to identify gaps in our frameworks, and develop new solutions to address these challenges. In this role you will have the opportunity to influence team and security culture, facilitate technical delivery, and help drive team direction and execution. You'll collaborate closely with Canonical's kernel team as well as the wider engineering organization to drive features impacting all Ubuntu users.Day-to-day responsibilitiesCollaborate with other engineers in the Security Hardening team to achieve and retain various Security certificationsExtend and enhance Linux cryptographic components (OpenSSL, Libgcrypt, GnuTLS, and others) with the features and functionality required for FIPS and CC certificationCollaborate with external security consultants to test and validate kernel and crypto module componentsWork with external partners to develop security hardening benchmarks and audit + remediation automation for UbuntuContribute to Ubuntu mainline and upstream projects to land solutions and benefit the communityCommunication and collaboration within and outside Canonical to identify opportunities to improve our security posture, rapidly resolve issues, and deliver high-quality solutions on scheduleWhat we are looking for in youHands-on experience with low-level Linux cryptography APIs and debuggingExcellent software engineering fundamentals, including prior experience with C development, and the ability to demonstrate suchHands-on experience with Linux system administration and shell scriptingDemonstrated knowledge of security and cryptography fundamentals + direct experience writing secure code and implementing best practicesSignificant development experience working with open source librariesExcellent verbal and written communications to enable efficient collaboration with internal and external partners in a remote-first environmentAdditional Skills That You Might Also BringPrior experience working on FIPS/Common Criteria certified products and in-depth knowledge of the underlying standardsPrior experience working directly with DISA-STIG or CIS benchmarks, including related audit + remediation tooling (e.g. Compliance as Code)Experience working directly with Linux KernelPrior experience with Python, OVAL (Open Vulnerability Assessment Language), and AnsibleHistory of contributions to open source projectsWhat we offer youWe consider geographical location, experience, and performance in shaping compensation worldwide. We revisit compensation annually (and more often for graduates and associates) to ensure we recognise outstanding performance. In addition to base pay, we offer a performance-driven annual bonus. We provide all team members with additional benefits, which reflect our values and ideals. We balance our programs to meet local needs and ensure fairness globally.Distributed work environment with twice-yearly team sprints in person - we've been working remotely since 2004!Personal learning and development budget of USD 2,000 per yearAnnual compensation reviewRecognition rewardsAnnual holiday leaveMaternity and paternity leaveEmployee Assistance ProgrammeOpportunity to travel to new locations to meet colleagues from your team and othersPriority Pass for travel and travel upgrades for long haul company eventsAbout CanonicalCanonical is a pioneering tech firm that is at the forefront of the global move to open source. As the company that publishes Ubuntu, one of the most important open source projects and the platform for AI, IoT and the cloud, we are changing the world on a daily basis. We recruit on a global basis and set a very high standard for people joining the company. We expect excellence - in order to succeed, we need to be the best at what we do.Canonical has been a remote-first company since its inception in 2004. Work at Canonical is a step into the future, and will challenge you to think differently, work smarter, learn new skills, and raise your game. Canonical provides a unique window into the world of 21st-century digital business.Canonical is an equal opportunity employerWe are proud to foster a workplace free from discrimination. Diversity of experience, perspectives, and background create a better work environment and better products. Whatever your identity, we will give your application fair consideration.                                                                Show more                                                                                      Show less Information Technology Technology, Information and Internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecommerce Conversion Rate Optimization Manager Since our founding in 2018, Verbolia has experienced rapid international growth and achieved remarkable success. We earned the title of Belgian Startup of the Year in 2021 and have been honoured with numerous awards, including the IAB MIXX Award for the 'Best MarkAd-Tech Tools' and the Digital Wallonia Startup of the Year award. Most recently, we were recognized as Deloitte's 2023 Fast 500 EMEA winner, further establishing our position as a leader in the digital marketing space.    For our new product called Vmax, we're looking for an Ecommerce Conversion Rate Optimization Manager to help our customers, which are large e-commerce websites, drive paid campaigns’ conversion rates and profitability. We are seeking a result-driven conversion rate optimization manager.    The ideal candidate will be passionate about leveraging data and insights to improve conversion rates. This role will be a great fit for you if you are data-driven, passionate about e-commerce and conversion rate optimization, and with excellent communication skills for internal collaboration and client relationships.    Tasks    In this role, you will        use your analytics expertise to conduct experiments and analyse results for our customers.   plan, prioritise, and manage A/B tests, multivariate tests, and other experimentation initiatives to validate hypotheses and drive continuous improvement for our customers.   collaborate closely with Customer Success and Sales to implement test strategies and make sure learnings are shared across the whole company.   collaborate closely with Product to make sure Vmax provides our customers with the needed web analytics, heatmaps and merchandising insights to continuously improve conversion rates and engagement.   Stay informed about industry trends, best practices, and emerging technologies in CRO and web optimization for e-commerce.   Champion a culture of experimentation and build a knowledge base as we grow the number of experiments we do for our customers.   Requirements    Skills and experience        Proven experience (3-5 years) in conversion rate optimization, digital marketing, or related roles, with a track record of driving measurable improvements in conversion rates and website performance in e-commerce.   Strong analytical skills, with the ability to interpret data, draw actionable insights, and make data-driven recommendations.   Proficiency in web analytics tools such as Google Analytics, as well as experience with A/B testing platforms and other CRO tools.   Excellent project management skills, with the ability to prioritise tasks, manage multiple projects simultaneously, and meet deadlines in a fast-paced environment.   Exceptional communication and collaboration skills, with the ability to work effectively across cross-functional teams and influence stakeholders at all levels of the organisation.   Creative problem-solving abilities, with a passion for experimenting, testing hypotheses, and continuously optimising digital experiences.   Knowledge of UX principles, web design best practices, SEO fundamentals, and other factors impacting website performance and user behaviour.   Ability to take initiative and adapt.   Fluent in English, any other languages are assets.   Benefits    What we offer        Be part of an international start-up environment that is just at the beginning of a bright future   A high degree of independence, responsibility, and impact on business operations   A competitive salary with plenty of fringe benefits, a company car, a mobile subscription, 5 extra holidays, meal vouchers, a group and hospitalisation insurance   A hybrid working model, a good mix of home and office working   It is truly important to us that each team member is happy in the team, with interesting challenges, a good understanding of their contribution to the company, a nice environment, a super flexible home working policy,...    When recruiting a new team member, we’ll always focus primarily on:        company culture fit: be trustworthy, friendly, willing to help   adaptability: be ready to evolve along with the company   being solution-oriented: never come up with a problem, always come up with a solution to a problem   Join a start-up company that takes care of its people:      yearly team building celebrating our successes   quarterly team activities focusing on fun   monthly lunches, just because we're hungry sometimes   weekly fresh fruits to stay healthy   daily collaboration with fantastic colleagues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales Trainer David Kennedy Recruitment is working with a "Top Workplace" tech business outsourcing company who is looking to hire a Sales Trainer. As a Sales Trainer, you will play a vital role in designing, delivering, and evaluating training programs to enhance the knowledge and skills of our employees. The ideal candidate should be passionate about employee learning, possess excellent communication skills, and have a strong ability to engage and motivate learners.      Position: Sales Trainer    Location: Dublin, Republic of Ireland    Employment type: Full-time    Remuneration: Base salary + bonus       DUTIES AND RESPONSIBILITIES:       Develop effective onboarding and training plans for new employees    Develop effective 90-day ramping plans    Create comprehensive training materials and modules that cover sales techniques, product knowledge, and company policies    Tailor training sessions to meet the specific needs of the sales team and address gaps in skills or knowledge    Lead interactive workshops and seminars to teach sales strategies, objection handling, and closing techniques    Provide personalized coaching to individual sales representatives to enhance their performance and address specific challenges    Monitor the progress of members of the sales team through assessments, role-plays, and performance reviews    Analyze sales data and performance metrics to identify areas where the team or individual members need further development    Design competency frameworks for key roles    Design and maintain 6-month rolling training calendar with a combination of online and live training suitable for various levels and roles    Serve as product and service subject matter expert with an acute understanding of the client’s value proposition from both a technical and business prospective new clients    Understand the competitive landscape and coach reps to win         REQUIREMENTS:       2+ years of experience in a sales training role; experience with SaaS, IT Services, or system integrator spaces preferred.    Successful track record in designing training programs, delivering training content, and engaging with training cohorts both in-person and remotely.    Bachelor's degree or equivalent experience in sales, marketing, business, or related field preferred    Strong sales expertise including in-depth knowledge of various sales methodologies (SPIN, Challenger, Sandler, Winning by Design, etc) and an ability to provide real-world examples and insights from own hands-on experience.    Ability to engage with and motivate sales professionals of all levels of experience and tenure.    Utilize strong analytical and assessment skills to evaluate data, identify trends, and make strategic recommendations for continuous improvement and decision-making.    Strong communication and presenting skills supported by an energetic and engaging attitude    Ability to be flexible and agile in responding to evolving business priorities and dealing with ambiguity    Ability to work within a group as a collaborative team player, partnering across the organization and with internal and external stakeholders.    Tech-savvy with an affinity for innovative and emerging technology    Self-reliant, adaptable, decisive, and professional; able to effectively multi-task in a dynamic environment    Fluent English Speaker with additional language a benefit    Proficient in basic computer skills, Microsoft Office, GSuite, and general sales tools such as CRMs.        OFFER:       Comprehensive VHI Health cover from day one    Structured training &amp; career development opportunities    Education reimbursement    Paid birthday leave    Child/Dependent care reimbursement    Personal Hardship Loan Program    Mental health and 24/7 employee assistance program    Bike To Work Scheme / Taxsaver Leap Card Scheme    Top-performer and tenure awards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senior Test Automation Engineer The Opportunity:    The Automation Platform Team is responsible for evolving our test automation framework and our internal test tooling. The main ethos of the Automation Platform team is to make testing easier for the feature application teams. We do this by continuing to adapt and improve our test automation framework and adding the correct functionality to our internal tooling.    The successful candidate will work closely with other members of the quality team and with the wider ESW organisation to identify ways to enhance our automation strategy, framework, and tooling.         Key Responsibilities      Continue to evolve our Test Automation and testing related tooling solutions.    Work with key stakeholders to identify and drive innovations to improve our overall approach to our internal test tooling.    Working with the feature teams to ensure the strategy and frameworks suit their needs.    Develop new capabilities for our internal testing application as required.    Ensure code quality and test coverage.    Continuously strive to introduce improvements and innovations to the team.           Key Experience &amp; Skills:      Experience with writing code in Typescript or JavaScript (ES6).    Proven experience writing and extending automation test frameworks.    Experience with using design patterns suitable for building scalable and maintainable test automation.    Experience with Selenium, or frameworks such as Webdriver.io or Playwright.    Experience with web development, with frameworks such as Angular.    Experience in a continuous delivery environment.    Good understanding of general testing approaches and automation strategies.    Strong critical thinking and problem-solving skills.    Excellent communication and influencing skills.    Demonstrable experience of staying up to date with changes and trends in industry.    Solid understanding of software development approaches of an agile nature    Self-motivated.    Knowledge of when and when not to use automation in testing.     What's on offer?      Competitive salary and a career path adapted to each person's abilities and experience within a company that is growing continuously.    2 days a week working from home.    A flexible schedule and total conciliation between work and family life including reduced timetable during one month in summer.    Become part of a multi-cultural company where you can contribute with your experience and learn from the experience of others.    Work with amazing brands.    Get the opportunity to influence the future of our services and platform.    Excellent working environment with frequent social activities (hackathons, Spartan races, quarterly whole-team social event).    Central Madrid office located an 8-minute walk from Atocha train station, with a bus stop and BiciMad station right outside the office.    Kitchen and dining facilities as well as a fully stocked games room with games consoles etc. - great to disconnect from work for a while and have fun with your colleagues.    Discounted parking space in the office building if you're coming by car, bicycle parking for those worried about their carbon footprint.    Access to private sales by some of the exclusive brands we work with.    Enrollment in English, French, and Spanish lessons that take place during working hours.    Mental Health Wellbeing Program.          About us:     ESW is the leading global and domestic direct-to-consumer (DTC) ecommerce company, empowering the world's best-loved brands to create safer, simpler and faster shopping experiences for consumers all around the globe. ESW acquired Scalefast in June 2022, and the combined 1,300 person organization offers brands and retailers a complete portfolio of technology and services that cost-effectively support any stage of company's development.     From compliance, data security, fraud protection, taxes and tariffs to demand generation, checkout, delivery, returns and customer service, our powerful combination of technology and human ingenuity covers the entire shopper journey across 200 markets, with 100% carbon neutral shipping to consumers. Headquartered in Dublin, Ireland, ESW has global offices in the US, UK, Spain, France, Italy, Japan, Hong Kong and Singapore. ESW is an Asendia Group company, a joint venture between La Poste and Swiss Post.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Head Sommelier Job Number 24129332   Job Category Food and Beverage &amp; Culinary   Location W Algarve, Estrada da Gale, Sesmarias, Albufeira, Portugal, Portugal VIEW ON MAP   Schedule Full-Time   Located Remotely? N   Relocation? N   Position Type Non-Management         POSITION SUMMARY       Communicate with guests, employees, and/or departments to make certain staff is working together as a team to ensure that guest needs are met. Answer guest questions or concerns regarding the origin, vintage, and style of various wines. Create, update and maintain wine lists. Pair and suggest wines that will best complement menu items. Attend wine tastings and develop relationships with vendors. Request new wines and products. Design and implement wine promotions and incentive programs. Monitor and replenish inventory of wine cellar, equipment, and glassware. Conduct vintage and BIN number checks. Conduct staff wine tastings. Complete opening and closing duties including setting up necessary supplies and tools, cleaning all equipment and areas, locking doors, etc. Inspect storage areas for organization, use of FIFO, and cleanliness. Complete scheduled inventories and stock and requisition necessary supplies. Monitor dining rooms for seating availability, service, safety, and well being of guests. Complete work orders for maintenance repairs. Issue, open, and serve wine/champagne bottles. Secure liquors, beers, wines, coolers, cabinets, and storage areas. Follow all state and local laws for serving alcohol responsibly. Maintain accurate spill sheet.       Assist management in hiring, training, scheduling, evaluating, and motivating and coaching employees; serve as a role model and first point of contact of the Guarantee of Fair Treatment/Open Door Policy process. Follow all company and safety and security policies and procedures; report accidents, injuries, and unsafe work conditions to manager; and complete safety training and certifications. Ensure uniform and personal appearance are clean and professional, maintain confidentiality of proprietary information, and protect company assets. Welcome and acknowledge all guests according to company standards, anticipate and address guests’ service needs, assist individuals with disabilities, and thank guests with genuine appreciation. Speak with others using clear and professional language. Develop and maintain positive working relationships with others, support team to reach common goals, and listen and respond appropriately to the concerns of other employees. Ensure adherence to quality expectations and standards; and identify, recommend, develop, and implement new ways to increase organizational efficiency, productivity, quality, safety, and/or cost-savings. Read and visually verify information in a variety of formats (e.g., small print). Stand, sit, or walk for an extended period of time or for an entire work shift. Move, lift, carry, push, pull, and place objects weighing less than or equal to 50 pounds without assistance. Grasp, turn, and manipulate objects of varying size and weight, requiring fine motor skills and hand-eye coordination. Move through narrow, confined, or elevated spaces. Move over sloping, uneven, or slippery surfaces as well as up and down stairs and/or service ramps. Reach overhead and below the knees, including bending, twisting, pulling, and stooping. Perform other reasonable job duties as requested by Supervisors.       PREFERRED QUALIFICATION    Education: High school diploma or G.E.D. equivalent.    Related Work Experience: 2 years of related work experience.    Supervisory Experience: 1 year of supervisory experience.    License or Certification: None             Marriott International is an equal opportunity employer. We believe in hiring a diverse workforce and sustaining an inclusive, people-first culture. We are committed to non-discrimination on any protected basis, such as disability and veteran status, or any other basis covered under applicable law.   W Hotels’ mission is to Ignite Curiosity, Expand Worlds. We are a place to experience life. We’re here to open doors and open minds. We are constantly inspired by new faces and new experiences. A tuned-in, up-for-anything spirit is at our core and has made us renowned for reinventing the norms of luxury around the globe. Whatever/Whenever is our culture and service philosophy that brings our guests’ passions to life. If you are original, innovative, and always looking towards the future of what’s possible, welcome to W Hotels. In joining W Hotels, you join a portfolio of brands with Marriott International. Be where you can do your best work, begin your purpose, belong to an amazing global team, and become the best version of you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PhD Student (f/m) for X-ray fluorescence tomography in the Algo. and Sci. Data Analylisis group. The European Synchrotron, the ESRF, is an international research centre based in Grenoble, France.Through its innovative engineering, pioneering scientific vision and a strong commitment from its 700 staff members, the ESRF is recognised as one of the top research facilities worldwide. Its particle accelerator produces intense X-ray beams that are used by thousands of scientists each year for experiments in diverse fields such as biology, medicine, environmental sciences, cultural heritage, materials science, and physics.Supported by 21 countries, the ESRF is an equal opportunity employer and encourages diversity. Thesis subject: Hybrid physics- and data-driven methods for X-ray fluorescence computed tomography (XRFCT)Scientific context and motivationX-ray fluorescence CT (XRFCT) is based on the analysis of the fluorescence signal of a sample excited by a thin X-ray pencil beam. It has several applications in the fields of material science, earth and environmental science and biomedicine. For example, it is used to track specific elements in biological tissues (e.g.prostate) orin combination with heavynano-particles which serve as a fluorescence probe. In earth sciences, XRFCT has been used to determine elemental composition of meteorites fragments.In XRFCT, the sample is excited with a monochromatic pencil beam (see Figure 1). Interactions of the imping- ing beam with the sample’s atoms produce fluorescence photons, whose energy is characteristic of the chemical element. A fluorescence detector collects all fluorescence photons with high energy resolution, for many sample positions and orientations. The collected spectra are then fitted to elemental data and finally passed on to a tomographic reconstruction algorithm to produce 3D spatial elemental maps.Unlike absorption tomography, the attenuation along the impinging and the emitted X-rays must be accounted for in the reconstruction algorithm. Early theoretical works introduced analytic and possibly exact inversion formulas, assuming a complete sampling of the projection space (i.e. full angular coverage, non-truncated projections). In many cases though, these conditions cannot be met and iterative methods like MLEM or SART become solutions of choice.Among the technical challenges that prevent XRFCT to becoming a routine 3D technique, one can cite:Non complete angular coverage of the acquisition: due to mechanical / technical constraints, angular coverage of the sample cannot exceed 120 degrees approximately.Alignment: During the several-hour-long acquisition, the sample may drift. The image quality depends crucially on the accurate identification of these drifts.Sample radiation damage: due to the very small size of the sample, the radiation dose may induce sample deformation, which makes the whole dataset inconsistent.Scientific goals and technical approachDerive practical consistency conditions for XRFCT.Data Consistency conditions (DCC) are mathematical relations that are satisfied by a set of data if it is consistent with their physics model. In some cases, self-absorption of the fluorescence signal can be neglected, and Helgason-Ludwig[1], conditions can be efficient. But in other cases, self-absorption is too significant and must be accounted for. No DCC exist for the fluorescence forward model. Finding such DCC may allow to better guide the estimation of the alignment parameters. The project will benefit from the long-time expertise in the field of DCC developed by the supervisors[2].[1] Ludwig D., Comm. on Pure and Applied Mathematics, 1966.[2] Lesaint et al., IEEE TRPMS, 2017.Design hybrid data/physics driven alignment methods.To further push the accuracy of the critical alignment procedure, we plan to explore methods that combine the universal expressivity of deep neural networks with physics-informed techniques (e.g. DCC-based techniques). Recent research has proved that convolutional networks can be efficient in geometric calibration of transmission CT data[3]. More recently, gradient-based geometric calibration methods combined with deep-learning techniques have investigated these hybrid-methods for classical CT[4].[3]Xiao and Yan, Applied Optics, 2021.[4]Schoonhoven et al., Optics Express, 2024.Generalize hybrid methods to the XRFCT reconstruction problem.Finally, the hybrid methods will be extended to the full 3D XRFCT reconstruction problem. It has been shown that learned inverse problem methods are all the more effective as the data are very noisy. The severe acquisition conditions (under-sampling, missing wedge, low signal) found in XRFCT make these methods good candidates: we can expect from these methods a significant improvement of the image quality compared to state-of-the-art regularization-based variational methods. For more information, please contact Jérome Lesaint (jerome.lesaint@esrf.fr) or Simon Rit (simon.rit@creatis.insa-lyon.fr). Research FieldOtherEducation LevelMaster Degree or equivalent Skills/QualificationsMaster degree (or equivalent diploma that entitles the candidate to enroll for a PhD) in applied maths or computer sciences. Master in Physics with strong interest in applied maths/computer sciences is also possible.Proficiency in signal and image processing.Knowledge of X-ray physics would be a plus.Autonomy, creativity, ability to work within an interdisciplinary team (physics, computer sciences, mathematics, instrumentation).Programming language: Python mainly (C++/CUDA optionally).Excellent written and oral English (working language at ESRF). Specific RequirementsThe salary will be calculated on the basis of relevant qualifications and professional experience.Do you recognize yourself in this description? Apply now for your next professional adventure!What we offer:Join an innovative international research institute, with a workforce from 38 different countriesCollaborate with global experts to advance science and address societal challengesCome and live in a vibrant city, in the heart of the Alps, and Europe's Green Capital 2022Enjoy a workplace designed to support your quality of lifeBenefit from our competitive compensation and allowances package, including financial support for your relocation to GrenobleFor further information on employment terms and conditions, please refer to https://www.esrf.fr/home/Jobs/what-we-offer.htmlThe ESRF is an equal opportunity employer and encourages applications from disabled persons. -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postdoctoral Researcher Position in the Laboratory of Cellular Genomics The Laboratory of Cellular Genomics at the International Institute for Molecular and Cell Biology (IIMCB) https://shorturl.at/EEwOl Warsaw, headed by Dr Aleksandra Kołodziejczyk, seeks a motivated Postdoctoral Researcher to join a project that aims to study molecular mechanisms behind liver fibrosis and the role of the microbiome in the profibrotic processes. You will work on the project funded by OPUS grant of the National Science Centre, Poland entitled: “Finding molecular mechanisms behind the activation of stellate cells” (2023/51/B/NZ2/02649). More information about the lab: olab.com.pl Research FieldComputer science » Modelling toolsEducation LevelPhD or equivalent Research FieldBiological sciences » BiologyEducation LevelPhD or equivalent Research FieldChemistry » BiochemistryEducation LevelPhD or equivalent Research FieldMedical sciences » Health sciencesEducation LevelPhD or equivalent Skills/QualificationsAs a Postdoctoral researcher, you will be responsible for multi-omic analysis of the fibrotic processes in the host, with a particular focus on the liver stellate cells and the impact of the microbiota. Specific RequirementsRequirements:Hold a PhD degree in Biology, Biotechnology, Medicine or an equivalent field. Candidates with degrees in other fields including Engineering, Computer science, or Physics will also be considered if they have relevant experienceExcellent written and oral communication skills in EnglishHigh motivation and proactive and collaborative attitudePrevious experience in one or more methods mentioned below:Experience in working with mice (FELASA certificate or equivalent)Sequencing libraries generation (RNAseq, ATACseq, ChIPseq, single-cell genomics, metagenomics)Cell culture (cell lines, organoids, CRISPR-based cell line modification techniques)Microbiology (culturing bacterial isolates, phenotyping, working anaerobically)Bioinformatics, Data science (R, Python, analysis of sequencing data) LanguagesENGLISHLevelGood Research FieldComputer science » Modelling toolsBiological sciences » BiologyChemistry » BiochemistryMedical sciences » Health sciencesYears of Research Experience1 - 4 BenefitsWe offer:Full employment contract initially for 6 months, with the possibility of extension up to 36 monthsCompetitive salary (8300 - 10500 PLN gross/month depending on the skills and experience)A friendly working atmosphere in an international environment Interesting scientific projectsPosition with 100% focus on research (no teaching obligations)Benefits including reduced-rate for an individual medical care package and membership in MultiSport programmeFull technical, administrative and organizational support from professional English-speaking personnel Selection processCandidates will be selected in an open competition, according to the procedure complying with the rules of the European Charter for Researchers and the Code of Conduct for the Recruitment of Researchers as a part of HR Excellence in Research strategy https://shorturl.at/mJ6Rk&amp;nbsp; Additional commentsHow to apply:Please send your application to recruitment@iimcb.gov.plIn the email subject line, please include "Postdoc OPUS Kolodziejczyk" followed by your first and last name.Your application must be submitted in English and should contain: CV (including a list of publications)motivation letter (max one page)contact information (email address or phone number) to two people who can evaluate you (such as your thesis supervisor, or academic advisor)Please include the following statement in your CV: “I hereby agree to the processing of my personal data, included in the application documents by the International Institute of Molecular and Cell Biology in Warsaw, 4 Księcia Trojdena Street, 02-109 Warsaw, for the purpose of carrying out the current recruitment process.” Your personal data will be processed for the purpose of the recruitment procedure by the International Institute of Molecular and Cell Biology in Warsaw. Full information is available https://bit.ly/3UFWpY2 .If you have questions about further details, please email akolodziejczyk@iimcb.gov.pl Website for additional job detailshttps://shorturl.at/EewOl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemistry/Physics: Fully Funded EPSRC DTP PhD Scholarship: Towards Organic Quantum Memristors Chemistry/Physics: Fully Funded EPSRC DTP PhD Scholarship: Towards Organic Quantum MemristorsThis fully funded project will explore the application of organic semiconductors in quantum computing. Building on research into organic memristors for neuromorphic computing, we are looking to exploit quantum phenomena in these devices and to ultimately realise an organic quantum memristor (QM). Memristors themselves are promising devices for realising multi-state memory, physical neural networks and neuromorphic computing [1]. Recently, we have developed high quality organic memristors that emulate the synaptic behaviour of the brain using squaraine molecules, first using self-assembled nanowires before moving to thin-film devices that are can be integrated with current semiconductor processes [2]. A QM is a device that couples classical memristive behaviour with quantum coherence [3]. Several approaches to realise QMs have been envisaged and more recently a quantum optical memristor has been demonstrated experimentally [4-7]. Quantum coherent states can be realised in certain organic semiconductors through the coupling of photons and excitons to form an exciton polariton [8,9]. In this project, the application of organic exciton polaritons in memristors will be explored to first understand how they can be exploited in optoelectronic memristors before using them to devise a true organic quantum memristor. The role will test a number of novel organic semiconductors and involve thin-film processing and characterisation, device fabrication, advanced spectroscopy, and optical modelling. It will be highly collaborative, working with researchers across the university as well as the UK and abroad. Several training opportunities will be available during the project. For e.g., industry-standard training opportunities in cleanroom practices, device fabrication and characterisation will be run to enhance research skills and improve future employment opportunities. Within the CISM community, informal seminars and training in advanced optics and spectroscopy, thin-film deposition and coding are regularly offered. Furthermore, project costs towards dissemination of research results and enhanced training in quantum technologies are included in this studentship. The candidate will be supervised by Dr James Ryan and Dr Emrys Evans, both academics in the Department of Chemistry and Principal Investigators in the Centre for Integrative Semiconducting Materials (CISM), located in Swansea University’s Bay Campus. This project is aligned with Swansea University’s major expansion in Semiconductor Science and Engineering – both research and teaching. This expansion is spearheaded through the new Centre for Integrative Semiconductor Materials (CISM) – a £90M decadal vision of a bespoke new £30M industry-focused R&amp;D facility. This facility is the first of its kind to fully integrate materials-and-device-level fabrication, analysis and testing across mainstream and emerging semiconductor platforms (silicon, narrow and wide gap compound semiconductors, soft next generation semiconductors such as organics and perovskites). This world-leading initiative is in direct response to the needs of the rapidly expanding regional semiconductor industry, and our shared vision of a thriving and modern manufacturing-intensive Welsh Economy. Research FieldChemistry » OtherEducation LevelBachelor Degree or equivalent Skills/QualificationsCandidates must hold a UK bachelor’s degree with a minimum of Upper Second Class honours in chemistry or a related subject or overseas bachelor’s degree deemed equivalent to UK Bachelor (by UK ECCTIS) and achieved a grade equivalent to UK Upper Second Class honours in chemistry or a related subject. Or a master’s degree with a minimum overall grade at ‘Merit’ in chemistry or a related subject (or Non-UK equivalent as defined by Swansea University). Specific RequirementsIdeally, candidates should hold an MSc or equivalent in chemistry, physics or related subject. Candidates with a strong BSc degree project will also be considered.Please note that you may need to provide evidence of your English Language proficiency. Due to funding restrictions, this scholarship is open to applicants eligible to pay tuition fees at the UK rate only, as defined by UKCISA regulations. BenefitsThis scholarship covers the full cost of tuition fees and an annual stipend at £19,237.Additional research expenses of up to £3,000 per year will also be available. Eligibility criteriaCandidates must hold a UK bachelor’s degree with a minimum of Upper Second Class honours in chemistry or a related subject or overseas bachelor’s degree deemed equivalent to UK Bachelor (by UK ECCTIS) and achieved a grade equivalent to UK Upper Second Class honours in chemistry or a related subject. Or a master’s degree with a minimum overall grade at ‘Merit’ in chemistry or a related subject (or Non-UK equivalent as defined by Swansea University).Ideally, candidates should hold an MSc or equivalent in chemistry, physics or related subject. Candidates with a strong BSc degree project will also be considered. Please note that you may need to provide evidence of your English Language proficiency. Due to funding restrictions, this scholarship is open to applicants eligible to pay tuition fees at the UK rate only, as defined by UKCISA regulations. Selection processPlease see our website for more information. Website for additional job detailshttps://www.swansea.ac.uk/postgraduate/scholarships/research/chemistry-physics-…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postdoc in physics-based machine learning jointly with the MedTech industry Job description Are you looking for a postdoc combining academic research in machine learning with close collaboration with the industry? Do you want to join our research group at KTH developing fundamental machine learning times series algorithms and the team at Getinge producing the next generation ventilators for the intensive care? Are you passionate about physical simulation and proficient in parameter estimation? If so, we believe you will find our project developing a digital twin of the respiratory system a perfect match. This project is co-funded by Vinnova, within the program Advanced Digitalization, and Getinge. Getinge is a world leading MedTech provider with 12.000 employees worldwide. The company has a long tradition of creating innovations that save lives. Their Critical Care Product Area is based in Stockholm, Sweden, and you will interact with its Innovation team regularly during this project. The close collaboration with this multi-disciplinary team of experts is a valuable opportunity for you to create a bridge between academia and industry, in an open and collaborative way. This is also a unique chance that will open multiple future career paths for you. What we offer We offer a dynamic environment where academic research meets industrial R&amp;D, where fundamental aspects of machine learning are combined with physical modelling and applied to intensive-care ventilators to save human lives. A position at a leading technical university that generates knowledge and skills for a sustainable future Engaged and ambitious colleagues along with a creative, international and dynamic working environment Work in Stockholm, in close proximity to nature Help to relocate and be settled in Sweden and at KTH Read more about what it is like to work at KTH Qualifications Requirements A doctoral degree or an equivalent foreign degree in machine learning, engineering physics, computer science or electrical engineering. This eligibility requirement must be met no later than the time the employment decision is made. Research expertise including machine learning, modeling and simulation as well as parameter estimation. As a person, you possess both collaborative abilities as well as the capacity to work independently. Preferred qualifications A doctoral degree or an equivalent foreign degree, obtained within the last three years prior to the application deadline. PhD or master degree experience in time series machine learning, dynamical systems theory and simulation including ODE-models. Experience and knowledge of biomedical applications. Experience and teaching abilities in machine learning. Awareness of diversity and equal opportunity issues, with specific focus on gender equality Great emphasis will be placed on personal skills. Trade union representatives Contact information to trade union representatives. To apply for the position Log into KTH's recruitment system to apply for this position. You are responsible for ensuring that your application is complete according to the instructions in the ad. The application must include: A personal letter. Brief account of why you want to conduct research, your academic interests and how they relate to your previous studies and future goals. Maximally two pages long. CV including relevant professional experience and knowledge. Publication list Copy of diplomas and grades from your previous university studies. Translations into English or Swedish if the original documents have not been issued in any of these languages. Your complete application must be received at KTH no later than the last day of application, midnight CET/CEST (Central European Time/Central European Summer Time). About the employment The position offered is for, at the most, three years. A position as a postdoctoral fellow is a time-limited qualified appointment focusing mainly on research, intended as a first career step after a dissertation. Others Striving towards gender equality, diversity and equal conditions is both a question of quality for KTH and a given part of our values. For information about processing of personal data in the recruitment process. According to The Protective Security Act (2018-585), the candidate must undergo and pass security vetting if the position is placed in a security class. Information regarding whether the position is subject to such a classification will be provided during the recruitment process. We firmly decline all contact with staffing and recruitment agencies and job ad salespersons. Disclaimer: In case of discrepancy between the Swedish original and the English translation of the job announcement, the Swedish version takes precedence. About KTH KTH Royal Institute of Technology in Stockholm has grown to become one of Europe’s leading technical and engineering universities, as well as a key centre of intellectual talent and innovation. We are Sweden’s largest technical research and learning institution and home to students, researchers and faculty from around the world. Our research and education covers a wide area including natural sciences and all branches of engineering, as well as architecture, industrial management, urban planning, history and philosophy. Read more here Type of employment: Temporary position Contract type: Full time First day of employment: According to agreement Salary: Monthly salary Number of positions: 1 Full-time equivalent: 100% City: Stockholm County: Stockholms län Country: Sweden Reference number: J-2024-1793 Contact: Professor Erik Fransén, erikf@kth.se Patrick Sjöstedt (HR-frågor), pss@kth.se Published: 2024-06-28 Last application date: 2024-09-06 Research FieldComputer scienceYears of Research Experience4 - 10 Research FieldEngineeringYears of Research Experience4 - 10 Research FieldEngineeringYears of Research Experience4 - 10 Research FieldEngineeringYears of Research Experience4 - 10 Website for additional job detailshttps://academicpositions.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postdoc Polar ecology and cumulative impacts of tourism Within this project we are looking for a motivated postdoc to identify and map out Antarctic biodiversity values, and to quantify direct and cumulative human impacts on Antarctic terrestrial flora and fauna. Antarctic flora and fauna is dominated by mosses, lichens and small soil invertebrates, and these will be the primary focus in this position. Your dutiesIdentify biodiversity indicators for Antarctic terrestrial biodiversity.Mapping of biodiversity hotspots.Quantify impacts of human activity on Antarctic terrestrial biodiversity.Design and test indicators for monitoring of Antarctic biodiversity Specific RequirementsPhD in polar ecological sciences or relevant biodiversity experienceExperience with spatial biodiversity patterns (potential GIS experience)Experience with (polar) field surveys and laboratory experimentsWillingness and physical ability to work in a cold polar environmentProficiency with statistical approaches and use of R.Excellent social skills to work in an interdisciplinary international research team.English language proficiency both in speech and in writing As a university, we strive for equal opportunities for all, recognising that diversity takes many forms. We believe that diversity in all its complexity is invaluable for the quality of our teaching, research and service. We are always looking for talent with diverse backgrounds and experiences. This also means that we are committed to creating an inclusive community so that we can use diversity as an asset. We realise that each individual brings a unique set of skills, expertise and mindset. Therefore we are happy to invite anyone who recognises themselves in the profile to apply, even if you do not meet all the requirements. BenefitsA challenging position in a socially engaged organisation. At VU Amsterdam, you contribute to education, research and service for a better world. And that is valuable. So in return for your efforts, we offer you: a salary of minimum € 3.877,00 (Scale 10.4) and maximum € 4.786,00 (Scale 10.10) gross per month, on a full-time basis. This is based on UFO profile Researcher 4. The exact salary depends on your education and experience.a position for at least 0.8 FTE. Your employment contract will initially start with a 1 year contract with the possibility to extend with another 2 years.We also offer you attractive fringe benefits and regulations. Some examples: A full-time 38-hour working week comes with a holiday leave entitlement of 232 hours per year. If you choose to work 40 hours, you have 96 extra holiday leave hours on an annual basis. For part-timers, this is calculated pro rata.8% holiday allowance and 8.3% end-of-year bonushybrid working enables a good work-life balancecontribution to commuting expensesspace for personal development Additional commentsAre you interested in this position and do you believe that your experience will contribute to the further development of our university? In that case, we encourage you to submit your application. Submitting a diploma and a reference check are part of the application process. Applications received by e-mail will not be considered.Acquisition in response to this advertisement is not appreciated. Website for additional job detailshttps://www.academictransfer.com/342278/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a System Engineer specializing in Navigation and Communication Systems, you will combine the functions of System Engineer (80% of your time) and Team Lead of the System Engineering Team (20% of your time).As a System Engineer, you will be responsible for:Providing support for satellite projects from the pre-development phase up to spacecraft integration, working closely with project leaders and business development.Assisting in the preparation of proposals and evaluate subcontractor proposals to ensure the feasibility and success of projects.Conducting assessments and evaluations of subsystem concept trades across feasibility and pre-development studies.Analysing system requirements and extract Navigation or Communication subsystem relevant requirements.Generating and maintaining documentation, including analyses, specifications, test procedures, reports, and design descriptions.Designing and configuring Navigation or Communication subsystems for satellite applications.Coordinating technical aspects with customers, vendors, subcontractors, project teams, system engineering, and other divisions.Presenting work results internally and in front of customers.Developing test concepts and providing support during the test phase.As a Team Lead of the System Engineers, you are the supervisor of the System Engineers. You will be responsible for:Monitoring proper execution of tasks assigned to the teamPeople Management of the team:Managing the team skills and expertise in line with the company &amp; project needs.Following up on career and personal growth through evaluations and individual trainingFacilitating communication and collaboration, in and outside the teamSupporting the hiring of new colleaguesOn-boarding and mentoring/coachingHarmonizing the system engineering methodology and tools across all projects, in line with the relevant standards (e.g. ECSS)Ensuring the integrity, consistency and technological evolution of products and/or team specific competences in support of projects. This includes supporting business development and proposal activities with strategical insights on product roadmaps and the company’s technical capabilities.Supporting the COO in close coordination with the other team leads in creating/maintaining balanced project teams, by taking into account skills, aspirations and availability of resources. Desired skillsMaster's degree in electrical engineering, communication engineering or a comparable qualificationProfessional experience as a multidisciplinary system engineer in Navigation, Radar, or Communication projectsAble to work both independently and in large projectsExperience in dealing with customers and vendors is advantageousPlanning &amp; organization skillsFluency in English; knowledge of Dutch is a plusMandatory Requirements Eligible for an EU security clearance (EU citizen, or eligible for citizenship and living in the EU for at least 10 years) -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNSS Engineer – Space Unit Position DescriptionJoin CGI Space to fuel tomorrow's GNSS Innovations!Your role in our teamAs CGI Space in the Netherlands, we're at the forefront of developing a cutting-edge G2G user performance tool, and we're on the lookout for a highly motivated engineer as you to join our team. We focus on GNSS and, more specifically, G2G related projects. In addition to this, we're actively involved in creating simulation tools that replicate behavior and analyze the performance and reliability of GNSS signals.In this role, you'll play a pivotal part in the continuous advancement of our G2G performance tool. Your contributions will shape the future of GNSS technology and its impact. Your enthusiasm and expertise will be valued as we explore new horizons in this dynamic field.How You Strengthen Our TeamYour interest in technology, coupled with your willingness to explore beyond your expertise, is highly valued. We're looking for candidates like you with the following skills and competencies: A Bachelor's or Master's degree in Electrical, Telecommunications, Geodetic, Aerospace, or related engineering fields. Strong understanding of GNSS principles from both user and system perspectives. Knowledge of error sources affecting GNSS and associated models (e.g., ionosphere or multipath models). Experience in evaluating GNSS performance and related statistics and algorithms. Proficiency in precise GNSS products (e.g., precise ephemerides and clock data). Understanding of PNT principles using GNSS technologies (e.g., pseudorange calculations and Kalman filtering). Familiarity with object-oriented programming in MATLAB and/or C++ is advantageous. Proficiency in software engineering aspects, including requirement definition, architectural design, implementation, and testing. Please note that holding an EU passport is mandatory for obtaining an EU Personal Security Clearance at the CONFIDENTIAL level, which is a part of our selection process. Your contributions will be instrumental in strengthening our team and advancing our GNSS technology initiatives.A pre-employment screening is part of the application processWhy CGI? CGI is one of the world's largest IT consultancy firms. Our people keep the Netherlands running. Government agencies, banks, aerospace, infrastructure organizations and energy and manufacturing companies are clients of CGI. We work on interesting projects that touch the daily lives of millions of people. We are present regionally, augmented with global domain knowledge, our ecosystem, and colleagues spread all over the world. We are proud of the impactful projects that we, together with our colleagues, make a success.At CGI, we place great value on diversity and inclusion, as this not only promotes collaboration but often leads to better results. We look forward to your contribution to our team! Work in small self-managing teams consisting of experts in your field Take control of your own career with the space to continue developing yourself You work with the latest technologies An excellent salary and attractive secondary employment conditions Immediate permanent contract Part-time possibilities And the opportunity to become a CGI shareholderJoin our team of experts and apply now! We will contact you as soon as possible. Questions about the position? Ask them to Gert Mariën, Director Consulting Services via gert.marien@cgi.com.For more information about the application procedure, please contact recruiter Chris Nikijuluw via + 31 6 204 51 105 or chris.nikijuluw@cgi.comWe do not collaborate with external recruitment agencies. Therefore, unsolicited acquisition is not appreciated.Your future duties and responsibilitiesRequired Qualifications To Be Successful In This RoleTogether, as owners, let’s turn meaningful insights into action.Life at CGI is rooted in ownership, teamwork, respect and belonging. Here, you’ll reach your full potential because…You are invited to be an owner from day 1 as we work together to bring our Dream to life. That’s why we call ourselves CGI Partners rather than employees. We benefit from our collective success and actively shape our company’s strategy and direction.Your work creates value. You’ll develop innovative solutions and build relationships with teammates and clients while accessing global capabilities to scale your ideas, embrace new opportunities, and benefit from expansive industry and technology expertise.You’ll shape your career by joining a company built to grow and last. You’ll be supported by leaders who care about your health and well-being and provide you with opportunities to deepen your skills and broaden your horizons.Come join our team—one of the largest IT and business consulting services firms in the world.                                                                Show more                                                                                      Show less Engineering and Information Technology IT Services and IT Consulting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PhD position - degrowth and tipping points of food systems, Maastricht Sustainability Institute The Maastricht Sustainability Institute is offering an exciting opportunity for a fulltime PhD position of four years in political economy and sustainability science. Job Description The emerging paradigm of degrowth entails unprecedented changes in policy, economic activities, and individual behaviours in order to constrain production-consumption systems within planetary boundaries. The PhD candidate will empirically explore the feasibility and impacts of such changes on food provision systems in the European Union. Urgent research is needed to improve the understanding of systemic interactions between 1. evolutions of food supply chains, markets, individual livelihoods, and dietary habits; 2. their consequences on spatial organisation, social inequality and conflicts; and 3. the political dynamics of populism and nationalism in Europe. The PhD candidate is expected to conduct novel research on food production-consumption systems in France and the Netherlands. Research tasks can be adjusted to suit specific skills and expertise, but will rely on a systemic perspective and an empirical exploration of degrowth via, e.g.: Mapping out and comparing social aspects and material flows of food systems in France and the Netherlands;Exploring the consequences of degrowth on food systems, e.g., retraining of the workforce and reorganisation of space;Shedding light on interactions between nationalist or populist trends and food systems, such as the entanglement of meat consumption with certain political worldviews;Improving understanding of derailment risks and positive tipping points by comparing “business-as-usual” and “degrowth” scenarios;Developping a transition toolbox for the benefit of food systems actors (farmers, cooperatives) to act on positive tipping points. The candidate will be supervised by Prof. Frank Boons, based at Maastricht Sustainability Institute (MSI), Maastricht University, and be co-supervised by Dr. Clarence Bluntz at MSI. The candidate is expected to contribute to teaching activities in the field of sustainability at the department, taking max. 20% of their time (typically Master-level courses and supervision of Master theses). Requirements We are looking for candidates: who have successfully completed a Master’s degree in a relevant area, e.g.: political economy, ecological economics, sustainability science, food systems.with a record of high academic achievement: Master thesis’ grade, involvement in research papers, in other academic activities; or in research activities outside of academia (e.g., think tanks, NGOs).with a strong interest in one or more of the following research topics: degrowth, food, populism, nationalism, social and environmental impacts of dietary habits, rural-urban divide.with a very good command of written and spoken English, and with working knowledge of Dutch and/or French.enthusiastic about travelling in the Netherlands and France to work with food systems’ actors.What we offerAs PhD position - degrowth and tipping points of food systems, Maastricht Sustainability Instituteat School of Business and Economics, you will be employed by the most international university in the Netherlands, located in the beautiful city of Maastricht. In addition, we offer you:Good employment conditions. The position is graded in scale PhD according to UFO profile PhD, with corresponding salary based on experience ranging from €2770,00 and €3539,00 gross per month (based on a full-time employment of 38 hours per week). In addition to the monthly salary, an 8.0% holiday allowance and an 8.3% year-end bonus apply.An employment contract for a period of 18 months with a scope of 1.0 FTE. Upon a positive evaluation, an extension of 2,5 years will follow.At Maastricht University, the well-being of our employees is of utmost importance, we offer flexible working hours and the possibility to work partly from home if the nature of your position allows it. You will receive a monthly commuting and internet allowance for this. If you work full-time, you will be entitled to 29 vacation days and 4 additional public holidays per year, namely carnival Monday, carnival Tuesday, Good Friday, and Liberation Day. If you choose to accumulate compensation hours, an additional 12 days will be added. Furthermore, you can personalize your employment conditions through a collective labor agreement (CAO) choice model.As Maastricht University, we offer various other excellent secondary employment conditions. These include a good pension scheme with the ABP and the opportunity for UM employees to participate in company fitness and make use of the extensive sports facilities that we also offer to our students.Last but certainly not least, we provide the space and facilities for your personal and professional development. We facilitate this by offering a wide range of training programs and supporting various well-established initiatives such as 'acknowledge and appreciate'. The terms of employment at Maastricht University are largely set out in the collective labor agreement of Dutch Universities. In addition, local provisions specific to UM apply. For more information, click here. Maastricht University Why work at Maastricht University? At Maastricht University (UM), everything revolves around the future. The future of our students, as we work to equip them with a solid, broad-based foundation for the rest of their lives. And the future of society, as we seek solutions through our research to issues from all around the world. Our six faculties combined provide a comprehensive package of study programmes and research. In our teaching, we use the Problem-Based Learning (PBL) method. Students work in small groups, looking for solutions to problems themselves. By discussing issues and working together to draw conclusions, formulate answers and present them to their peers, students develop essential skills for their future careers. With over 22,300 students and more than 5,000 employees from all over the world, UM is home to a vibrant and inspiring international community. Are you drawn to an international setting focused on education, science and scholarship? Are you keen to contribute however your skills and qualities allow? Our door is open to you! As a young European university, we value your talent and look forward to creating the future together. Click here for more information about UM. The School of Business and Economics The School of Business and Economics (SBE) is one of Maastricht University’s six faculties. Our mission is to contribute to a better world by addressing societal problems, by co-creating knowledge and developing team players and leaders for the future. By joining SBE, you will be part of the 1% of business schools worldwide to be Triple Crown accredited (EQUIS, AACSB and AMBA). You will join an inspiring and international environment, where learning and development is priority. Department The Maastricht Sustainability Institute has strong collaborations with other institutes and departments at Maastricht University and elsewhere. We offer a dynamic and challenging job in an internationally oriented organisation. Curious? Are you interested in this exciting position but still have questions? Feel free to contact Clarence Bluntz via c.bluntz@maastrichtuniversity.nl for more information. Applying? Or are you already convinced and ready to become our new PhD? Apply now, no later than August 25th, 2024 for this position. Applicants are expected to include a motivation letter (max. 2 pages), a CV, and contact information for one referee. Applicants selected for an interview will be contacted by the end of August and given instructions to write a short (3-5 pages) research proposal. This is to get a broad idea of how they would tackle the research topic. They will present this proposal during the interview, which will be conducted in September The successful candidate is expected to start in the position fully by January 2025 at the latest; earlier if possible. The vacancy is open for internal and external candidates. In case of equal qualifications, internal candidates will be prioritized. Maastricht University is committed to promoting and nurturing a diverse and inclusive community. We believe that diversity in our staff and student population contributes to the quality of research and education at UM, and strive to enable this through inclusive policies and innovative projects led by teams of staff and students. We encourage you to apply for this position. - Website for additional job detailshttps://www.academictransfer.com/343618/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">About the project:The transition of airflow from laminar to turbulent state is a major contributor to aerodynamic drag and consequently aircraft emissions. Often, unavoidable modifications of the wing surface, such as panel joints or skin deformations decrease the extent of laminar airflow by promoting transition. However, through our research, we showed that this is not always the case. In a recent breakthrough, our team discovered the “Delft Laminar Hump”, a passive smooth surface modification. The proof-of-concept experiments showed the capability of the Hump to create an unprecedented delay of transition, effectively increasing the extent of laminar flow.The “Running up that Hill” project aims at achieving a clear physical understanding of the interaction between laminar-turbulent transition and surface modifications such as the Delft Laminar Hump.The fundamental and technical outcomes of this work will position Hump-like surface modifications as an enabling technology for curbing environmental emissions of aviation. In addition to fundamental work, the project is supported by leading aerospace partners such as KLM, DNW, and Deharde as well as by world-leading groups at U. Waterloo, Canada and KTH, Sweden. Opportunities for research stays with these organisations will be available within the project.We are seeking two enthusiastic and skilled PhD candidates to join our team and work on this exciting project.Important: during submission, please indicate in your motivation letter which of the following two positions you are interested in:PhD position 1: will encompass theoretical and numerical modelling, necessary to simulate the effect of surface modifications on swept wing transition. Flow stability analysis tools available in our team can be used, including Orr-Sommerfeld solvers, linear/non-linear Parabolised Stability Equations and our non-linear Harmonic Navier-Stokes solver. An extensive validation effort will involve high-fidelity Direct Numerical Simulations, in collaboration with the group at KTH Stockholm (Prof. D. Henningson and Dr. A. Hanifi). Research stays at KTH will be covered by the project.PhD position 2: will explore the experimental design and testing of laminar hump models and undertake advanced flow measurements to characterise the underlying transition mechanisms. The candidate will work in the state-of-art windtunnel facilities at TU Delft. The experimental activities will also involve collaboration with U. Waterloo, Canada (Prof. S. Yarusevych), with research stays available.About the team:We are a young, international, and diverse team of colleagues working on topics closely related to the newly founded chair of Flow Control. We approach problems in a horizontal “team spirit” and continuously traverse boundaries between theory, simulations, and experiments towards understanding and controlling fluid flows. Our team, strives for a co-creative and stimulating environment where we can develop our skills as a scientist, team member and teacher. We place great emphasis on a collegial working environment where everyone is welcome and encouraged to shape their PhD track. We also enjoy many team-building activities and events where you can get to know your teammates in a different environment, share personal life experiences and have a great time outside of the lab!Accessibility:Almost 90% of our laboratory and offices are wheelchair accessible, including all wind tunnel facilities. If you have any specific concerns about accessibility, please don’t hesitate to contact us (see below for contact information).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area of research:Scientific / postdoctoral posts,SonstigesJob description:Increasingly, model-based system design (MBSE) is applied in the development of space systems. Information is exchanged using central domain models, which on the one hand allows engineers to work closely together on the design and on the other hand enables analyses and optimizations of the entire system. DLR's own MBSE-tool "Virtual Satellite" has been used successfully for years for system design and within concurrent engineering studies. Join us in our work on developing MBSE as well as “Virtual Satellite” and be responsible for the following tasks: you will maintain close contact with project partners and engineers in order to continuously improve the design processes for space systemsyou will develop new modelling approaches/processes and conduct research in the field of requirements engineeringyou will integrate the developed approaches into "Virtual Satellite”you will support the planning of new space missions in the DLR Concurrent Engineering FacilityIf you enjoy software development and want to become part of our team, we look forward to receive your application. We are looking for highly motivated colleagues who can identify with their work and inspire others. We also offer you the opportunity to contribute with your own ideas and to initiate new projects on your own responsibility. You will be expected to present your work at international conferences and in scientific journals. We offer an exciting, friendly, and flexible working environment where part-time employment is also possible. This research center is part of the Helmholtz Association of German Research Centers. With more than 42,000 employees and an annual budget of over € 5 billion, the Helmholtz Association is Germany's largest scientific organisation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area of research:Scientific / postdoctoral posts,SonstigesJob description:A central research area of the "Optical Satellite Links" department is optical satellite communication for connections from low and geostationary orbit to the ground and between satellites. The department is also involved in laser-optical aeronautical communication for passenger aircraft and drones, for example. Another important area of research is satellite-based quantum communication. Here, the department is working on solutions to efficiently transmit photonic quantum states between satellites and ground stations.The research group "Mitigation of Atmospheric Influences" deals with future applications of optical free-beam transmission (using laser technology) through the atmosphere and in space. Research activities are focussing in particular on overcoming the Earth's atmospheric layers and the resulting interference to transmission paths. The research work is then simulated and verified as part of laboratory tests and extensive measurement campaigns.In order to be able to transmit the extremely high and constantly growing volumes of data, optical communication methods must achieve ever higher performance. Overcoming atmospheric turbulence between ground and GEO stations orbiting the earth is a key prerequisite for this. Research focuses on the development of highly efficient field sensors for adaptive optics systems under strong turbulence, real-time control systems that can process the sensor data and make corrections at high speed, control algorithms for the best possible calculation of the required correction and "pre-distortion" systems that stabilise the uplink beam to the satellite.As the responsible group leader, you will ideally have a solid knowledge of the fundamentals of physics, especially adaptive optics, for these activities. In addition, in-depth knowledge of optical communication technologies is of great importance. As a group leader, you are also responsible for the technical management and achievement of your group's research objectives. This includes the organisation of your group with a clear allocation of tasks and roles, but also the individual development of your employees and supporting the head of department in technical and administrative matters.We offer you the opportunity to work on innovative research projects with state-of-the-art technology in an ambitious international environment. Flexible working hours including an individual agreement on mobile working are part of our offer to you.This research center is part of the Helmholtz Association of German Research Centers. With more than 42,000 employees and an annual budget of over € 5 billion, the Helmholtz Association is Germany's largest scientific organisation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area of research:Scientific / postdoctoral posts,Sonstiges,PromotionJob description:The Navigation department develops methods and systems for interference-free satellite navigation and communication for high-precision positioning and wireless broadband data transmission, for example via satellites.The "Antenna Systems" research group is involved in the development of the next generation of satellite navigation and communication systems.For future satellite and terminal antennas, which will be used in satellite navigation for interference-free and highly accurate positioning and in communication for broadband data transmission, you will work with us to design technologies and contributions to improve and expand the calculation methods. We set up appropriate laboratory models for validation and test them in teams and with other research groups as part of demonstrations.Your tasks will include analysing, critically evaluating and verifying the electromagnetic properties of antennas in the high-frequency and microwave range (computationally and experimentally). We offer you a pleasant working atmosphere in a successful research and development group, state-of-the-art equipment and an environment with national and international co-operations. Opportunities for professional development (e.g. PhD, PMP Project Management) are available.Flexible working hours and an individual agreement for mobile working are a matter of course for us. If you are interested, we look forward to getting to know you!This research center is part of the Helmholtz Association of German Research Centers. With more than 42,000 employees and an annual budget of over € 5 billion, the Helmholtz Association is Germany's largest scientific organisation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doctoral network – DC8 University of Évora (UÉ) Supervisors: Célia Antunes and Inga Wessels The Dust-DN doctoral network Atmospheric dust or mineral dust (or simply “dust”) is a major atmospheric aerosol, and it gives us one of the most visible and detectable aspects of transboundary transport of atmospheric constituents, impacting visibility, radiation and climate. What is less evident are its quantitative impacts on health, transportation and energy production. Atmospheric dust is not fully understood at the fundamental level (microphysical properties, dust emissions, source regions) and hence atmospheric models fail to fully reproduce its impacts. Moreover, dust observations using ground-based instrumentation, remote sensing and aircraft are abundant, but not evenly distributed; in particular they are missing near the major dust sources. Moreover, the techniques are still under development, with each giving a different picture of a phenomenon with multiple facets. For example, it is now known that super-coarse and giant dust particles have gone undetected for a long time due to limitations in the measurement and modelling tools that have been in use for decades, and this misdetection alters the understanding and the prediction of a number of processes. Finally, dust affects the environment, society, and several economic sectors, with impacts on the transportation and energy sectors for example, the nature and cost of which is not fully understood and quantified. Several methodologies exist to study mineral dust, each giving its own differing picture of a complex phenomenon: numerical modelling, remote sensing, in-situ observations, laboratory research. We established the Dust Doctoral Network (Dust-DN), in order to address gaps in the understanding of dust and its impacts by linking the different disciplines and methods. The aim is to train a team of early career scientists into overcoming compartmentalism in this field of science, and into developing a multi-disciplinary approach to mineral dust. Dust-DN will set up a network of academic and non-academic partners working on different aspects of dust research, and will coordinate a program of doctoral projects that will enhance knowledge across a broad range of fundamental, but linked, components of the atmospheric dust life cycle and its impacts. The projects will span across the disciplines of atmospheric sciences (dust processes, modelling, and remote sensing), geology (dust emissions and source regions), as well as the impacts on society and economic sectors. The knowledge will be shared among participating institutions and the wider public and scientific community. Common activities will be held, so as to enhance the network among the partner institutions and among the doctoral researchers, delivering an ambitious advanced training program for capacity building. The University of Évora The University of Évora (UÉ) in Portugal is a public institution organized into five schools: Fine Arts, Sciences and Technology, Social Sciences, Health and Human Development, and Nursing. Within UÉ, the Institute for Advanced Studies and Research (IIFA) serves as a crucial unit, merging teaching with research to foster interdisciplinary knowledge and support existing R&amp;D units. IIFA coordinates 35 PhD programs and two Erasmus Mundus Master programs, ensuring an integrated advanced training environment and offering a wide range of soft skill training. IIFA also oversees 19 research centres, funded by the PT Foundation for Science and Technology. One of these R&amp;D units is the Institute of Earth Sciences (ICT), a multidisciplinary team focusing on Earth System Science and Energy. This team is transitioning to the newly established Centre for Sci-Tech Research in Earth System and Energy (CREATE). CREATE emphasizes integrated research on critical Earth System and Energy challenges, along with technological innovation. It comprises 121 members, including 48 integrated PhD researchers and 39 PhD students. The selected candidate will be working at the ICT/CREATE R&amp;D units of UÉ, gaining access to several observational platforms for atmospheric research in southern Portugal. These platforms include the Évora Atmospheric Sciences Observatory, the Alqueva Lake floating station, oceanic sites at Cabo da Roca and Sines, a mobile air quality platform, and regional networks of weather and solar radiation (BSRN compliant) stations. The team also coordinates specialized research labs in Precision Optics, Atmospheric Physics, Solar Radiation Sensors, Thermofluids &amp; Energy, Bioaerosol &amp; Aerobiology, and Health &amp; Environment. Additionally, a computational cluster with 512 processing cores and 1TB of RAM distributed over eight nodes is available for research purposes. Researchers at all stages of their careers find at ICT/CREATE a dynamic and friendly environment, where personal relationships easily thrive in an inclusive atmosphere, and flexible work planning promotes a life beyond work. The PhD project Doctoral Candidate 8 (DC8) – “Assessment of the respiratory health impact of atmospheric dust” Enrolled in the University of Évora’s PhD programme on “Earth and Space Sciences”. This project has the objective of evaluating the impact of different dust conditions simulating reality on lung epithelial layer function, with a focus on its relation to the concentration and physical and chemical features of the dust. The candidate will prepare and characterize the dust samples in terms of particle size and composition and will expose the lung epithelial cells in air-lift culture to controlled dust conditions, simulating real atmospheric aerosol concentrations. The candidate will also assess the integrity of the epithelial barrier by TEER (Trans-epithelial Electrical Resistances) measurements and histomorphology evaluation, as well as evaluate the epithelial cell activation and inflammation biomarkers (proinflammatory cytokines IL-18, IL-6, IL-8, TNF alpha and fibrotic chemokines, e.g. TGF beta;) and epithelial responses (mucus production; Reactive Oxygen species – ROS). The doctoral candidate will be based at UÉ in Évora, Portugal and will be supervised by Prof. Célia Antunes (UÉ) and Doctor Inga Wessels (ZAUM). Prof. Daniele Bortoli (UÉ) will also contribute to the supervision. The project will include a planned secondment at the Center of Allergy and Environment – Technical University of Munich (Germany) (7 months in the beginning of the second year). Details The recruited PhD candidate will be enrolled in UÉ’s PhD programme on “Earth and Space Sciences” and is included in the “Dust Doctoral Network”, which involves highly prestigious research groups on this scientific topic, and which will ensure that the cohort of doctoral candidates is integrated in a dynamic and enthusiastic scientific environment. The doctoral candidate will learn about the consortium partners’ unique facilities and research topics/methods, and will exploit these opportunities for their research. All Dust-DN doctoral candidates will work side-by-side with lead scientists at world-leading institutes, and they will: ● Take responsibility for the scientific project that they are involved in, and the instruments and/or softwares required. ● Collect scientific knowledge through experiments and/or numerical modelling. ● Develop tailor-made data processing methods. ● Advance the fields of research in atmospheric dust and/or the related measurement techniques. ● Participate in the Dust Doctoral Network training and networking activities ● Publish the results of the research in scientific peer reviewed journals, and present at conferences and workshops. Qualification Requirements · The candidates are required to possess an excellent master’s degree (or equivalent) in natural or life sciences and to not have any kind of PhD degree. · Motivation for research on atmospheric dust. · Experience or aptitude to develop scientific software (computer-based programming) · Demonstrated ability in being a strong team player. · Strong international mobility for the purpose of research, training, and dissemination is mandatory. Preferred Qualifications Additional appreciated skills and competencies are: ● Experience in applying broad scientific knowledge to a range of specific problems or scenarios. ● Previous research experience and/or previous interest in the natural or life sciences or closely related discipline will be appreciated. ● Experience with written or oral communications. ● Fluency in written and oral English is highly valued. ● Publication record. ● Driving licence. Eligibility Requirements · Qualifications: The candidate must hold a title satisfying the admission requirements for a doctoral candidate at the institution where they will be enrolled (see qualification requirements). A doctoral degree in any field is not compatible with these positions. · Mobility: Transnational mobility is an essential requirement of MSCA Doctoral Networks. At the time of recruitment, the candidates must not have resided or carried out their main activity (work, studies, etc.) in Portugal for more than 12 months in the 3 years immediately prior to the recruitment date. Applicants must be aware that seconding periods are planned for this position as described above. International applicants are welcomed. Rights and Responsibilities of Researchers Participating in Marie Skłodwska-Curie Actions The European Charter for Researchers is a set of general principles and requirements which specify the roles, responsibilities and entitlements of both researchers and the employers and/or funders of researchers. The aim of the Charter is to ensure that the nature of the relationship between researchers and employers or funders is conducive to successful performance in generating, transferring, sharing and disseminating knowledge and technological development and to the career development of the researchers. It is obligatory for applicants to read and understand the detailed information regarding the rights and responsibilities of researchers engaged in an MSCA Doctoral Network. The European Charter for researchers can be accessed at: https://euraxess.ec.europa.eu/jobs/charter/european-charter Employment Contract and Financial Aid The selected candidate will be appointed under a 36-months full-time employment contract. A competitive financial aid package will be offered to the successful candidate with a gross annual salary of €35,246 (living allowance and mobility allowance). In addition, there can be further allowances depending on family status and other needs, as per MSCA relevant provisions. It is understood that failure to successfully continue the PhD program will result in immediate cancellation of the employment contract and the financial support provided. Start date The position starts on 3 February 2025 and is a full-time position (40 hours/week), funded for a period of 36 months. Application and selection Application advisory: A pre-screening of the candidates will be made by the Dust-DN consortium as a first step prior to the formal recruitment process. Candidates should submit a CV and motivation letter on the Dust-DN website, together with their university transcripts and the name and contact information of two referees, and indicating up to 3 preferred doctoral projects (in order of preference) amongst the ones advertised within the whole Dust-DN (which includes the one in the present advert). It is very important that the motivation letter should recall each of the qualification requirements and preferred qualifications indicated in this advert, clearly justifying how the candidate is able to meet each of them, and providing evidence. After short-listing, the most suitable candidates will be called for an interview. Formal recruitment phase: The most highly-ranked applicants interviewed during the application advisory phase will be re-directed for the formal application. With the submission of the documents, applicants agree that the documents will be shared among all supervisors of the Dust-DN consortium and members of the respective shortlisting and interviewing panels. Dust-DN respects and supports the compatibility of professional and private life and promotes development opportunities for its cohort of doctoral researchers. We promote equality of opportunity, value diversity and nurture a working and learning environment. Deadlines: Applications for the advisory phase must be submitted by 31 August 2024. Formal applications must be submitted by 30 November 2024. We reserve the possibility to extend the deadline(s) if not enough candidates apply. Contact Information For further information, please contact Professor Célia Antunes (e-mail: cmma@uevora.pt).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assessing the evolution of marine heat waves in conjunction with ocean warming and induced variations in ocean stratification/vertical structureSubject areaPhysical oceanography, air-sea interactions, global warming, climate change, extreme events, marine heat wavesSubject descriptionThe last two decades have seen a significant increase in the frequency and intensity of extreme weather events, including tropical cyclones, heat waves, heavy precipitation, and wildfires. The same is true for extreme events in the ocean, notably marine heat waves. These are part of a new and alarming trend in which we see the compounding effect of multiple extreme events occurring simultaneously or in succession, amplifying the collective impact and posing increasing challenges to human infrastructure and livelihoods around the world.Extreme events and their linkages are a combination of synoptic atmospheric (weather) and ocean circulation and their linkage to climate drivers that result in potentially high-impact events. To mitigate and better adapt to compound extreme events, we need to better understand the phenomenology and evolution of these extremes in a changing climate. These events, and in particular, marine extreme events might be related to the observed ocean warming. In fact, terrestrial weather patterns and climate are determined by the amount and distribution of solar radiation incident on our planet.To maintain a climate (statistical) equilibrium, the radiation leaving the Earth system towards space must equal the solar radiation absorbed, although numerous atmospheric, oceanic and terrestrial phenomena interact to couple these fluxes. Solar radiation can be diffused, reflected or absorbed by the atmosphere and the earth's surface, then transformed into heat, latent, potential and kinetic energy, before being re-emitted to space in the form of long-wave radiation. This energy can be stored, transported and converted, generating various meteorological and oceanic phenomena. Today, this energy balance is being perturbed in unprecedented ways by human activities, with the ocean playing a central role in this disruption. More energy is entering the climate system as compared to the amount of energy leaving it. This unbalance is defined as the Earth Energy Imbalance (EEI). As a consequence, heat is accumulating in Earth climate. Most of this surplus heat is stored in the ocean, about 90%, and it is measured in terms of ocean heat content. The latest results indicate that global warming is accelerating (Minière et al., 2023; Storto et al., 2024).This, potentially accelerating, ocean warming alters the vertical structure of the ocean inducing a stronger stratification of the upper layers and might favor the genesis, intensification and duration of Marine Heat Waves together with changes in atmospheric ocean circulation drivers (Oliver, 2019). Indeed, the surface temperature of the oceans has been rising, with extreme periods occurring more frequently over the past two decades. These are known as marine heat waves, or MHWs (Frölicher et al., 2018). We do not yet know the extent and depth of such events, nor do we know their connection to the atmosphere in terms of drivers and impacts. Nevertheless, these extreme warming events have been documented to have significant impacts on marine ecosystems (Smale et al., 2019; Smith et al., 2023), as well as on human well-being and regional economies (Holbrook et al., 2022). In this PhD project, we will address this issue by focusing on the Atlantic Ocean which has been identified as one of the major regions of ocean warming (e.g., Cheng et al., 2023; Li et al., 2023) and where changes and extreme events have been observed to increase in frequency and intensity.The candidate will work within the framework of the Europe Horizon2030 project ObsSea4Clim (Ocean observations and indicators for climate and assessments : https://obssea4clim.eu). One of the main focus of ObsSea4Clim is to assess MHWs and with this provide a better framework for observing and predicting actionable indicators for sustainable development and climate change adaptation.The objectives are to:Analyze critical areas of regional heat accumulation and changes in stratification as well as MHWs impacted areas under global warming.Identify the most critical areas (e.g., structure of the ocean circulation, modes of internal climate variability, synoptic atmospheric circulation) how heat is redistributed into the deep ocean layers, and how this has changed the vertical ocean stratification.Understand the regional development of MHWs processes and decipher how these have changed with ocean warming and stratification together with the regional synoptic atmospheric circulation.The questions to be addressed are:What are the elements of the regional ocean system that are changing ? Are there key ocean processes that can explain the observed behavior ?What are the respective roles of the ocean warming and atmosphere circulation and their interactions in a warming climate in the observed changes in MHWs ?Do current climate models correctly represent these phenomena? What do large ensembles of climate simulations tell us about the processes in point (b)? Indicative work programDetailed characterization of regional ocean warming and marine heat waves based on analysis of analysis of historical data from observations and reanalyses.We will focus on the Atlantic OceanComposite study of periods of ocean warming, stratification and marine heat wavAnalysis of CMIP6 models using the methods defined in points (1) and (2). At the end of the thesis, based on the results obtained, we will be able to design sensitivity experiments using the IPSL global climate model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are looking for GIS and remote sensing expert to work with data from drones with LIDAR and hyperspectral sensors and other spatial data processing and analysis within the new project:FORSOMICS: Research team and infrastructure upgrade to study the mechanism of conifer resistance to bark beetles in a changing climate: From Gene to Tree Level.And also partially within the project RESDiNET: NETWORK FOR NOVEL REMOTE SENSING TECHNOLOGIES IN FOREST DISTURBANCE ECOLOGY.https://resdinet.eu/The project job position ends on 30.6.2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are seeking a Satellite Imagery Data Scientist to analyze high-resolution satellite imagery for various space-related applications. The candidate will develop machine learning models, process geospatial data, and generate actionable insights for industry-specific use cases like agriculture, defense, and environmental monitoring. A degree in Data Science, Remote Sensing, or GIS is required. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> As a Geospatial Systems Integration Engineer, you will integrate various geospatial systems with existing IT infrastructure to improve efficiency in spatial data analysis. Responsibilities include designing, developing, and testing system integration protocols. Expertise in GIS, programming, and IT systems is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Join our forestry research institute as a Remote Sensing Technician. You will be responsible for processing satellite and UAV data to monitor forest health and track deforestation. Experience with satellite imagery and GIS is essential, and a background in Environmental Science is preferred.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are looking for a GNSS Software Developer to design and develop software applications for Global Navigation Satellite Systems (GNSS). You will work on real-time positioning algorithms and navigation solutions, collaborating closely with research and engineering teams. A degree in Software Engineering or related fields and experience in GNSS technology is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our urban planning consultancy is seeking a GIS Consultant to assist in the development of smart city solutions. You will be tasked with integrating geospatial data into urban development projects, focusing on infrastructure and sustainability. Experience with GIS software and urban planning is essential.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Marine Geospatial Data Specialist will analyze oceanographic and marine geospatial datasets to support research and navigation. Duties include processing satellite imagery and producing bathymetric maps. A degree in Marine Science or GIS is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> We are hiring a LiDAR Data Analyst to support our renewable energy projects by analyzing LiDAR data for wind and solar site assessments. The role involves processing 3D point cloud data to optimize renewable energy installations. A degree in GIS, Environmental Science, or Engineering is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Transportation Infrastructure GIS Specialist will manage spatial data related to road networks, bridges, and public transit systems. Responsibilities include creating and maintaining geospatial datasets for infrastructure planning and analysis. A background in civil engineering and GIS is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Join our environmental consultancy as a Coastal Erosion GIS Specialist to assess and map coastal erosion patterns. You will work with satellite and drone data to model erosion risks and support sustainable coastal management. A degree in Environmental Science or GIS is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Environmental Risk GIS Analyst will analyze geospatial data to assess environmental risks such as flooding, wildfires, and landslides. Responsibilities include spatial data modeling and report generation for mitigation strategies. A degree in GIS and Environmental Science is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are hiring a Geospatial Intelligence Analyst to provide support to defense operations through spatial data analysis. Responsibilities include analyzing satellite imagery and providing insights into military strategy. Experience with GIS and remote sensing is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Civil Defense Geospatial Analyst will provide geospatial data support for civil defense and homeland security efforts, analyzing satellite data and spatial models for threat assessments. A degree in GIS and Security Studies is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Smart Buildings Geospatial Analyst will analyze geospatial data for optimizing smart building designs and energy efficiency. Responsibilities include integrating sensor data with GIS systems to support facility management. A background in Smart Technologies and GIS is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are seeking a Marketing Campaign Manager to oversee the creation and implementation of marketing strategies for our product line. Responsibilities include campaign planning, budget management, and performance analysis. A background in Marketing and Communications is required. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Business Development Manager, you will identify new business opportunities and build relationships with clients in the IT sector. Duties include market research, lead generation, and contract negotiation. Experience in IT sales and business development is essential. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are hiring an HR Generalist to manage recruitment, employee relations, and benefits administration for our growing company. The ideal candidate will have experience in HR management and a strong understanding of labor laws and regulations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are seeking a Supply Chain Coordinator to manage logistics, track inventory, and ensure timely delivery of goods. The role involves coordinating with vendors, managing transportation schedules, and optimizing supply chain processes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are seeking a Data Engineer to build and maintain data pipelines, optimize data architecture, and ensure data quality across various systems. A background in Data Engineering and experience with data warehousing tools is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are hiring a Technical Support Specialist to provide troubleshooting assistance to clients for our software products. The ideal candidate will have strong technical knowledge and excellent communication skills.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are seeking an Event Coordinator to organize and manage company events, from conferences to product launches. The ideal candidate will have strong organizational skills and experience in event planning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Office Manager will be responsible for overseeing daily office operations, managing staff, and ensuring the office runs smoothly. Duties include administrative support, office supply management, and budget tracking.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are looking for an experienced Marketing Director to lead our marketing department for a fast-growing consumer products company. The successful candidate will be responsible for overseeing all marketing activities, from conceptualizing creative campaigns to implementing digital strategies that maximize brand awareness and drive revenue growth. This role requires a strategic thinker with the ability to manage a diverse team of marketing professionals, coordinate with the sales and product development teams, and align marketing objectives with business goals.  Key Responsibilities:      Develop and implement comprehensive marketing strategies to strengthen the company’s market position.     Manage the marketing budget, ensuring a strong return on investment (ROI) for all campaigns.     Lead a team of marketing professionals, including content creators, social media managers, and digital marketing specialists.     Collaborate with the sales team to align marketing campaigns with sales goals.     Conduct market research to identify trends, customer needs, and potential new product lines.     Oversee the creation of compelling content for digital platforms, including websites, social media, and email marketing.     Ensure consistent branding across all channels and campaigns.  Requirements:      Proven experience as a Marketing Director or in a similar leadership role.     Strong understanding of market research, consumer behavior, and digital marketing strategies.     Excellent communication, leadership, and project management skills.     Bachelor's or Master’s degree in Marketing, Business Administration, or a related field.     Experience in consumer products or retail is highly desirable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are seeking a dynamic Human Resources Business Partner (HRBP) to join our tech firm. As the HRBP, you will be a trusted advisor to the leadership team and provide strategic human resource support to align HR initiatives with the company’s business objectives. You will work closely with managers to address employee relations issues, support organizational development, and manage talent acquisition efforts to ensure the company attracts and retains top talent in a highly competitive market.  Key Responsibilities:      Act as a trusted HR consultant to the leadership team and department heads.     Lead the development and implementation of HR initiatives that align with the company’s business strategy.     Oversee talent acquisition, employee onboarding, and training programs to ensure employee growth and retention.     Advise on employee relations, performance management, and conflict resolution to maintain a positive work environment.     Provide guidance on compensation and benefits policies and practices.     Lead diversity and inclusion efforts within the organization to foster a more inclusive workplace culture.     Analyze HR metrics and provide reports to senior management, highlighting key areas for improvement.  Requirements:      Minimum of 5 years of experience in an HR Business Partner or similar role, preferably in the technology sector.     In-depth knowledge of labor laws, HR best practices, and employee relations.     Strong leadership, communication, and interpersonal skills.     Ability to work effectively in a fast-paced and dynamic environment.     Bachelor’s degree in Human Resources, Business Administration, or a related field; Master’s preferred.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description: Our global manufacturing firm is looking for an experienced Financial Controller to oversee the financial operations of our production facilities. The Financial Controller will manage all aspects of financial reporting, budgeting, and forecasting, while also ensuring that all financial procedures comply with corporate policies and industry standards. This is a strategic role that will work closely with senior management to provide insights that guide business decisions.  Key Responsibilities:      Manage the financial operations, including the preparation of financial statements, monthly reports, and forecasting.     Ensure accurate financial reporting in compliance with local regulations and corporate policies.     Oversee the development of budgets, variance analysis, and cost control measures to ensure profitability.     Collaborate with operational leaders to identify areas for financial improvement and cost reduction.     Manage audits and ensure compliance with internal and external financial regulations.     Lead the finance team, providing training and development to support their professional growth.  Requirements:      Proven experience as a Financial Controller or similar role within a manufacturing environment.     In-depth knowledge of financial and accounting principles, including IFRS or GAAP.     Strong analytical skills with attention to detail and a strategic mindset.     Excellent leadership and team management skills.     CPA or ACCA certification preferred.     Bachelor’s degree in Finance, Accounting, or a related field; Master’s degree preferred.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Success Manager – SaaS  Description: As a Customer Success Manager, you will be the main point of contact for our enterprise clients, ensuring they are satisfied with our Software as a Service (SaaS) platform. Your role will involve understanding client needs, offering proactive support, and driving adoption of the product to ensure retention and customer success. This is a critical role for building long-term relationships and fostering customer loyalty.  Key Responsibilities:      Serve as the main contact for clients, ensuring they maximize the value from our SaaS platform.     Conduct regular check-ins with clients to provide product updates and training.     Address customer concerns, troubleshooting issues, and working with the support team to resolve technical problems.     Monitor product usage to identify opportunities for upselling and driving customer engagement.     Collaborate with sales and product teams to provide feedback from clients and ensure continuous product improvement.     Track customer satisfaction and implement strategies to enhance customer loyalty.  Requirements:      Proven experience in a customer success or account management role, preferably in a SaaS environment.     Strong communication and interpersonal skills, with the ability to manage multiple client relationships.     Technical aptitude with the ability to understand and explain complex software products.     Problem-solving skills and a customer-first mindset.     Bachelor’s degree in Business, Marketing, or a related field.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Scientist – Agriculture Applications  Description: We are looking for a highly skilled Remote Sensing Data Scientist to join our research team focused on agricultural applications. The ideal candidate will have extensive experience in analyzing remote sensing data for precision agriculture, land use monitoring, and crop yield prediction. You will be responsible for developing algorithms to process satellite and drone imagery, integrating machine learning techniques to extract insights, and collaborating with agricultural scientists to develop solutions that improve crop management and sustainability.  Key Responsibilities:      Develop and implement advanced algorithms to process and analyze remote sensing data (satellite, UAV) for agricultural applications.     Apply machine learning and data science techniques to predict crop health, yield, and optimize water and fertilizer usage.     Collaborate with agronomists and farmers to develop actionable insights and recommendations based on geospatial data.     Conduct research to improve the accuracy and reliability of remote sensing technologies in agriculture.     Present research findings in academic papers, conferences, and industry forums.  Requirements:      PhD or Master’s degree in Remote Sensing, Geospatial Science, Data Science, or a related field.     Experience in processing satellite imagery (Sentinel, Landsat, MODIS) and UAV data for agriculture.     Proficiency in Python, R, or similar programming languages, with a focus on machine learning libraries.     Experience with geospatial analysis tools such as QGIS, ENVI, or similar platforms.     Strong background in agricultural science or willingness to learn domain-specific knowledge.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Join our innovative team as a Geospatial Engineer focused on developing advanced geospatial solutions for the defense and aerospace sectors. In this role, you will work on cutting-edge projects that involve the integration of satellite data, remote sensing technologies, and GIS applications to enhance national security and defense operations. This position offers the opportunity to collaborate with government agencies, military personnel, and technology developers to create tools that support mission-critical decision-making.  Key Responsibilities:      Develop and implement geospatial solutions using satellite and drone imagery to support defense and aerospace applications.     Analyze spatial data to identify patterns and provide actionable intelligence for military operations.     Work with cross-functional teams to develop real-time geospatial tools for monitoring and situational awareness.     Collaborate with defense agencies to ensure the secure and efficient use of geospatial data in defense missions.     Stay current with advancements in geospatial technologies and apply them to defense applications.  Requirements:      Bachelor’s or Master’s degree in Geospatial Engineering, Remote Sensing, or a related field.     Experience with geospatial tools such as ArcGIS, ENVI, and other GIS platforms.     Knowledge of defense and aerospace systems, including satellite-based navigation and remote sensing.     Strong analytical skills and experience working with large geospatial datasets.     Ability to obtain and maintain security clearance for defense-related projects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geodetic Surveyor – Construction and Infrastructure Projects  Description: We are seeking a skilled Geodetic Surveyor to join our team working on large-scale construction and infrastructure projects. In this role, you will be responsible for conducting precise geodetic surveys to support the design and development of highways, bridges, and other critical infrastructure. The successful candidate will have a deep understanding of geodetic principles and the ability to use advanced surveying equipment and software to ensure accurate measurements and mapping.  Key Responsibilities:      Conduct geodetic surveys using GPS, total stations, and other high-precision instruments to support infrastructure projects.     Create accurate maps and geodetic control networks for construction planning and design.     Collaborate with engineers and construction teams to ensure surveys meet project specifications and timelines.     Manage geospatial data, ensuring that it is properly processed, stored, and accessible for project teams.     Stay updated on advances in geodetic survey technology and implement new methods to improve efficiency and accuracy.  Requirements:      Bachelor’s degree in Geomatics, Surveying, or Civil Engineering.     Extensive experience with geodetic survey techniques and equipment, including GPS, total stations, and GNSS.     Strong knowledge of geodetic reference systems, coordinate systems, and map projections.     Experience with CAD and GIS software for mapping and data management.     Excellent problem-solving and communication skills, with the ability to work in a team-oriented environment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aviation GIS Specialist – Airspace Management  Description: We are looking for an experienced Aviation GIS Specialist to support airspace management and aviation safety projects. You will work closely with air traffic controllers, aviation authorities, and flight operations teams to analyze and visualize airspace data, helping to optimize flight routes, reduce congestion, and enhance safety. This role will involve creating detailed GIS models of airspace and integrating real-time data from radar, satellite, and flight tracking systems.  Key Responsibilities:      Develop and maintain GIS models of national and international airspace, including flight corridors, restricted zones, and navigation aids.     Analyze spatial data to support air traffic management and route optimization.     Integrate real-time data from radar, satellite, and other aviation systems to provide up-to-date maps and visualizations.     Collaborate with aviation authorities to ensure compliance with regulations and optimize airspace usage.     Prepare detailed reports and visualizations to support decision-making by air traffic controllers and aviation planners.  Requirements:      Bachelor’s or Master’s degree in GIS, Aviation Science, or a related field.     Experience with GIS software (ArcGIS, QGIS) and aviation-related data sources (ADS-B, radar).     Strong knowledge of air traffic management, flight operations, and airspace regulations.     Excellent communication skills, with the ability to present complex data to both technical and non-technical audiences.     Ability to work in a fast-paced environment and manage multiple projects simultaneously.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autonomous Vehicles  Description: We are seeking a Geospatial Data Scientist to work on cutting-edge projects in the autonomous vehicle industry. In this role, you will analyze geospatial data to improve vehicle navigation systems, helping to optimize route planning, obstacle detection, and overall safety. The successful candidate will have experience working with large geospatial datasets, machine learning techniques, and advanced mapping tools to support the development of next-generation autonomous driving technology.  Key Responsibilities:      Develop geospatial models to improve the accuracy of autonomous vehicle navigation and route planning.     Analyze sensor data from LIDAR, cameras, and GPS to enhance vehicle perception and decision-making.     Collaborate with software engineers and robotics experts to integrate geospatial data into autonomous vehicle systems.     Conduct research on new geospatial techniques and technologies that can improve autonomous driving performance.     Present findings to stakeholders and contribute to the development of technical papers and presentations.  Requirements:      Master’s or PhD in Geospatial Science, Data Science, or a related field.     Experience working with geospatial datasets and tools such as ArcGIS, QGIS, and Python.     Strong understanding of machine learning algorithms and their application to geospatial data.     Knowledge of autonomous vehicle technology and sensor integration (LIDAR, GPS, cameras).     Excellent problem-solving and communication skills, with the ability to work in a collaborative environment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environmental Monitoring  Description: We are looking for a UAV Geospatial Analyst to join our environmental monitoring team. In this role, you will operate unmanned aerial vehicles (UAVs) to collect geospatial data for environmental assessments, including land use changes, wildlife habitats, and natural resource management. You will analyze the collected data and provide detailed reports to support conservation efforts and sustainable development initiatives.  Key Responsibilities:      Plan and execute UAV flights to collect geospatial data for environmental monitoring projects.     Analyze UAV-collected data using GIS software to assess land use changes, deforestation, and other environmental impacts.     Collaborate with environmental scientists and policymakers to provide actionable insights from geospatial data.     Manage and maintain UAV equipment, ensuring compliance with regulations and safety protocols.     Present findings in detailed reports and visualizations for use in environmental impact assessments.  Requirements:      Bachelor’s degree in Geospatial Science, Environmental Science, or a related field.     Experience with UAV operation, including flight planning and data collection.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solgate is a new research-driven biopharmaceutical startup that develops drugs targeting solute carrier (SLC) proteins, the largest family of membrane transporters. By modulating the function of the “gates” to cellular metabolism, Solgate aims to address unmet medical needs in neurological diseases and in metabolic and autoimmune disorders. Solgate is located in the newly established xista Park, a space housing a growing community of technology startups and biotech companies, adjacent to IST Austria in Klosterneuburg, near Vienna.    Solgate is seeking to hire a motivated and accomplished Research Associate as laboratory Technician to join our fast-growing interdisciplinary research team. Together, you will take part in developing novel small molecule therapeutics that modulate the functions of membrane transporters. The position is part of a team of scientists working together at the interface of functional genomics, molecular biology, chemistry and advanced computational methodologies.    Role and Responsibilities        Collaborate in multidisciplinary research projects towards the development of small molecules     Contribute to laboratory organization (ordering, documentation, database, consumable and infrastructure management)     Take part in the planning and execution of projects through various experimental and analytical methods, such as manipulation of cell lines and cell-based assays     Independently execute analytical methods and report data to the team in a timely, accurate and organized fashion.     Record, analyze, summarize experimental data as part of reporting in written and oral presentations        To accomplish the responsibilities of this role, the candidate must demonstrate excellent interpersonal, organization and communication skills in addition to rigorous scientific thinking.    Qualifications        Master’s in Life Sciences (Cell Biology, Molecular Biology, Biochemistry or related) or Chemical Biology with at least one year of practical experience in the laboratory     Excellent skills in performing and documenting experiments (for example: molecular biology techniques, mammalian cell culture, biochemistry)     Experience in CRISPR-Cas9 based engineering, 96/384 well cell-based assays, FACS are considered a valued asset     Experience in immunology or neuroscience and experience with in vivo models are considered an advantage     Proactive, efficient team player who is able to work both independently and as part of an interdisciplinary team     Creative problem solving and excellent planning and analytical skills     Fluency in English (spoken and written) and working knowledge of German is highly valued.        At Solgate, you will have the opportunity to expand your knowledge and skills to advance your career and take part in the growth of Solgate from its early days. Solgate embraces diversity and equal opportunity and we are committed to building our team to represent a range of backgrounds, perspectives, and skills. We can offer you market-rate gross monthly remuneration starting from 2961€, paid 14 times per year in Austria. The actual remuneration package will be guided by your professional experience and your qualifications, with readiness to pay in excess of collectively agreed amount.    To apply, please submit your letter of motivation and your curriculum vitae to our recruitment team using the link. For any questions, just contact us (hr[at]solgate.com). Please provide the documents as PDF, with your name. We can only consider full applications submitted through our portal. Applications are reviewed on a rolling basis until the position is filled.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your mission   Imagine a world where tax preparation is seamless and stress-free for expatriates. That's the future we envision. To turn this vision into reality, we seek exceptional individuals like you to join our team. We value creative thinkers, proactive doers, and innovative problem-solvers who embrace challenges and thrive in a diverse and ever-evolving environment. At MyExpatTaxes, we foster a culture of collaboration, self-initiative, and continuous learning. We encourage you to think outside the box, leverage data-driven insights, experiment with new ideas, and contribute your unique perspective.  Job responsibilities:      Liase with our external Austrian tax consultants who handle Austria taxes for US expats    Set up and monitor the process and keep up communication with the clients    Work with the Engineering team on new features    Review Austrian tax preparations to hand over for submission       Your profile   When it comes to communication, you exchange ideas with colleagues from a wide variety of backgrounds using English and German easily. You are good at dealing with many tasks at the same time and prioritizing them correctly. You have a pronounced affinity for numbers, quick comprehension, operational readiness and out-of-the box thinking. You enjoy identifying and designing accounting processes and are happy to look for optimization options  Your skillset:      English B2 minimum (company language is English)    German C1 minimum (working with Austrian Finanzamt &amp; Accounting firms)    Completed studies in Finance/Accounting or equivalent work experience/certifications    Experience with Austrian Tax Law    Willingness to learn new things    Strong communication skills    You are used to taking responsibility and doing things independently    You can deal with quickly understanding processes and appropriating a meaningful workflow    Technical proficiency (eg, comfortable using computers and various softwares)    3+ years of relevant work experience   Ideal skills:         Austrian CPA/Steuerberater       Why us?   We are an equal opportunity employer and value diversity at our company. We do not discriminate on the basis of race, religion, color, national origin, gender, sexual orientation, or age. We respect that family always comes first and you will find us willing to accommodate your schedule. We care for our employees and for our customers.  Our core values revolve around delivering freedom and responsibility to our team members. We provide a supportive work environment where you have the autonomy to shape your role and make a meaningful impact. There is no one-size-fits-all approach here. We value your expertise and encourage you to bring your flair. Join us at MyExpatTaxes, and together, we can revolutionize the way expatriates navigate their tax obligations while embracing the exciting opportunities of living abroad. Learn more about our services and join our passionate team today.  We offer you a competitive compensation plus these benefits:         Flexible working hours (Flexitime) and the freedom to regularly work from home or our great office    Free snacks and beverages in the office    Regular team events    A modern office environment which fits our innovative mindset and enables us to collaborate with our diverse team    Mental health counselling and tips from NiloHealth    Monthly Wellness Budget    Home Office set up budget    25 vacation days annually, plus local holidays    Additional day off for your birthday   Following the guidelines of the Austrian collective bargaining agreement for IT, we offer a minimum monthly gross salary of €3000. Depending on your experience and credentials we plan for an overpayment.   We’re also open to part-time employment.     About us        MyExpatTaxes, a project of Software Spinner GmbH, is a global software company established to provide comprehensive tax solutions for Americans residing outside the United States. Since our inception, we have assembled a diverse team of tax professionals, developers, service employees, and marketers from around the world who are passionate about simplifying the complex tax process for Americans living and working abroad. Headquartered in the world’s “Most Liveable City” of Vienna, Austria, with satellite employees across continents, we are dedicated to serving the international community.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company Description   About Us     We are a young and highly motivated company with a start-up character, in which every opinion counts. We develop solutions that accelerate the digital transformation of the property business. Through our solution, day-to-day processes in big complexes such as co-living and co-working spaces can reach maximum efficiency.   Our company was formed after we realized that to better run our fully digitalized self-storage site, we needed to design our own cutting-edge software application. That is how we began with access control in self-storage facilities, but we are now moving beyond opening doors – we strive to provide premium solutions to manage community spaces. At KINNOVIS, we not only aim to advance the quality of working and living so we may all thrive together, but we also encourage it inside our own company culture.   Additional Information   Your Future Role           You will support the development team in designing complex web applications based on individual customer requirements using the latest technologies    You willingly work in dynamic, agile environments, and design products that make our customers happy    You will design innovative concepts that contribute significantly to the improvement of our products    Through writing extensive automated tests, you contribute significantly to increasing our product's quality       You Bring With           Preferably an IT education degree (HTL/FH/Uni) with a focus on software development    Minimum one year of relevant professional experience in web development, ideally with technologies such as Laravel, PHP, Docker, RESTful Services and Stripe    A team player mentality with a desire to be influential in decision-making processes    An outgoing and communicative nature    Excellent knowledge of English (must) and German (nice-to-have)    Your primary place of residence must be Austria       What We Offer           Co-design of software tools that are used daily by our international customers    A secure, stable corporate environment in which teamwork plays a massive role    Flexible working hours and home officing    Very contemporary and brand new office in the south of Vienna    A diverse international team who make you feel like “at home”, with regular employee gatherings    State-of-the-art office equipment, almost everything (desk, blinds, lights, air conditioning, etc.) is controlled by app in our office    A top coffee maker that brings you a little closer to an Italian vibe    A parking space directly in front of the door       For this position, a minimum salary of € 3.100 gross/month is foreseen with the willingness to adjust overpayments, depending on your personal qualifications and experience.   We exclusively hire new members who have their primary living residence in Austria, as we are all big fans of meeting in person, even if it is only once in a while.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEF DE PARTIE at C.O.P.     (m/f/d) as of now, full-time     We are looking for someone who blends professionalism with humor, efficiency with culinary creativity, and a deep-seated passion for gastronomy with responsible kitchen management. This role goes beyond the typical kitchen position. It's about being part of a community just as much as reinventing dining experiences and being bold!     About C.O.P. Vienna    C.O.P., stands for Collection of Produce. It’s not just a restaurant; it's a place where the stories of rural producers, winemakers, and farmers intertwine with Vienna's vibrant creative community. Our focus lies on fresh produce, low intervention, and instinctive, honest cooking.     Your Role: We are looking for someone who shares our dedication to enhancing the culinary experience and our connection with the community. Your role involves not just preparing food, but also managing your station with a focus on quality and sustainability. We value someone who sees the significance of contributing to an environment where both personal and professional growth are achieved through participation and teamwork     Your Job:      ✦ Preparation of Food      ✦ Manage your station and inventory      ✦ Keep control of quality, service, and hygiene standards     What you bring to the table:      ✦ Experience in a similar position      ✦ Good German and English skills      ✦ Passion for gastronomy and quality produce      ✦ Awareness of social impact and sustainability    ✦ Flexible mindset and conflict management abilities    What we bring to the table:    ✦ the opportunity to express your creativity and live out your visions ✦ a dynamic and motivated working environment in the 1st district of Vienna    ✦ to be part of something bigger, and change the way we perceive and experience hospitality    ✦ Gross monthly salary of € 2.300,- with readiness to pay more depending on qualification and experience, plus tips        Join Us    If our vision resonates with you, we are eager to meet you.    Dress up - work the ground - eat the fruits - give back – grace.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solgate is a new research-driven biopharmaceutical startup that develops drugs targeting solute carrier (SLC) proteins, the largest family of membrane transporters. By modulating the function of the “gates” to cellular metabolism, Solgate aims to address unmet medical needs in neurological diseases and in immunological and metabolic disorders. Solgate is located in the newly established xista Park, a space housing a growing community of technology startups and biotech companies, adjacent to IST Austria in Klosterneuburg, near Vienna.    The Position    Solgate is seeking to hire a motivated and accomplished Computational Chemist to join our fast-growing interdisciplinary research team, developing together with biologists and medicinal chemists novel small molecule therapeutics that modulate the functions of membrane transporters. We have a high-performance and result-oriented culture, looking for colleagues eager to contribute and learn. The ideal candidate will bring relevant experience, entrepreneurial drive, and a passion for advancing our mission.           Roles and Responsibilities        Develop and implement emerging workflows for computational pipelines in hit-finding, compound optimization and structural biology, along with well-documented code and reports           Develop and apply methods to model and predict relationships among protein sequence, structure, function, and protein-protein interactions           Collaborate with interdisciplinary teams to design and prioritize compounds with improved potency, selectivity, and ADME properties.           Contribute to team strategy by interpreting and disseminating data using structural modeling, AI/ML, statistical and data mining/data-visualization techniques.           Develop and implement workflows for virtual screening, lead optimization, and structure-based design.           Analyze and interpret simulation data to provide insight into molecular interactions and binding modes of ligands with protein targets.           Engage in multidisciplinary research projects and closely collaborate with Solgate team members to progress strategic targets and support experimental design, statistical analyses, and documentation           Provide subject matter expertise on the data needs for project deliverables in ways that enable efficient decision making           Provide leadership within the team through scientific/technical mentoring, contribution to documentation, and infrastructure management           Organize, summarize and deliver data, in written and oral presentations              To accomplish the responsibilities of this role, the candidate must demonstrate excellent interpersonal, organization and communication skills in addition to rigorous scientific thinking.    Your Qualifications        PhD or equivalent experience in a relevant field such as Computational Chemistry, Computational Biology, Data Science, Bioinformatics, Cheminformatics or Computer Science with 3+ years of hands-on experience in applying advanced computational and data science methods.           Experience in implementing methodologies for structural computational analysis, SBDD, ligand-based optimization, homology modelling, data visualization           High proficiency in R or Python scripting languages, basic knowledge in a second scripting language           Familiarity with relational databases, SQL, Rshiny and/or software engineering are a plus           Experience with one of the following is valued: molecular dynamics, machine learning, chemoinformatics, virtual screening, statistical modelling           Good presentation and communication skills, explaining complex analytics concepts to colleagues at all levels           Comfortable in an agile working environment           Fluent in English; other languages is a plus              At Solgate, you will have the opportunity to expand your knowledge and skills to advance your career and take part in the growth of the company. Solgate embraces diversity and equal opportunity and we are committed to building our team to represent a range of backgrounds, perspectives, and skills. We can offer you a gross monthly (brutto) remuneration starting from 4419 €. The actual market-rate remuneration package will be guided by your professional experience and your qualifications, with readiness to pay in excess of the collectively agreed amount.    To apply, please submit your letter of motivation and your curriculum vitae (including the contact details of two references) to our recruitment team using the link below.    Please provide the documents with your name. We can only consider full applications through the portal. Applications are reviewed on a rolling basis until the position is filled. For any questions regarding the position, e-mail us at hr(AT)solgate.com.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHO ARE WE LOOKING FOR?     At Journi we’re building an app that allows customers to create beautiful photo books and other print products without effort. Using AI technology, we automatically create personalized designs based on the content our users want to print.   Are you positive, emphatic and customer-centric? You love to lend a helping hand and are known for your heart of gold? You have a passion for writing and are a multilingual talent? Sound like you? Then keep reading! We are looking for a support hero to join the Journi team as a Customer Care Specialist!     WHAT YOU'LL DO        Work full time (38.5 h/w) and learn from a passionate, motivated and super international team    Be the first point of contact for our customers    Manage customer communication (in multiple languages) through various support channels and user touchpoints    Define new support templates, filters and shortcuts to constantly optimise support    Be the voice of our customers by reporting issues and user pain points to the product team    Support in customer development, customer surveys and beta testing groups    Be hands-on in reporting, analysing and presenting data and results    Work with the design, product and marketing teams    Reach monthly targets to fulfill your own and company-wide objectives    Give and receive constructive feedback and foster an environment for constant improvement    Help document processes to better share knowledge with team members    Be creative by always finding new ways to help or delight our users       YOUR BAG OF TRICKS        You bring 1+ years of working in customer support/care related roles    You can speak French (C2 level) as English (C1 level)    You have playful and empathetic writing skills    You care about good grammar and spelling!    You are patient, service-oriented and genuinely want to resolve problems    You are a strong communicator and don’t shy away from presenting or talking in front of a group of people    You are known for your creativity and out-of-the-box approach when it comes to finding solutions for any challenge that comes your way    You are interested in the “why” (e.g. Why does a customer behave in a certain way?)    You are a pro with social media (Facebook, Instagram, Twitter) and email    You work efficiently, prioritise workloads, and meet critical project deadlines    You are constantly learning, asking for feedback, self-motivated and hungry to succeed    You are an EU-citizen or have a valid working permit for Austria    You are able to relocate to / based in Vienna - the world’s most liveable city!       NICE TO HAVE        Experience with support tools such as kayako or zendesk    Experience with office and project management tools such as Slack and Asana    You are passionate about photography and traveling    You have an interest in technical tools and topics       WHAT WE OFFER     A happy team makes for a happy workplace. We wouldn’t be able to do what we are doing without our team and that’s why we offer:      A fair annual gross salary in accordance with the Collective Agreement, starting from €35,000. Our final offer depends on your experience and qualifications amongst other factors.    A bunch of awesome social benefits (incl. public transport card, pension fund, in-house yoga and German classes, access to premium language learning app)    Daily lunch vouchers worth €5,50 per day which you can use in more than 1000+ restaurants in Vienna and our downstairs cantina.    Fully functional kitchen in our office with access to healthy and organic foods (cornflakes, fresh fruit, yoghurt, Italian portafilter coffee and a huge range of teas)    25 vacation days per year plus get up to 5 extra holidays per year (1 extra day for each additional working anniversary at Journi)    Team activities - annual team trip, get-togethers and digital events    €2,000 personal development budget per employee per year    Work in a fun, bright and award-winning office - built by the Journi Team! Including ping-pong and foosball to blow off steam    High-end computer (Mac) set-up and tools that will make you enjoy getting your work done    Flexible working hours (with core hours: 10am-4pm Mo-Th; and 10am-2pm on Fr)    Hybrid working model with 40% home office days    Be part of a team of highly motivated and like-minded individuals who you can learn from and want to learn from you too!       APPLY NOW!     Please include: CV, and motivation letter in your application :)   What steps can you expect in the interview process:      Screen call with our People &amp; Culture team    Technical interview with the Customer Care Team    Founders cultural fit interview     Looking forward to meeting you!     About us   About us  We are proud to promote inclusion and diversity at Journi - no matter what race, nationality, gender, religion or sexual orientation - there is always a space for exceptional individuals in our team. At Journi, our mission is to build the most customer-centric way to hold onto your memories. We leverage the power of massive amounts of data and modern AI to enable people to print their memories as easily as taking pictures using the Journi Print app. The smart algorithm in the Journi apps processes 1,000 photos within less than 30 seconds to find the perfect photo layout. You capture the moments and we enable you to convert these into beautiful print products within seconds. We believe in innovation, collaboration and a future where digital and print go hand in hand to preserve lasting memories. We want to become the leading destination to share and print your moments. We have already inspired more than 5 million users around the globe and established Journi as a key player in a booming market, however, we have only scratched the surface of our potential. We are a startup and the creators of the most successful photo and print apps on the market. The Journi apps are downloaded and used by millions of users worldwide. We have been featured by Apple and Google over 20k times and have been covered by Forbes, the L.A. Times, TNW, Techcrunch and many more. At Journi, we look for exceptionally motivated people to become a member of our innovative team of 65+ people from all around the world. People who are passionate about solving challenges and making decisions that impact the success of the company. If you think this could be you, why not send us your application? ;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Life as a Digital Brand Strategist - Luxury Automotive   Are you ready to collaborate with top-tier automotive brands in a global digital agency? Do you excel at crafting brand communication strategies and spotting digital trends?          Are you passionate about leading workshops and crafting excellent solutions for a hands-on international client? For the right candidate this is a prime opportunity to set the strategy and drive long-term growth for an exciting and contemporary global brand.                             Requirements and Responsibilities                     Brand Whisperer: Understand brands like the back of your hand, knowing how to make them relevant to consumers at every touchpoint. Experience with luxury brands is a plus.        Digital Enthusiast: Dive headfirst into social media and digital tech, treating trend research like your daily workout routine.        Strategic Communication: Develop impactful strategies and creative springboards for luxury automotive brands. Analyse brand status quo and trends, devising plans to propel them to the next level.        Collaboration Connoisseur: Define digital and social media strategies in tandem with the creative team, ensuring cohesive brand storytelling.        Analytical Ace: Understand the key KPIs in digital marketing, using data-driven insights to improve brand performance.        Presentation Prodigy: Craft pitch-perfect decks that bring insights and strategies to life, captivating clients and colleagues alike.        Strategic Consultant: Act as an integral part of brand account teams and client meetings, offering strategic insights and guidance. Deliver consultancy into the client’s own organization.        Workshop Wizard: Plan and execute client workshops, laying the foundation for digital communication and content strategies.        Solution Seeker: A self-starting problem-solver, always eager to learn and push boundaries.        Deadline Management: Structure work and team efforts to meet deadlines and handle high volumes effectively.        Language Luminary: Fluent in English. German is a plus.                    Your entry level and starting salary will be based on your experience. To be considered for this role, send your application, CV and earliest possible start date to us.                         Benefits              4-day Workweek       At LOOP you can choose between a 5-day or a 4-day workweek – and have the freedom to switch between these models twice a year.       Free Sports and Fitness       Yoga, fitness, climbing, tennis and more. LOOP covers the costs and gives you access to fitness studios and sports facilities across Austria or Germany.       +20% Vacation       We don’t believe there can be enough time to recharge, that’s why all our team members get +20% vacation days per year — we call it Sunny Hours.       4000+ m² Office Space       Our loft space is part of our identity. An ideal environment for working, collaborating and finding inspiration — with an additional 600m² film- and photo studio.       100% Hybrid Work       Home office or LOOP office space? It’s your choice every day, and you don’t even need approval. In addition, most of our jobs are available as remote jobs.       International and Diverse       Team members from 40+ different nationalities in 7 locations, English as main language and a 55% female leadership quota.       And much more       Language Courses, Visa Support, LOOP.Horizon workshops and trainings, Klimaticket Contribution, Audiobook Library, Headspace App Subscription, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOOP is a digital-first lead agency, exploring the intersections between design, technology and digital brand building for leading brands. With a team of 400 digital talents and through data driven marketing, we help brave clients to stand out in the digital age. Over the last few years our brilliant team has done remarkable and innovative work for internationally recognised high-profile brands such as Puma, Audi, Breitling, Red Bull and numerous others.    Do you want to work closely with our design and mobile development teams to create and continuously improve upon digital products for our international clients? Are you an excellent communicator and skilled at keeping a clear overview of a complex app, webapp and mobile projects? This is your chance to join the LOOP team and become an integral part of the product management and development process and work closely with our clients.    Requirements:      Profound experience as a Project Manager or Product Owner for digital products and the ownership of their full life cycle.   Skillfully execute client strategies for mobile app projects, meticulously managing budgets and timelines.   In-depth understanding of concept, UX/UI design and development of apps and webapps. Experience on software on smart devices is a plus.   Able to set up and facilitate meetings, workshops and collaborative processes within interdisciplinary stakeholders groups as well as our clients BO and POs in order to create the best product possible.   Profound client consulting expertise to build a strong long-term relationship with our clients and consistently manage client expectations ensuring delivery of highest quality product.   You can clearly summarise client expectations into succinct design and development briefings.   Exceptional project management skills and experience in agile methodologies such as SCRUM.   Excellent Jira &amp; Confluence skills.   Be a team-centric player, advocating for collaborative, objective, and respectful dialogue.   Be a strong and proactive communicator, both written and verbal.   Stay up-to-date with emerging trends with a relentless sense of curiosity.   Love to work collaboratively and on eye-level with international clients and within an international team.   You have at least 3 years’ digital agency and/or project / product management experience.   Fluent German language and excellent English language skills.   Benefits:      4-day Workweek   At LOOP you can choose between a 5-day or a 4-day workweek – and have the freedom to switch between these models twice a year.      Free Sports and Fitness   Yoga, fitness, climbing, tennis and more. LOOP covers the costs and gives you access to fitness studios and sports facilities across Austria or Germany.      +20% Vacation   We don’t believe there can be enough time to recharge, that’s why all our team members get +20% vacation days per year, we call it Sunny Hours.      4000+ m² Office Space   Our loft space is part of our identity. An ideal environment for working, collaborating and finding inspiration — with an additional 600m² film- and photo studio.      100% Hybrid Work   Home office or LOOP office space? It’s your choice every day, and you don’t even need approval. In addition, most of our jobs are available as remote jobs.      International and Diverse   Team members from 40+ different nationalities in 7 locations, English as main language and a 55% female leadership quota.      And much more   Language Courses, Visa Support, LOOP.Horizon workshops and trainings, Klimaticket Contribution, Audiobook Library, Headspace App Subscription, etc.    So, if you are motivated to join the LOOP Team, we are happy to offer you a position as a Digital Product Owner in Salzburg, Vienna or Berlin. We are looking forward to receiving your online application!</t>
   </si>
   <si>
     <r>
@@ -193,7 +373,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Business Intelligence Director Ref: BBBH4772              Location. London     Salary. Bonus, Pension     Type. Permanent           Job Description.    Global BI Director:    We are seeking a Global Business Intelligence Director to shape our future strategy and lead the design and development of core data and reporting applications. Collaborating with the Head of Systems and Integration and the Enterprise Architect, you will identify company needs, build fully automated dashboards, create our first Enterprise Data Warehouse, and execute the full strategy. You will oversee data standards and repositories to support business needs.            5 Days a week on-site in Victoria     up to 20% bonus     £7 a day contributory lunch allowance          Key Responsibilities:            Define solution architecture and delivery for data standards across all company applications, systems, and platforms.     Ensure application software aligns with data standards and reporting strategy.     Understand business processes, systems, tools, regulations, and structure to provide valuable intelligence and reporting services.     Oversee information design for application software and continuous improvement initiatives.     Manage design, coding, verification, testing, documentation, amendments, and refactoring of programs/scripts.     Approve database specifications, maintaining standards and data integrity.     Install and test complex databases and products to meet internal and customer requirements.     Design and select critical storage, data center, and client/server environments in line with industry best practices, and provide third-line escalation for global infrastructure solutions.     Redesign complex software applications or components using agreed standards, patterns, and tools.     Produce specifications for cloud-based or on-premise components for detailed design.     Support change programs or projects with technical plans adhering to enterprise and solution architecture standards, including security.     Evaluate alternative architectures for cost, performance, and scalability.     Monitor emerging technologies to assess potential impacts, threats, and opportunities.     Document and present solutions to stakeholders, including business and technical design authorities.     Evaluate potential risks and defects, analyze specifications, and customize applications.     Define and manage technology governance processes for the Information and Data landscape.     Produce documentation for application architecture, design steps, integration processes, and testing procedures.           Technical Experience required:            Strong knowledge of architecture and data methodologies, principles and frameworks.     A strong familiarity working with data platforms especially SQL server and PowerBI are a must have.           Diversity, equity and inclusion are at the heart of what we value as an organisation. Boston Hale is an equal opportunities employer and all qualified applicants will receive consideration for employment without regard to race, religion, sex, sexual orientation, age, disability or any other status protected by law.    If you are able to operate across the top-level of an organisation, have an enthusiastic and positive attitude and can explain the complicated in simple terms whilst driving a Global Organisation's BI environment towards best in class technologies and Best Practices, then please get in touch ASAP                      David Pynor      Head of Data &amp; Technology      +44 (0)20 3587 7905      </t>
+      <t xml:space="preserve">EMTensor GmbH is developing novel biomedical imaging modality utilizing RF-technologies at frequency band around 1GHz. EMTensor GmbH is privately owned MedTech located in Vienna, Austria (www.emtensor.com). The primary focus of the Company is on human brain imaging and diagnostic of brain disorders.     The Company is seeking to recruit an experienced RF electronics engineer with a proven track record and preferably a PhD in microwave / radiofrequency electronic engineering to work as part of our team in Vienna, Austria. The ideal candidate must have hands-on experience in electronic RF engineering and R&amp;D of modern RF/MW devices and technologies at frequency band around 1GHz is desirable.     Role and responsibilities:        Architect novel RF-based biomedical imaging systems     R&amp;D, testing and optimization of RF electronics for novel biomedical imaging systems     Breadth of RF design experience     Innovation and effectiveness in designs produced     Ability to act as lead engineer for new RF product design     Strong practical RF design skills (ability to design, make and test circuitry)     EM simulations using state of the art EM simulation tools     Support the experimental and test activities in the lab     Take part in FDA/CE certification and commercialization of novel biomedical imaging technology and scanners     Provide output and results according to EMTensor’s Quality Management       Essential Qualifications and experiences:        Experience in design, testing and optimization of RF electronics     Experience in commercial electromagnetic simulation tools such as HFSS, CST.     Experience in RF and/or communication system development     Practical lab experience in RF system verification (VNA, spectrum analyzer, oscilloscope utilization etc).     Experience working with EMC and safety certification test labs is a plus.     A passion for hardware development, including working in a fast-paced environment and hands-on design and development.     Interpersonal skills and abilities to communicate and work in a team environment across all levels of the organisation.     Understanding of quality standards and FDA/CE Quality System Regulations is a plus.       Education:        MS +10 years of experience or PhD + 5 years of experience in EE and/or RF engineering        Please send your CV along with a cover letter to </t>
     </r>
     <r>
       <rPr>
@@ -202,149 +382,120 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">dpynor@bostonhale.com</t>
+      <t xml:space="preserve">elke.ebner@emtensor.com</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Linux Cryptography and Security Engineer This is a unique opportunity to use your software engineering and cryptography skills to build and maintain the security foundation that enables Ubuntu and its users to operate securely and remain compliant to international information security standards such as FIPS 140-3 and Common Criteria. You will use your applied cryptography, Linux Security, and coding skills to enhance the Ubuntu distribution and work with organizations such as DISA and CIS to draft and implement security hardening benchmarks for Ubuntu.As a member of the Security Hardening team you will work with and develop automation tooling to audit deployed systems for DISA-STIG and CIS benchmark compliance. You will interact with internal and external stakeholders to identify gaps in our frameworks, and develop new solutions to address these challenges. In this role you will have the opportunity to influence team and security culture, facilitate technical delivery, and help drive team direction and execution. You'll collaborate closely with Canonical's kernel team as well as the wider engineering organization to drive features impacting all Ubuntu users.Day-to-day responsibilitiesCollaborate with other engineers in the Security Hardening team to achieve and retain various Security certificationsExtend and enhance Linux cryptographic components (OpenSSL, Libgcrypt, GnuTLS, and others) with the features and functionality required for FIPS and CC certificationCollaborate with external security consultants to test and validate kernel and crypto module componentsWork with external partners to develop security hardening benchmarks and audit + remediation automation for UbuntuContribute to Ubuntu mainline and upstream projects to land solutions and benefit the communityCommunication and collaboration within and outside Canonical to identify opportunities to improve our security posture, rapidly resolve issues, and deliver high-quality solutions on scheduleWhat we are looking for in youHands-on experience with low-level Linux cryptography APIs and debuggingExcellent software engineering fundamentals, including prior experience with C development, and the ability to demonstrate suchHands-on experience with Linux system administration and shell scriptingDemonstrated knowledge of security and cryptography fundamentals + direct experience writing secure code and implementing best practicesSignificant development experience working with open source librariesExcellent verbal and written communications to enable efficient collaboration with internal and external partners in a remote-first environmentAdditional Skills That You Might Also BringPrior experience working on FIPS/Common Criteria certified products and in-depth knowledge of the underlying standardsPrior experience working directly with DISA-STIG or CIS benchmarks, including related audit + remediation tooling (e.g. Compliance as Code)Experience working directly with Linux KernelPrior experience with Python, OVAL (Open Vulnerability Assessment Language), and AnsibleHistory of contributions to open source projectsWhat we offer youWe consider geographical location, experience, and performance in shaping compensation worldwide. We revisit compensation annually (and more often for graduates and associates) to ensure we recognise outstanding performance. In addition to base pay, we offer a performance-driven annual bonus. We provide all team members with additional benefits, which reflect our values and ideals. We balance our programs to meet local needs and ensure fairness globally.Distributed work environment with twice-yearly team sprints in person - we've been working remotely since 2004!Personal learning and development budget of USD 2,000 per yearAnnual compensation reviewRecognition rewardsAnnual holiday leaveMaternity and paternity leaveEmployee Assistance ProgrammeOpportunity to travel to new locations to meet colleagues from your team and othersPriority Pass for travel and travel upgrades for long haul company eventsAbout CanonicalCanonical is a pioneering tech firm that is at the forefront of the global move to open source. As the company that publishes Ubuntu, one of the most important open source projects and the platform for AI, IoT and the cloud, we are changing the world on a daily basis. We recruit on a global basis and set a very high standard for people joining the company. We expect excellence - in order to succeed, we need to be the best at what we do.Canonical has been a remote-first company since its inception in 2004. Work at Canonical is a step into the future, and will challenge you to think differently, work smarter, learn new skills, and raise your game. Canonical provides a unique window into the world of 21st-century digital business.Canonical is an equal opportunity employerWe are proud to foster a workplace free from discrimination. Diversity of experience, perspectives, and background create a better work environment and better products. Whatever your identity, we will give your application fair consideration.                                                                Show more                                                                                      Show less Information Technology Technology, Information and Internet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecommerce Conversion Rate Optimization Manager Since our founding in 2018, Verbolia has experienced rapid international growth and achieved remarkable success. We earned the title of Belgian Startup of the Year in 2021 and have been honoured with numerous awards, including the IAB MIXX Award for the 'Best MarkAd-Tech Tools' and the Digital Wallonia Startup of the Year award. Most recently, we were recognized as Deloitte's 2023 Fast 500 EMEA winner, further establishing our position as a leader in the digital marketing space. 
- For our new product called Vmax, we're looking for an Ecommerce Conversion Rate Optimization Manager to help our customers, which are large e-commerce websites, drive paid campaigns’ conversion rates and profitability. We are seeking a result-driven conversion rate optimization manager. 
- The ideal candidate will be passionate about leveraging data and insights to improve conversion rates. This role will be a great fit for you if you are data-driven, passionate about e-commerce and conversion rate optimization, and with excellent communication skills for internal collaboration and client relationships. 
- Tasks 
- In this role, you will 
- use your analytics expertise to conduct experiments and analyse results for our customers. 
- plan, prioritise, and manage A/B tests, multivariate tests, and other experimentation initiatives to validate hypotheses and drive continuous improvement for our customers. 
- collaborate closely with Customer Success and Sales to implement test strategies and make sure learnings are shared across the whole company. 
- collaborate closely with Product to make sure Vmax provides our customers with the needed web analytics, heatmaps and merchandising insights to continuously improve conversion rates and engagement. 
- Stay informed about industry trends, best practices, and emerging technologies in CRO and web optimization for e-commerce. 
- Champion a culture of experimentation and build a knowledge base as we grow the number of experiments we do for our customers. 
- Requirements 
- Skills and experience 
- Proven experience (3-5 years) in conversion rate optimization, digital marketing, or related roles, with a track record of driving measurable improvements in conversion rates and website performance in e-commerce. 
- Strong analytical skills, with the ability to interpret data, draw actionable insights, and make data-driven recommendations. 
- Proficiency in web analytics tools such as Google Analytics, as well as experience with A/B testing platforms and other CRO tools. 
- Excellent project management skills, with the ability to prioritise tasks, manage multiple projects simultaneously, and meet deadlines in a fast-paced environment. 
- Exceptional communication and collaboration skills, with the ability to work effectively across cross-functional teams and influence stakeholders at all levels of the organisation. 
- Creative problem-solving abilities, with a passion for experimenting, testing hypotheses, and continuously optimising digital experiences. 
- Knowledge of UX principles, web design best practices, SEO fundamentals, and other factors impacting website performance and user behaviour. 
- Ability to take initiative and adapt. 
- Fluent in English, any other languages are assets. 
- Benefits 
- What we offer 
- Be part of an international start-up environment that is just at the beginning of a bright future 
- A high degree of independence, responsibility, and impact on business operations 
- A competitive salary with plenty of fringe benefits, a company car, a mobile subscription, 5 extra holidays, meal vouchers, a group and hospitalisation insurance 
- A hybrid working model, a good mix of home and office working 
- It is truly important to us that each team member is happy in the team, with interesting challenges, a good understanding of their contribution to the company, a nice environment, a super flexible home working policy,... 
- When recruiting a new team member, we’ll always focus primarily on: 
- company culture fit: be trustworthy, friendly, willing to help 
- adaptability: be ready to evolve along with the company 
- being solution-oriented: never come up with a problem, always come up with a solution to a problem 
- Join a start-up company that takes care of its people:
- yearly team building celebrating our successes 
- quarterly team activities focusing on fun 
- monthly lunches, just because we're hungry sometimes 
- weekly fresh fruits to stay healthy 
- daily collaboration with fantastic colleagues</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sales Trainer David Kennedy Recruitment is working with a "Top Workplace" tech business outsourcing company who is looking to hire a Sales Trainer. As a Sales Trainer, you will play a vital role in designing, delivering, and evaluating training programs to enhance the knowledge and skills of our employees. The ideal candidate should be passionate about employee learning, possess excellent communication skills, and have a strong ability to engage and motivate learners. 
-  Position: Sales Trainer 
-  Location: Dublin, Republic of Ireland 
-  Employment type: Full-time 
-  Remuneration: Base salary + bonus
-  DUTIES AND RESPONSIBILITIES:
-   Develop effective onboarding and training plans for new employees 
-  Develop effective 90-day ramping plans 
-  Create comprehensive training materials and modules that cover sales techniques, product knowledge, and company policies 
-  Tailor training sessions to meet the specific needs of the sales team and address gaps in skills or knowledge 
-  Lead interactive workshops and seminars to teach sales strategies, objection handling, and closing techniques 
-  Provide personalized coaching to individual sales representatives to enhance their performance and address specific challenges 
-  Monitor the progress of members of the sales team through assessments, role-plays, and performance reviews 
-  Analyze sales data and performance metrics to identify areas where the team or individual members need further development 
-  Design competency frameworks for key roles 
-  Design and maintain 6-month rolling training calendar with a combination of online and live training suitable for various levels and roles 
-  Serve as product and service subject matter expert with an acute understanding of the client’s value proposition from both a technical and business prospective new clients 
-  Understand the competitive landscape and coach reps to win
- REQUIREMENTS:
-   2+ years of experience in a sales training role; experience with SaaS, IT Services, or system integrator spaces preferred. 
-  Successful track record in designing training programs, delivering training content, and engaging with training cohorts both in-person and remotely. 
-  Bachelor's degree or equivalent experience in sales, marketing, business, or related field preferred 
-  Strong sales expertise including in-depth knowledge of various sales methodologies (SPIN, Challenger, Sandler, Winning by Design, etc) and an ability to provide real-world examples and insights from own hands-on experience. 
-  Ability to engage with and motivate sales professionals of all levels of experience and tenure. 
-  Utilize strong analytical and assessment skills to evaluate data, identify trends, and make strategic recommendations for continuous improvement and decision-making. 
-  Strong communication and presenting skills supported by an energetic and engaging attitude 
-  Ability to be flexible and agile in responding to evolving business priorities and dealing with ambiguity 
-  Ability to work within a group as a collaborative team player, partnering across the organization and with internal and external stakeholders. 
-  Tech-savvy with an affinity for innovative and emerging technology 
-  Self-reliant, adaptable, decisive, and professional; able to effectively multi-task in a dynamic environment 
-  Fluent English Speaker with additional language a benefit 
-  Proficient in basic computer skills, Microsoft Office, GSuite, and general sales tools such as CRMs. 
-  OFFER:
-   Comprehensive VHI Health cover from day one 
-  Structured training &amp; career development opportunities 
-  Education reimbursement 
-  Paid birthday leave 
-  Child/Dependent care reimbursement 
-  Personal Hardship Loan Program 
-  Mental health and 24/7 employee assistance program 
-  Bike To Work Scheme / Taxsaver Leap Card Scheme 
-  Top-performer and tenure awards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Senior Test Automation Engineer The Opportunity:    The Automation Platform Team is responsible for evolving our test automation framework and our internal test tooling. The main ethos of the Automation Platform team is to make testing easier for the feature application teams. We do this by continuing to adapt and improve our test automation framework and adding the correct functionality to our internal tooling.    The successful candidate will work closely with other members of the quality team and with the wider ESW organisation to identify ways to enhance our automation strategy, framework, and tooling.         Key Responsibilities      Continue to evolve our Test Automation and testing related tooling solutions.    Work with key stakeholders to identify and drive innovations to improve our overall approach to our internal test tooling.    Working with the feature teams to ensure the strategy and frameworks suit their needs.    Develop new capabilities for our internal testing application as required.    Ensure code quality and test coverage.    Continuously strive to introduce improvements and innovations to the team.           Key Experience &amp; Skills:      Experience with writing code in Typescript or JavaScript (ES6).    Proven experience writing and extending automation test frameworks.    Experience with using design patterns suitable for building scalable and maintainable test automation.    Experience with Selenium, or frameworks such as Webdriver.io or Playwright.    Experience with web development, with frameworks such as Angular.    Experience in a continuous delivery environment.    Good understanding of general testing approaches and automation strategies.    Strong critical thinking and problem-solving skills.    Excellent communication and influencing skills.    Demonstrable experience of staying up to date with changes and trends in industry.    Solid understanding of software development approaches of an agile nature    Self-motivated.    Knowledge of when and when not to use automation in testing.     What's on offer?      Competitive salary and a career path adapted to each person's abilities and experience within a company that is growing continuously.    2 days a week working from home.    A flexible schedule and total conciliation between work and family life including reduced timetable during one month in summer.    Become part of a multi-cultural company where you can contribute with your experience and learn from the experience of others.    Work with amazing brands.    Get the opportunity to influence the future of our services and platform.    Excellent working environment with frequent social activities (hackathons, Spartan races, quarterly whole-team social event).    Central Madrid office located an 8-minute walk from Atocha train station, with a bus stop and BiciMad station right outside the office.    Kitchen and dining facilities as well as a fully stocked games room with games consoles etc. - great to disconnect from work for a while and have fun with your colleagues.    Discounted parking space in the office building if you're coming by car, bicycle parking for those worried about their carbon footprint.    Access to private sales by some of the exclusive brands we work with.    Enrollment in English, French, and Spanish lessons that take place during working hours.    Mental Health Wellbeing Program.          About us:     ESW is the leading global and domestic direct-to-consumer (DTC) ecommerce company, empowering the world's best-loved brands to create safer, simpler and faster shopping experiences for consumers all around the globe. ESW acquired Scalefast in June 2022, and the combined 1,300 person organization offers brands and retailers a complete portfolio of technology and services that cost-effectively support any stage of company's development.     From compliance, data security, fraud protection, taxes and tariffs to demand generation, checkout, delivery, returns and customer service, our powerful combination of technology and human ingenuity covers the entire shopper journey across 200 markets, with 100% carbon neutral shipping to consumers. Headquartered in Dublin, Ireland, ESW has global offices in the US, UK, Spain, France, Italy, Japan, Hong Kong and Singapore. ESW is an Asendia Group company, a joint venture between La Poste and Swiss Post.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Head Sommelier Job Number 24129332   Job Category Food and Beverage &amp; Culinary   Location W Algarve, Estrada da Gale, Sesmarias, Albufeira, Portugal, Portugal VIEW ON MAP   Schedule Full-Time   Located Remotely? N   Relocation? N   Position Type Non-Management         POSITION SUMMARY       Communicate with guests, employees, and/or departments to make certain staff is working together as a team to ensure that guest needs are met. Answer guest questions or concerns regarding the origin, vintage, and style of various wines. Create, update and maintain wine lists. Pair and suggest wines that will best complement menu items. Attend wine tastings and develop relationships with vendors. Request new wines and products. Design and implement wine promotions and incentive programs. Monitor and replenish inventory of wine cellar, equipment, and glassware. Conduct vintage and BIN number checks. Conduct staff wine tastings. Complete opening and closing duties including setting up necessary supplies and tools, cleaning all equipment and areas, locking doors, etc. Inspect storage areas for organization, use of FIFO, and cleanliness. Complete scheduled inventories and stock and requisition necessary supplies. Monitor dining rooms for seating availability, service, safety, and well being of guests. Complete work orders for maintenance repairs. Issue, open, and serve wine/champagne bottles. Secure liquors, beers, wines, coolers, cabinets, and storage areas. Follow all state and local laws for serving alcohol responsibly. Maintain accurate spill sheet.       Assist management in hiring, training, scheduling, evaluating, and motivating and coaching employees; serve as a role model and first point of contact of the Guarantee of Fair Treatment/Open Door Policy process. Follow all company and safety and security policies and procedures; report accidents, injuries, and unsafe work conditions to manager; and complete safety training and certifications. Ensure uniform and personal appearance are clean and professional, maintain confidentiality of proprietary information, and protect company assets. Welcome and acknowledge all guests according to company standards, anticipate and address guests’ service needs, assist individuals with disabilities, and thank guests with genuine appreciation. Speak with others using clear and professional language. Develop and maintain positive working relationships with others, support team to reach common goals, and listen and respond appropriately to the concerns of other employees. Ensure adherence to quality expectations and standards; and identify, recommend, develop, and implement new ways to increase organizational efficiency, productivity, quality, safety, and/or cost-savings. Read and visually verify information in a variety of formats (e.g., small print). Stand, sit, or walk for an extended period of time or for an entire work shift. Move, lift, carry, push, pull, and place objects weighing less than or equal to 50 pounds without assistance. Grasp, turn, and manipulate objects of varying size and weight, requiring fine motor skills and hand-eye coordination. Move through narrow, confined, or elevated spaces. Move over sloping, uneven, or slippery surfaces as well as up and down stairs and/or service ramps. Reach overhead and below the knees, including bending, twisting, pulling, and stooping. Perform other reasonable job duties as requested by Supervisors.       PREFERRED QUALIFICATION    Education: High school diploma or G.E.D. equivalent.    Related Work Experience: 2 years of related work experience.    Supervisory Experience: 1 year of supervisory experience.    License or Certification: None             Marriott International is an equal opportunity employer. We believe in hiring a diverse workforce and sustaining an inclusive, people-first culture. We are committed to non-discrimination on any protected basis, such as disability and veteran status, or any other basis covered under applicable law.   W Hotels’ mission is to Ignite Curiosity, Expand Worlds. We are a place to experience life. We’re here to open doors and open minds. We are constantly inspired by new faces and new experiences. A tuned-in, up-for-anything spirit is at our core and has made us renowned for reinventing the norms of luxury around the globe. Whatever/Whenever is our culture and service philosophy that brings our guests’ passions to life. If you are original, innovative, and always looking towards the future of what’s possible, welcome to W Hotels. In joining W Hotels, you join a portfolio of brands with Marriott International. Be where you can do your best work, begin your purpose, belong to an amazing global team, and become the best version of you.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PhD Student (f/m) for X-ray fluorescence tomography in the Algo. and Sci. Data Analylisis group. The European Synchrotron, the ESRF, is an international research centre based in Grenoble, France.Through its innovative engineering, pioneering scientific vision and a strong commitment from its 700 staff members, the ESRF is recognised as one of the top research facilities worldwide. Its particle accelerator produces intense X-ray beams that are used by thousands of scientists each year for experiments in diverse fields such as biology, medicine, environmental sciences, cultural heritage, materials science, and physics.Supported by 21 countries, the ESRF is an equal opportunity employer and encourages diversity. Thesis subject: Hybrid physics- and data-driven methods for X-ray fluorescence computed tomography (XRFCT)Scientific context and motivationX-ray fluorescence CT (XRFCT) is based on the analysis of the fluorescence signal of a sample excited by a thin X-ray pencil beam. It has several applications in the fields of material science, earth and environmental science and biomedicine. For example, it is used to track specific elements in biological tissues (e.g.prostate) orin combination with heavynano-particles which serve as a fluorescence probe. In earth sciences, XRFCT has been used to determine elemental composition of meteorites fragments.In XRFCT, the sample is excited with a monochromatic pencil beam (see Figure 1). Interactions of the imping- ing beam with the sample’s atoms produce fluorescence photons, whose energy is characteristic of the chemical element. A fluorescence detector collects all fluorescence photons with high energy resolution, for many sample positions and orientations. The collected spectra are then fitted to elemental data and finally passed on to a tomographic reconstruction algorithm to produce 3D spatial elemental maps.Unlike absorption tomography, the attenuation along the impinging and the emitted X-rays must be accounted for in the reconstruction algorithm. Early theoretical works introduced analytic and possibly exact inversion formulas, assuming a complete sampling of the projection space (i.e. full angular coverage, non-truncated projections). In many cases though, these conditions cannot be met and iterative methods like MLEM or SART become solutions of choice.Among the technical challenges that prevent XRFCT to becoming a routine 3D technique, one can cite:Non complete angular coverage of the acquisition: due to mechanical / technical constraints, angular coverage of the sample cannot exceed 120 degrees approximately.Alignment: During the several-hour-long acquisition, the sample may drift. The image quality depends crucially on the accurate identification of these drifts.Sample radiation damage: due to the very small size of the sample, the radiation dose may induce sample deformation, which makes the whole dataset inconsistent.Scientific goals and technical approachDerive practical consistency conditions for XRFCT.Data Consistency conditions (DCC) are mathematical relations that are satisfied by a set of data if it is consistent with their physics model. In some cases, self-absorption of the fluorescence signal can be neglected, and Helgason-Ludwig[1], conditions can be efficient. But in other cases, self-absorption is too significant and must be accounted for. No DCC exist for the fluorescence forward model. Finding such DCC may allow to better guide the estimation of the alignment parameters. The project will benefit from the long-time expertise in the field of DCC developed by the supervisors[2].[1] Ludwig D., Comm. on Pure and Applied Mathematics, 1966.[2] Lesaint et al., IEEE TRPMS, 2017.Design hybrid data/physics driven alignment methods.To further push the accuracy of the critical alignment procedure, we plan to explore methods that combine the universal expressivity of deep neural networks with physics-informed techniques (e.g. DCC-based techniques). Recent research has proved that convolutional networks can be efficient in geometric calibration of transmission CT data[3]. More recently, gradient-based geometric calibration methods combined with deep-learning techniques have investigated these hybrid-methods for classical CT[4].[3]Xiao and Yan, Applied Optics, 2021.[4]Schoonhoven et al., Optics Express, 2024.Generalize hybrid methods to the XRFCT reconstruction problem.Finally, the hybrid methods will be extended to the full 3D XRFCT reconstruction problem. It has been shown that learned inverse problem methods are all the more effective as the data are very noisy. The severe acquisition conditions (under-sampling, missing wedge, low signal) found in XRFCT make these methods good candidates: we can expect from these methods a significant improvement of the image quality compared to state-of-the-art regularization-based variational methods. For more information, please contact Jérome Lesaint (jerome.lesaint@esrf.fr) or Simon Rit (simon.rit@creatis.insa-lyon.fr). Research FieldOtherEducation LevelMaster Degree or equivalent Skills/QualificationsMaster degree (or equivalent diploma that entitles the candidate to enroll for a PhD) in applied maths or computer sciences. Master in Physics with strong interest in applied maths/computer sciences is also possible.Proficiency in signal and image processing.Knowledge of X-ray physics would be a plus.Autonomy, creativity, ability to work within an interdisciplinary team (physics, computer sciences, mathematics, instrumentation).Programming language: Python mainly (C++/CUDA optionally).Excellent written and oral English (working language at ESRF). Specific RequirementsThe salary will be calculated on the basis of relevant qualifications and professional experience.Do you recognize yourself in this description? Apply now for your next professional adventure!What we offer:Join an innovative international research institute, with a workforce from 38 different countriesCollaborate with global experts to advance science and address societal challengesCome and live in a vibrant city, in the heart of the Alps, and Europe's Green Capital 2022Enjoy a workplace designed to support your quality of lifeBenefit from our competitive compensation and allowances package, including financial support for your relocation to GrenobleFor further information on employment terms and conditions, please refer to https://www.esrf.fr/home/Jobs/what-we-offer.htmlThe ESRF is an equal opportunity employer and encourages applications from disabled persons. -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postdoctoral Researcher Position in the Laboratory of Cellular Genomics The Laboratory of Cellular Genomics at the International Institute for Molecular and Cell Biology (IIMCB) https://shorturl.at/EEwOl Warsaw, headed by Dr Aleksandra Kołodziejczyk, seeks a motivated Postdoctoral Researcher to join a project that aims to study molecular mechanisms behind liver fibrosis and the role of the microbiome in the profibrotic processes. You will work on the project funded by OPUS grant of the National Science Centre, Poland entitled: “Finding molecular mechanisms behind the activation of stellate cells” (2023/51/B/NZ2/02649). More information about the lab: olab.com.pl Research FieldComputer science » Modelling toolsEducation LevelPhD or equivalent Research FieldBiological sciences » BiologyEducation LevelPhD or equivalent Research FieldChemistry » BiochemistryEducation LevelPhD or equivalent Research FieldMedical sciences » Health sciencesEducation LevelPhD or equivalent Skills/QualificationsAs a Postdoctoral researcher, you will be responsible for multi-omic analysis of the fibrotic processes in the host, with a particular focus on the liver stellate cells and the impact of the microbiota. Specific RequirementsRequirements:Hold a PhD degree in Biology, Biotechnology, Medicine or an equivalent field. Candidates with degrees in other fields including Engineering, Computer science, or Physics will also be considered if they have relevant experienceExcellent written and oral communication skills in EnglishHigh motivation and proactive and collaborative attitudePrevious experience in one or more methods mentioned below:Experience in working with mice (FELASA certificate or equivalent)Sequencing libraries generation (RNAseq, ATACseq, ChIPseq, single-cell genomics, metagenomics)Cell culture (cell lines, organoids, CRISPR-based cell line modification techniques)Microbiology (culturing bacterial isolates, phenotyping, working anaerobically)Bioinformatics, Data science (R, Python, analysis of sequencing data) LanguagesENGLISHLevelGood Research FieldComputer science » Modelling toolsBiological sciences » BiologyChemistry » BiochemistryMedical sciences » Health sciencesYears of Research Experience1 - 4 BenefitsWe offer:Full employment contract initially for 6 months, with the possibility of extension up to 36 monthsCompetitive salary (8300 - 10500 PLN gross/month depending on the skills and experience)A friendly working atmosphere in an international environment Interesting scientific projectsPosition with 100% focus on research (no teaching obligations)Benefits including reduced-rate for an individual medical care package and membership in MultiSport programmeFull technical, administrative and organizational support from professional English-speaking personnel Selection processCandidates will be selected in an open competition, according to the procedure complying with the rules of the European Charter for Researchers and the Code of Conduct for the Recruitment of Researchers as a part of HR Excellence in Research strategy https://shorturl.at/mJ6Rk&amp;nbsp; Additional commentsHow to apply:Please send your application to recruitment@iimcb.gov.plIn the email subject line, please include "Postdoc OPUS Kolodziejczyk" followed by your first and last name.Your application must be submitted in English and should contain: CV (including a list of publications)motivation letter (max one page)contact information (email address or phone number) to two people who can evaluate you (such as your thesis supervisor, or academic advisor)Please include the following statement in your CV: “I hereby agree to the processing of my personal data, included in the application documents by the International Institute of Molecular and Cell Biology in Warsaw, 4 Księcia Trojdena Street, 02-109 Warsaw, for the purpose of carrying out the current recruitment process.” Your personal data will be processed for the purpose of the recruitment procedure by the International Institute of Molecular and Cell Biology in Warsaw. Full information is available https://bit.ly/3UFWpY2 .If you have questions about further details, please email akolodziejczyk@iimcb.gov.pl Website for additional job detailshttps://shorturl.at/EewOl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemistry/Physics: Fully Funded EPSRC DTP PhD Scholarship: Towards Organic Quantum Memristors Chemistry/Physics: Fully Funded EPSRC DTP PhD Scholarship: Towards Organic Quantum MemristorsThis fully funded project will explore the application of organic semiconductors in quantum computing. Building on research into organic memristors for neuromorphic computing, we are looking to exploit quantum phenomena in these devices and to ultimately realise an organic quantum memristor (QM). Memristors themselves are promising devices for realising multi-state memory, physical neural networks and neuromorphic computing [1]. Recently, we have developed high quality organic memristors that emulate the synaptic behaviour of the brain using squaraine molecules, first using self-assembled nanowires before moving to thin-film devices that are can be integrated with current semiconductor processes [2]. A QM is a device that couples classical memristive behaviour with quantum coherence [3]. Several approaches to realise QMs have been envisaged and more recently a quantum optical memristor has been demonstrated experimentally [4-7]. Quantum coherent states can be realised in certain organic semiconductors through the coupling of photons and excitons to form an exciton polariton [8,9]. In this project, the application of organic exciton polaritons in memristors will be explored to first understand how they can be exploited in optoelectronic memristors before using them to devise a true organic quantum memristor. The role will test a number of novel organic semiconductors and involve thin-film processing and characterisation, device fabrication, advanced spectroscopy, and optical modelling. It will be highly collaborative, working with researchers across the university as well as the UK and abroad. Several training opportunities will be available during the project. For e.g., industry-standard training opportunities in cleanroom practices, device fabrication and characterisation will be run to enhance research skills and improve future employment opportunities. Within the CISM community, informal seminars and training in advanced optics and spectroscopy, thin-film deposition and coding are regularly offered. Furthermore, project costs towards dissemination of research results and enhanced training in quantum technologies are included in this studentship. The candidate will be supervised by Dr James Ryan and Dr Emrys Evans, both academics in the Department of Chemistry and Principal Investigators in the Centre for Integrative Semiconducting Materials (CISM), located in Swansea University’s Bay Campus. This project is aligned with Swansea University’s major expansion in Semiconductor Science and Engineering – both research and teaching. This expansion is spearheaded through the new Centre for Integrative Semiconductor Materials (CISM) – a £90M decadal vision of a bespoke new £30M industry-focused R&amp;D facility. This facility is the first of its kind to fully integrate materials-and-device-level fabrication, analysis and testing across mainstream and emerging semiconductor platforms (silicon, narrow and wide gap compound semiconductors, soft next generation semiconductors such as organics and perovskites). This world-leading initiative is in direct response to the needs of the rapidly expanding regional semiconductor industry, and our shared vision of a thriving and modern manufacturing-intensive Welsh Economy. Research FieldChemistry » OtherEducation LevelBachelor Degree or equivalent Skills/QualificationsCandidates must hold a UK bachelor’s degree with a minimum of Upper Second Class honours in chemistry or a related subject or overseas bachelor’s degree deemed equivalent to UK Bachelor (by UK ECCTIS) and achieved a grade equivalent to UK Upper Second Class honours in chemistry or a related subject. Or a master’s degree with a minimum overall grade at ‘Merit’ in chemistry or a related subject (or Non-UK equivalent as defined by Swansea University). Specific RequirementsIdeally, candidates should hold an MSc or equivalent in chemistry, physics or related subject. Candidates with a strong BSc degree project will also be considered.Please note that you may need to provide evidence of your English Language proficiency. Due to funding restrictions, this scholarship is open to applicants eligible to pay tuition fees at the UK rate only, as defined by UKCISA regulations. BenefitsThis scholarship covers the full cost of tuition fees and an annual stipend at £19,237.Additional research expenses of up to £3,000 per year will also be available. Eligibility criteriaCandidates must hold a UK bachelor’s degree with a minimum of Upper Second Class honours in chemistry or a related subject or overseas bachelor’s degree deemed equivalent to UK Bachelor (by UK ECCTIS) and achieved a grade equivalent to UK Upper Second Class honours in chemistry or a related subject. Or a master’s degree with a minimum overall grade at ‘Merit’ in chemistry or a related subject (or Non-UK equivalent as defined by Swansea University).Ideally, candidates should hold an MSc or equivalent in chemistry, physics or related subject. Candidates with a strong BSc degree project will also be considered. Please note that you may need to provide evidence of your English Language proficiency. Due to funding restrictions, this scholarship is open to applicants eligible to pay tuition fees at the UK rate only, as defined by UKCISA regulations. Selection processPlease see our website for more information. Website for additional job detailshttps://www.swansea.ac.uk/postgraduate/scholarships/research/chemistry-physics-…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postdoc in physics-based machine learning jointly with the MedTech industry Job description Are you looking for a postdoc combining academic research in machine learning with close collaboration with the industry? Do you want to join our research group at KTH developing fundamental machine learning times series algorithms and the team at Getinge producing the next generation ventilators for the intensive care? Are you passionate about physical simulation and proficient in parameter estimation? If so, we believe you will find our project developing a digital twin of the respiratory system a perfect match. This project is co-funded by Vinnova, within the program Advanced Digitalization, and Getinge. Getinge is a world leading MedTech provider with 12.000 employees worldwide. The company has a long tradition of creating innovations that save lives. Their Critical Care Product Area is based in Stockholm, Sweden, and you will interact with its Innovation team regularly during this project. The close collaboration with this multi-disciplinary team of experts is a valuable opportunity for you to create a bridge between academia and industry, in an open and collaborative way. This is also a unique chance that will open multiple future career paths for you. What we offer We offer a dynamic environment where academic research meets industrial R&amp;D, where fundamental aspects of machine learning are combined with physical modelling and applied to intensive-care ventilators to save human lives. A position at a leading technical university that generates knowledge and skills for a sustainable future Engaged and ambitious colleagues along with a creative, international and dynamic working environment Work in Stockholm, in close proximity to nature Help to relocate and be settled in Sweden and at KTH Read more about what it is like to work at KTH Qualifications Requirements A doctoral degree or an equivalent foreign degree in machine learning, engineering physics, computer science or electrical engineering. This eligibility requirement must be met no later than the time the employment decision is made. Research expertise including machine learning, modeling and simulation as well as parameter estimation. As a person, you possess both collaborative abilities as well as the capacity to work independently. Preferred qualifications A doctoral degree or an equivalent foreign degree, obtained within the last three years prior to the application deadline. PhD or master degree experience in time series machine learning, dynamical systems theory and simulation including ODE-models. Experience and knowledge of biomedical applications. Experience and teaching abilities in machine learning. Awareness of diversity and equal opportunity issues, with specific focus on gender equality Great emphasis will be placed on personal skills. Trade union representatives Contact information to trade union representatives. To apply for the position Log into KTH's recruitment system to apply for this position. You are responsible for ensuring that your application is complete according to the instructions in the ad. The application must include: A personal letter. Brief account of why you want to conduct research, your academic interests and how they relate to your previous studies and future goals. Maximally two pages long. CV including relevant professional experience and knowledge. Publication list Copy of diplomas and grades from your previous university studies. Translations into English or Swedish if the original documents have not been issued in any of these languages. Your complete application must be received at KTH no later than the last day of application, midnight CET/CEST (Central European Time/Central European Summer Time). About the employment The position offered is for, at the most, three years. A position as a postdoctoral fellow is a time-limited qualified appointment focusing mainly on research, intended as a first career step after a dissertation. Others Striving towards gender equality, diversity and equal conditions is both a question of quality for KTH and a given part of our values. For information about processing of personal data in the recruitment process. According to The Protective Security Act (2018-585), the candidate must undergo and pass security vetting if the position is placed in a security class. Information regarding whether the position is subject to such a classification will be provided during the recruitment process. We firmly decline all contact with staffing and recruitment agencies and job ad salespersons. Disclaimer: In case of discrepancy between the Swedish original and the English translation of the job announcement, the Swedish version takes precedence. About KTH KTH Royal Institute of Technology in Stockholm has grown to become one of Europe’s leading technical and engineering universities, as well as a key centre of intellectual talent and innovation. We are Sweden’s largest technical research and learning institution and home to students, researchers and faculty from around the world. Our research and education covers a wide area including natural sciences and all branches of engineering, as well as architecture, industrial management, urban planning, history and philosophy. Read more here Type of employment: Temporary position Contract type: Full time First day of employment: According to agreement Salary: Monthly salary Number of positions: 1 Full-time equivalent: 100% City: Stockholm County: Stockholms län Country: Sweden Reference number: J-2024-1793 Contact: Professor Erik Fransén, erikf@kth.se Patrick Sjöstedt (HR-frågor), pss@kth.se Published: 2024-06-28 Last application date: 2024-09-06 Research FieldComputer scienceYears of Research Experience4 - 10 Research FieldEngineeringYears of Research Experience4 - 10 Research FieldEngineeringYears of Research Experience4 - 10 Research FieldEngineeringYears of Research Experience4 - 10 Website for additional job detailshttps://academicpositions.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postdoc Polar ecology and cumulative impacts of tourism Within this project we are looking for a motivated postdoc to identify and map out Antarctic biodiversity values, and to quantify direct and cumulative human impacts on Antarctic terrestrial flora and fauna. Antarctic flora and fauna is dominated by mosses, lichens and small soil invertebrates, and these will be the primary focus in this position. Your dutiesIdentify biodiversity indicators for Antarctic terrestrial biodiversity.Mapping of biodiversity hotspots.Quantify impacts of human activity on Antarctic terrestrial biodiversity.Design and test indicators for monitoring of Antarctic biodiversity Specific RequirementsPhD in polar ecological sciences or relevant biodiversity experienceExperience with spatial biodiversity patterns (potential GIS experience)Experience with (polar) field surveys and laboratory experimentsWillingness and physical ability to work in a cold polar environmentProficiency with statistical approaches and use of R.Excellent social skills to work in an interdisciplinary international research team.English language proficiency both in speech and in writing As a university, we strive for equal opportunities for all, recognising that diversity takes many forms. We believe that diversity in all its complexity is invaluable for the quality of our teaching, research and service. We are always looking for talent with diverse backgrounds and experiences. This also means that we are committed to creating an inclusive community so that we can use diversity as an asset. We realise that each individual brings a unique set of skills, expertise and mindset. Therefore we are happy to invite anyone who recognises themselves in the profile to apply, even if you do not meet all the requirements. BenefitsA challenging position in a socially engaged organisation. At VU Amsterdam, you contribute to education, research and service for a better world. And that is valuable. So in return for your efforts, we offer you: a salary of minimum € 3.877,00 (Scale 10.4) and maximum € 4.786,00 (Scale 10.10) gross per month, on a full-time basis. This is based on UFO profile Researcher 4. The exact salary depends on your education and experience.a position for at least 0.8 FTE. Your employment contract will initially start with a 1 year contract with the possibility to extend with another 2 years.We also offer you attractive fringe benefits and regulations. Some examples: A full-time 38-hour working week comes with a holiday leave entitlement of 232 hours per year. If you choose to work 40 hours, you have 96 extra holiday leave hours on an annual basis. For part-timers, this is calculated pro rata.8% holiday allowance and 8.3% end-of-year bonushybrid working enables a good work-life balancecontribution to commuting expensesspace for personal development Additional commentsAre you interested in this position and do you believe that your experience will contribute to the further development of our university? In that case, we encourage you to submit your application. Submitting a diploma and a reference check are part of the application process. Applications received by e-mail will not be considered.Acquisition in response to this advertisement is not appreciated. Website for additional job detailshttps://www.academictransfer.com/342278/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a System Engineer specializing in Navigation and Communication Systems, you will combine the functions of System Engineer (80% of your time) and Team Lead of the System Engineering Team (20% of your time).As a System Engineer, you will be responsible for:Providing support for satellite projects from the pre-development phase up to spacecraft integration, working closely with project leaders and business development.Assisting in the preparation of proposals and evaluate subcontractor proposals to ensure the feasibility and success of projects.Conducting assessments and evaluations of subsystem concept trades across feasibility and pre-development studies.Analysing system requirements and extract Navigation or Communication subsystem relevant requirements.Generating and maintaining documentation, including analyses, specifications, test procedures, reports, and design descriptions.Designing and configuring Navigation or Communication subsystems for satellite applications.Coordinating technical aspects with customers, vendors, subcontractors, project teams, system engineering, and other divisions.Presenting work results internally and in front of customers.Developing test concepts and providing support during the test phase.As a Team Lead of the System Engineers, you are the supervisor of the System Engineers. You will be responsible for:Monitoring proper execution of tasks assigned to the teamPeople Management of the team:Managing the team skills and expertise in line with the company &amp; project needs.Following up on career and personal growth through evaluations and individual trainingFacilitating communication and collaboration, in and outside the teamSupporting the hiring of new colleaguesOn-boarding and mentoring/coachingHarmonizing the system engineering methodology and tools across all projects, in line with the relevant standards (e.g. ECSS)Ensuring the integrity, consistency and technological evolution of products and/or team specific competences in support of projects. This includes supporting business development and proposal activities with strategical insights on product roadmaps and the company’s technical capabilities.Supporting the COO in close coordination with the other team leads in creating/maintaining balanced project teams, by taking into account skills, aspirations and availability of resources. Desired skillsMaster's degree in electrical engineering, communication engineering or a comparable qualificationProfessional experience as a multidisciplinary system engineer in Navigation, Radar, or Communication projectsAble to work both independently and in large projectsExperience in dealing with customers and vendors is advantageousPlanning &amp; organization skillsFluency in English; knowledge of Dutch is a plusMandatory Requirements Eligible for an EU security clearance (EU citizen, or eligible for citizenship and living in the EU for at least 10 years) -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GNSS Engineer – Space Unit Position DescriptionJoin CGI Space to fuel tomorrow's GNSS Innovations!Your role in our teamAs CGI Space in the Netherlands, we're at the forefront of developing a cutting-edge G2G user performance tool, and we're on the lookout for a highly motivated engineer as you to join our team. We focus on GNSS and, more specifically, G2G related projects. In addition to this, we're actively involved in creating simulation tools that replicate behavior and analyze the performance and reliability of GNSS signals.In this role, you'll play a pivotal part in the continuous advancement of our G2G performance tool. Your contributions will shape the future of GNSS technology and its impact. Your enthusiasm and expertise will be valued as we explore new horizons in this dynamic field.How You Strengthen Our TeamYour interest in technology, coupled with your willingness to explore beyond your expertise, is highly valued. We're looking for candidates like you with the following skills and competencies: A Bachelor's or Master's degree in Electrical, Telecommunications, Geodetic, Aerospace, or related engineering fields. Strong understanding of GNSS principles from both user and system perspectives. Knowledge of error sources affecting GNSS and associated models (e.g., ionosphere or multipath models). Experience in evaluating GNSS performance and related statistics and algorithms. Proficiency in precise GNSS products (e.g., precise ephemerides and clock data). Understanding of PNT principles using GNSS technologies (e.g., pseudorange calculations and Kalman filtering). Familiarity with object-oriented programming in MATLAB and/or C++ is advantageous. Proficiency in software engineering aspects, including requirement definition, architectural design, implementation, and testing. Please note that holding an EU passport is mandatory for obtaining an EU Personal Security Clearance at the CONFIDENTIAL level, which is a part of our selection process. Your contributions will be instrumental in strengthening our team and advancing our GNSS technology initiatives.A pre-employment screening is part of the application processWhy CGI? CGI is one of the world's largest IT consultancy firms. Our people keep the Netherlands running. Government agencies, banks, aerospace, infrastructure organizations and energy and manufacturing companies are clients of CGI. We work on interesting projects that touch the daily lives of millions of people. We are present regionally, augmented with global domain knowledge, our ecosystem, and colleagues spread all over the world. We are proud of the impactful projects that we, together with our colleagues, make a success.At CGI, we place great value on diversity and inclusion, as this not only promotes collaboration but often leads to better results. We look forward to your contribution to our team! Work in small self-managing teams consisting of experts in your field Take control of your own career with the space to continue developing yourself You work with the latest technologies An excellent salary and attractive secondary employment conditions Immediate permanent contract Part-time possibilities And the opportunity to become a CGI shareholderJoin our team of experts and apply now! We will contact you as soon as possible. Questions about the position? Ask them to Gert Mariën, Director Consulting Services via gert.marien@cgi.com.For more information about the application procedure, please contact recruiter Chris Nikijuluw via + 31 6 204 51 105 or chris.nikijuluw@cgi.comWe do not collaborate with external recruitment agencies. Therefore, unsolicited acquisition is not appreciated.Your future duties and responsibilitiesRequired Qualifications To Be Successful In This RoleTogether, as owners, let’s turn meaningful insights into action.Life at CGI is rooted in ownership, teamwork, respect and belonging. Here, you’ll reach your full potential because…You are invited to be an owner from day 1 as we work together to bring our Dream to life. That’s why we call ourselves CGI Partners rather than employees. We benefit from our collective success and actively shape our company’s strategy and direction.Your work creates value. You’ll develop innovative solutions and build relationships with teammates and clients while accessing global capabilities to scale your ideas, embrace new opportunities, and benefit from expansive industry and technology expertise.You’ll shape your career by joining a company built to grow and last. You’ll be supported by leaders who care about your health and well-being and provide you with opportunities to deepen your skills and broaden your horizons.Come join our team—one of the largest IT and business consulting services firms in the world.
-            Show more
-            Show less Engineering and Information Technology IT Services and IT Consulting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PhD position - degrowth and tipping points of food systems, Maastricht Sustainability Institute The Maastricht Sustainability Institute is offering an exciting opportunity for a fulltime PhD position of four years in political economy and sustainability science. Job Description The emerging paradigm of degrowth entails unprecedented changes in policy, economic activities, and individual behaviours in order to constrain production-consumption systems within planetary boundaries. The PhD candidate will empirically explore the feasibility and impacts of such changes on food provision systems in the European Union. Urgent research is needed to improve the understanding of systemic interactions between 1. evolutions of food supply chains, markets, individual livelihoods, and dietary habits; 2. their consequences on spatial organisation, social inequality and conflicts; and 3. the political dynamics of populism and nationalism in Europe. The PhD candidate is expected to conduct novel research on food production-consumption systems in France and the Netherlands. Research tasks can be adjusted to suit specific skills and expertise, but will rely on a systemic perspective and an empirical exploration of degrowth via, e.g.: Mapping out and comparing social aspects and material flows of food systems in France and the Netherlands;Exploring the consequences of degrowth on food systems, e.g., retraining of the workforce and reorganisation of space;Shedding light on interactions between nationalist or populist trends and food systems, such as the entanglement of meat consumption with certain political worldviews;Improving understanding of derailment risks and positive tipping points by comparing “business-as-usual” and “degrowth” scenarios;Developping a transition toolbox for the benefit of food systems actors (farmers, cooperatives) to act on positive tipping points. The candidate will be supervised by Prof. Frank Boons, based at Maastricht Sustainability Institute (MSI), Maastricht University, and be co-supervised by Dr. Clarence Bluntz at MSI. The candidate is expected to contribute to teaching activities in the field of sustainability at the department, taking max. 20% of their time (typically Master-level courses and supervision of Master theses). Requirements We are looking for candidates: who have successfully completed a Master’s degree in a relevant area, e.g.: political economy, ecological economics, sustainability science, food systems.with a record of high academic achievement: Master thesis’ grade, involvement in research papers, in other academic activities; or in research activities outside of academia (e.g., think tanks, NGOs).with a strong interest in one or more of the following research topics: degrowth, food, populism, nationalism, social and environmental impacts of dietary habits, rural-urban divide.with a very good command of written and spoken English, and with working knowledge of Dutch and/or French.enthusiastic about travelling in the Netherlands and France to work with food systems’ actors.What we offerAs PhD position - degrowth and tipping points of food systems, Maastricht Sustainability Instituteat School of Business and Economics, you will be employed by the most international university in the Netherlands, located in the beautiful city of Maastricht. In addition, we offer you:Good employment conditions. The position is graded in scale PhD according to UFO profile PhD, with corresponding salary based on experience ranging from €2770,00 and €3539,00 gross per month (based on a full-time employment of 38 hours per week). In addition to the monthly salary, an 8.0% holiday allowance and an 8.3% year-end bonus apply.An employment contract for a period of 18 months with a scope of 1.0 FTE. Upon a positive evaluation, an extension of 2,5 years will follow.At Maastricht University, the well-being of our employees is of utmost importance, we offer flexible working hours and the possibility to work partly from home if the nature of your position allows it. You will receive a monthly commuting and internet allowance for this. If you work full-time, you will be entitled to 29 vacation days and 4 additional public holidays per year, namely carnival Monday, carnival Tuesday, Good Friday, and Liberation Day. If you choose to accumulate compensation hours, an additional 12 days will be added. Furthermore, you can personalize your employment conditions through a collective labor agreement (CAO) choice model.As Maastricht University, we offer various other excellent secondary employment conditions. These include a good pension scheme with the ABP and the opportunity for UM employees to participate in company fitness and make use of the extensive sports facilities that we also offer to our students.Last but certainly not least, we provide the space and facilities for your personal and professional development. We facilitate this by offering a wide range of training programs and supporting various well-established initiatives such as 'acknowledge and appreciate'. The terms of employment at Maastricht University are largely set out in the collective labor agreement of Dutch Universities. In addition, local provisions specific to UM apply. For more information, click here. Maastricht University Why work at Maastricht University? At Maastricht University (UM), everything revolves around the future. The future of our students, as we work to equip them with a solid, broad-based foundation for the rest of their lives. And the future of society, as we seek solutions through our research to issues from all around the world. Our six faculties combined provide a comprehensive package of study programmes and research. In our teaching, we use the Problem-Based Learning (PBL) method. Students work in small groups, looking for solutions to problems themselves. By discussing issues and working together to draw conclusions, formulate answers and present them to their peers, students develop essential skills for their future careers. With over 22,300 students and more than 5,000 employees from all over the world, UM is home to a vibrant and inspiring international community. Are you drawn to an international setting focused on education, science and scholarship? Are you keen to contribute however your skills and qualities allow? Our door is open to you! As a young European university, we value your talent and look forward to creating the future together. Click here for more information about UM. The School of Business and Economics The School of Business and Economics (SBE) is one of Maastricht University’s six faculties. Our mission is to contribute to a better world by addressing societal problems, by co-creating knowledge and developing team players and leaders for the future. By joining SBE, you will be part of the 1% of business schools worldwide to be Triple Crown accredited (EQUIS, AACSB and AMBA). You will join an inspiring and international environment, where learning and development is priority. Department The Maastricht Sustainability Institute has strong collaborations with other institutes and departments at Maastricht University and elsewhere. We offer a dynamic and challenging job in an internationally oriented organisation. Curious? Are you interested in this exciting position but still have questions? Feel free to contact Clarence Bluntz via c.bluntz@maastrichtuniversity.nl for more information. Applying? Or are you already convinced and ready to become our new PhD? Apply now, no later than August 25th, 2024 for this position. Applicants are expected to include a motivation letter (max. 2 pages), a CV, and contact information for one referee. Applicants selected for an interview will be contacted by the end of August and given instructions to write a short (3-5 pages) research proposal. This is to get a broad idea of how they would tackle the research topic. They will present this proposal during the interview, which will be conducted in September The successful candidate is expected to start in the position fully by January 2025 at the latest; earlier if possible. The vacancy is open for internal and external candidates. In case of equal qualifications, internal candidates will be prioritized. Maastricht University is committed to promoting and nurturing a diverse and inclusive community. We believe that diversity in our staff and student population contributes to the quality of research and education at UM, and strive to enable this through inclusive policies and innovative projects led by teams of staff and students. We encourage you to apply for this position. - Website for additional job detailshttps://www.academictransfer.com/343618/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">About the project:The transition of airflow from laminar to turbulent state is a major contributor to aerodynamic drag and consequently aircraft emissions. Often, unavoidable modifications of the wing surface, such as panel joints or skin deformations decrease the extent of laminar airflow by promoting transition. However, through our research, we showed that this is not always the case. In a recent breakthrough, our team discovered the “Delft Laminar Hump”, a passive smooth surface modification. The proof-of-concept experiments showed the capability of the Hump to create an unprecedented delay of transition, effectively increasing the extent of laminar flow.The “Running up that Hill” project aims at achieving a clear physical understanding of the interaction between laminar-turbulent transition and surface modifications such as the Delft Laminar Hump.The fundamental and technical outcomes of this work will position Hump-like surface modifications as an enabling technology for curbing environmental emissions of aviation. In addition to fundamental work, the project is supported by leading aerospace partners such as KLM, DNW, and Deharde as well as by world-leading groups at U. Waterloo, Canada and KTH, Sweden. Opportunities for research stays with these organisations will be available within the project.We are seeking two enthusiastic and skilled PhD candidates to join our team and work on this exciting project.Important: during submission, please indicate in your motivation letter which of the following two positions you are interested in:PhD position 1: will encompass theoretical and numerical modelling, necessary to simulate the effect of surface modifications on swept wing transition. Flow stability analysis tools available in our team can be used, including Orr-Sommerfeld solvers, linear/non-linear Parabolised Stability Equations and our non-linear Harmonic Navier-Stokes solver. An extensive validation effort will involve high-fidelity Direct Numerical Simulations, in collaboration with the group at KTH Stockholm (Prof. D. Henningson and Dr. A. Hanifi). Research stays at KTH will be covered by the project.PhD position 2: will explore the experimental design and testing of laminar hump models and undertake advanced flow measurements to characterise the underlying transition mechanisms. The candidate will work in the state-of-art windtunnel facilities at TU Delft. The experimental activities will also involve collaboration with U. Waterloo, Canada (Prof. S. Yarusevych), with research stays available.About the team:We are a young, international, and diverse team of colleagues working on topics closely related to the newly founded chair of Flow Control. We approach problems in a horizontal “team spirit” and continuously traverse boundaries between theory, simulations, and experiments towards understanding and controlling fluid flows. Our team, strives for a co-creative and stimulating environment where we can develop our skills as a scientist, team member and teacher. We place great emphasis on a collegial working environment where everyone is welcome and encouraged to shape their PhD track. We also enjoy many team-building activities and events where you can get to know your teammates in a different environment, share personal life experiences and have a great time outside of the lab!Accessibility:Almost 90% of our laboratory and offices are wheelchair accessible, including all wind tunnel facilities. If you have any specific concerns about accessibility, please don’t hesitate to contact us (see below for contact information).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area of research:Scientific / postdoctoral posts,SonstigesJob description:Increasingly, model-based system design (MBSE) is applied in the development of space systems. Information is exchanged using central domain models, which on the one hand allows engineers to work closely together on the design and on the other hand enables analyses and optimizations of the entire system. DLR's own MBSE-tool "Virtual Satellite" has been used successfully for years for system design and within concurrent engineering studies. Join us in our work on developing MBSE as well as “Virtual Satellite” and be responsible for the following tasks: you will maintain close contact with project partners and engineers in order to continuously improve the design processes for space systemsyou will develop new modelling approaches/processes and conduct research in the field of requirements engineeringyou will integrate the developed approaches into "Virtual Satellite”you will support the planning of new space missions in the DLR Concurrent Engineering FacilityIf you enjoy software development and want to become part of our team, we look forward to receive your application. We are looking for highly motivated colleagues who can identify with their work and inspire others. We also offer you the opportunity to contribute with your own ideas and to initiate new projects on your own responsibility. You will be expected to present your work at international conferences and in scientific journals. We offer an exciting, friendly, and flexible working environment where part-time employment is also possible. This research center is part of the Helmholtz Association of German Research Centers. With more than 42,000 employees and an annual budget of over € 5 billion, the Helmholtz Association is Germany's largest scientific organisation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area of research:Scientific / postdoctoral posts,SonstigesJob description:A central research area of the "Optical Satellite Links" department is optical satellite communication for connections from low and geostationary orbit to the ground and between satellites. The department is also involved in laser-optical aeronautical communication for passenger aircraft and drones, for example. Another important area of research is satellite-based quantum communication. Here, the department is working on solutions to efficiently transmit photonic quantum states between satellites and ground stations.The research group "Mitigation of Atmospheric Influences" deals with future applications of optical free-beam transmission (using laser technology) through the atmosphere and in space. Research activities are focussing in particular on overcoming the Earth's atmospheric layers and the resulting interference to transmission paths. The research work is then simulated and verified as part of laboratory tests and extensive measurement campaigns.In order to be able to transmit the extremely high and constantly growing volumes of data, optical communication methods must achieve ever higher performance. Overcoming atmospheric turbulence between ground and GEO stations orbiting the earth is a key prerequisite for this. Research focuses on the development of highly efficient field sensors for adaptive optics systems under strong turbulence, real-time control systems that can process the sensor data and make corrections at high speed, control algorithms for the best possible calculation of the required correction and "pre-distortion" systems that stabilise the uplink beam to the satellite.As the responsible group leader, you will ideally have a solid knowledge of the fundamentals of physics, especially adaptive optics, for these activities. In addition, in-depth knowledge of optical communication technologies is of great importance. As a group leader, you are also responsible for the technical management and achievement of your group's research objectives. This includes the organisation of your group with a clear allocation of tasks and roles, but also the individual development of your employees and supporting the head of department in technical and administrative matters.We offer you the opportunity to work on innovative research projects with state-of-the-art technology in an ambitious international environment. Flexible working hours including an individual agreement on mobile working are part of our offer to you.This research center is part of the Helmholtz Association of German Research Centers. With more than 42,000 employees and an annual budget of over € 5 billion, the Helmholtz Association is Germany's largest scientific organisation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area of research:Scientific / postdoctoral posts,Sonstiges,PromotionJob description:The Navigation department develops methods and systems for interference-free satellite navigation and communication for high-precision positioning and wireless broadband data transmission, for example via satellites.The "Antenna Systems" research group is involved in the development of the next generation of satellite navigation and communication systems.For future satellite and terminal antennas, which will be used in satellite navigation for interference-free and highly accurate positioning and in communication for broadband data transmission, you will work with us to design technologies and contributions to improve and expand the calculation methods. We set up appropriate laboratory models for validation and test them in teams and with other research groups as part of demonstrations.Your tasks will include analysing, critically evaluating and verifying the electromagnetic properties of antennas in the high-frequency and microwave range (computationally and experimentally). We offer you a pleasant working atmosphere in a successful research and development group, state-of-the-art equipment and an environment with national and international co-operations. Opportunities for professional development (e.g. PhD, PMP Project Management) are available.Flexible working hours and an individual agreement for mobile working are a matter of course for us. If you are interested, we look forward to getting to know you!This research center is part of the Helmholtz Association of German Research Centers. With more than 42,000 employees and an annual budget of over € 5 billion, the Helmholtz Association is Germany's largest scientific organisation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">doctoral network – DC8 University of Évora (UÉ) Supervisors: Célia Antunes and Inga Wessels The Dust-DN doctoral network Atmospheric dust or mineral dust (or simply “dust”) is a major atmospheric aerosol, and it gives us one of the most visible and detectable aspects of transboundary transport of atmospheric constituents, impacting visibility, radiation and climate. What is less evident are its quantitative impacts on health, transportation and energy production. Atmospheric dust is not fully understood at the fundamental level (microphysical properties, dust emissions, source regions) and hence atmospheric models fail to fully reproduce its impacts. Moreover, dust observations using ground-based instrumentation, remote sensing and aircraft are abundant, but not evenly distributed; in particular they are missing near the major dust sources. Moreover, the techniques are still under development, with each giving a different picture of a phenomenon with multiple facets. For example, it is now known that super-coarse and giant dust particles have gone undetected for a long time due to limitations in the measurement and modelling tools that have been in use for decades, and this misdetection alters the understanding and the prediction of a number of processes. Finally, dust affects the environment, society, and several economic sectors, with impacts on the transportation and energy sectors for example, the nature and cost of which is not fully understood and quantified. Several methodologies exist to study mineral dust, each giving its own differing picture of a complex phenomenon: numerical modelling, remote sensing, in-situ observations, laboratory research. We established the Dust Doctoral Network (Dust-DN), in order to address gaps in the understanding of dust and its impacts by linking the different disciplines and methods. The aim is to train a team of early career scientists into overcoming compartmentalism in this field of science, and into developing a multi-disciplinary approach to mineral dust. Dust-DN will set up a network of academic and non-academic partners working on different aspects of dust research, and will coordinate a program of doctoral projects that will enhance knowledge across a broad range of fundamental, but linked, components of the atmospheric dust life cycle and its impacts. The projects will span across the disciplines of atmospheric sciences (dust processes, modelling, and remote sensing), geology (dust emissions and source regions), as well as the impacts on society and economic sectors. The knowledge will be shared among participating institutions and the wider public and scientific community. Common activities will be held, so as to enhance the network among the partner institutions and among the doctoral researchers, delivering an ambitious advanced training program for capacity building. The University of Évora The University of Évora (UÉ) in Portugal is a public institution organized into five schools: Fine Arts, Sciences and Technology, Social Sciences, Health and Human Development, and Nursing. Within UÉ, the Institute for Advanced Studies and Research (IIFA) serves as a crucial unit, merging teaching with research to foster interdisciplinary knowledge and support existing R&amp;D units. IIFA coordinates 35 PhD programs and two Erasmus Mundus Master programs, ensuring an integrated advanced training environment and offering a wide range of soft skill training. IIFA also oversees 19 research centres, funded by the PT Foundation for Science and Technology. One of these R&amp;D units is the Institute of Earth Sciences (ICT), a multidisciplinary team focusing on Earth System Science and Energy. This team is transitioning to the newly established Centre for Sci-Tech Research in Earth System and Energy (CREATE). CREATE emphasizes integrated research on critical Earth System and Energy challenges, along with technological innovation. It comprises 121 members, including 48 integrated PhD researchers and 39 PhD students. The selected candidate will be working at the ICT/CREATE R&amp;D units of UÉ, gaining access to several observational platforms for atmospheric research in southern Portugal. These platforms include the Évora Atmospheric Sciences Observatory, the Alqueva Lake floating station, oceanic sites at Cabo da Roca and Sines, a mobile air quality platform, and regional networks of weather and solar radiation (BSRN compliant) stations. The team also coordinates specialized research labs in Precision Optics, Atmospheric Physics, Solar Radiation Sensors, Thermofluids &amp; Energy, Bioaerosol &amp; Aerobiology, and Health &amp; Environment. Additionally, a computational cluster with 512 processing cores and 1TB of RAM distributed over eight nodes is available for research purposes. Researchers at all stages of their careers find at ICT/CREATE a dynamic and friendly environment, where personal relationships easily thrive in an inclusive atmosphere, and flexible work planning promotes a life beyond work. The PhD project Doctoral Candidate 8 (DC8) – “Assessment of the respiratory health impact of atmospheric dust” Enrolled in the University of Évora’s PhD programme on “Earth and Space Sciences”. This project has the objective of evaluating the impact of different dust conditions simulating reality on lung epithelial layer function, with a focus on its relation to the concentration and physical and chemical features of the dust. The candidate will prepare and characterize the dust samples in terms of particle size and composition and will expose the lung epithelial cells in air-lift culture to controlled dust conditions, simulating real atmospheric aerosol concentrations. The candidate will also assess the integrity of the epithelial barrier by TEER (Trans-epithelial Electrical Resistances) measurements and histomorphology evaluation, as well as evaluate the epithelial cell activation and inflammation biomarkers (proinflammatory cytokines IL-18, IL-6, IL-8, TNF alpha and fibrotic chemokines, e.g. TGF beta;) and epithelial responses (mucus production; Reactive Oxygen species – ROS). The doctoral candidate will be based at UÉ in Évora, Portugal and will be supervised by Prof. Célia Antunes (UÉ) and Doctor Inga Wessels (ZAUM). Prof. Daniele Bortoli (UÉ) will also contribute to the supervision. The project will include a planned secondment at the Center of Allergy and Environment – Technical University of Munich (Germany) (7 months in the beginning of the second year). Details The recruited PhD candidate will be enrolled in UÉ’s PhD programme on “Earth and Space Sciences” and is included in the “Dust Doctoral Network”, which involves highly prestigious research groups on this scientific topic, and which will ensure that the cohort of doctoral candidates is integrated in a dynamic and enthusiastic scientific environment. The doctoral candidate will learn about the consortium partners’ unique facilities and research topics/methods, and will exploit these opportunities for their research. All Dust-DN doctoral candidates will work side-by-side with lead scientists at world-leading institutes, and they will: ● Take responsibility for the scientific project that they are involved in, and the instruments and/or softwares required. ● Collect scientific knowledge through experiments and/or numerical modelling. ● Develop tailor-made data processing methods. ● Advance the fields of research in atmospheric dust and/or the related measurement techniques. ● Participate in the Dust Doctoral Network training and networking activities ● Publish the results of the research in scientific peer reviewed journals, and present at conferences and workshops. Qualification Requirements · The candidates are required to possess an excellent master’s degree (or equivalent) in natural or life sciences and to not have any kind of PhD degree. · Motivation for research on atmospheric dust. · Experience or aptitude to develop scientific software (computer-based programming) · Demonstrated ability in being a strong team player. · Strong international mobility for the purpose of research, training, and dissemination is mandatory. Preferred Qualifications Additional appreciated skills and competencies are: ● Experience in applying broad scientific knowledge to a range of specific problems or scenarios. ● Previous research experience and/or previous interest in the natural or life sciences or closely related discipline will be appreciated. ● Experience with written or oral communications. ● Fluency in written and oral English is highly valued. ● Publication record. ● Driving licence. Eligibility Requirements · Qualifications: The candidate must hold a title satisfying the admission requirements for a doctoral candidate at the institution where they will be enrolled (see qualification requirements). A doctoral degree in any field is not compatible with these positions. · Mobility: Transnational mobility is an essential requirement of MSCA Doctoral Networks. At the time of recruitment, the candidates must not have resided or carried out their main activity (work, studies, etc.) in Portugal for more than 12 months in the 3 years immediately prior to the recruitment date. Applicants must be aware that seconding periods are planned for this position as described above. International applicants are welcomed. Rights and Responsibilities of Researchers Participating in Marie Skłodwska-Curie Actions The European Charter for Researchers is a set of general principles and requirements which specify the roles, responsibilities and entitlements of both researchers and the employers and/or funders of researchers. The aim of the Charter is to ensure that the nature of the relationship between researchers and employers or funders is conducive to successful performance in generating, transferring, sharing and disseminating knowledge and technological development and to the career development of the researchers. It is obligatory for applicants to read and understand the detailed information regarding the rights and responsibilities of researchers engaged in an MSCA Doctoral Network. The European Charter for researchers can be accessed at: https://euraxess.ec.europa.eu/jobs/charter/european-charter Employment Contract and Financial Aid The selected candidate will be appointed under a 36-months full-time employment contract. A competitive financial aid package will be offered to the successful candidate with a gross annual salary of €35,246 (living allowance and mobility allowance). In addition, there can be further allowances depending on family status and other needs, as per MSCA relevant provisions. It is understood that failure to successfully continue the PhD program will result in immediate cancellation of the employment contract and the financial support provided. Start date The position starts on 3 February 2025 and is a full-time position (40 hours/week), funded for a period of 36 months. Application and selection Application advisory: A pre-screening of the candidates will be made by the Dust-DN consortium as a first step prior to the formal recruitment process. Candidates should submit a CV and motivation letter on the Dust-DN website, together with their university transcripts and the name and contact information of two referees, and indicating up to 3 preferred doctoral projects (in order of preference) amongst the ones advertised within the whole Dust-DN (which includes the one in the present advert). It is very important that the motivation letter should recall each of the qualification requirements and preferred qualifications indicated in this advert, clearly justifying how the candidate is able to meet each of them, and providing evidence. After short-listing, the most suitable candidates will be called for an interview. Formal recruitment phase: The most highly-ranked applicants interviewed during the application advisory phase will be re-directed for the formal application. With the submission of the documents, applicants agree that the documents will be shared among all supervisors of the Dust-DN consortium and members of the respective shortlisting and interviewing panels. Dust-DN respects and supports the compatibility of professional and private life and promotes development opportunities for its cohort of doctoral researchers. We promote equality of opportunity, value diversity and nurture a working and learning environment. Deadlines: Applications for the advisory phase must be submitted by 31 August 2024. Formal applications must be submitted by 30 November 2024. We reserve the possibility to extend the deadline(s) if not enough candidates apply. Contact Information For further information, please contact Professor Célia Antunes (e-mail: cmma@uevora.pt).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assessing the evolution of marine heat waves in conjunction with ocean warming and induced variations in ocean stratification/vertical structureSubject areaPhysical oceanography, air-sea interactions, global warming, climate change, extreme events, marine heat wavesSubject descriptionThe last two decades have seen a significant increase in the frequency and intensity of extreme weather events, including tropical cyclones, heat waves, heavy precipitation, and wildfires. The same is true for extreme events in the ocean, notably marine heat waves. These are part of a new and alarming trend in which we see the compounding effect of multiple extreme events occurring simultaneously or in succession, amplifying the collective impact and posing increasing challenges to human infrastructure and livelihoods around the world.Extreme events and their linkages are a combination of synoptic atmospheric (weather) and ocean circulation and their linkage to climate drivers that result in potentially high-impact events. To mitigate and better adapt to compound extreme events, we need to better understand the phenomenology and evolution of these extremes in a changing climate. These events, and in particular, marine extreme events might be related to the observed ocean warming. In fact, terrestrial weather patterns and climate are determined by the amount and distribution of solar radiation incident on our planet.To maintain a climate (statistical) equilibrium, the radiation leaving the Earth system towards space must equal the solar radiation absorbed, although numerous atmospheric, oceanic and terrestrial phenomena interact to couple these fluxes. Solar radiation can be diffused, reflected or absorbed by the atmosphere and the earth's surface, then transformed into heat, latent, potential and kinetic energy, before being re-emitted to space in the form of long-wave radiation. This energy can be stored, transported and converted, generating various meteorological and oceanic phenomena. Today, this energy balance is being perturbed in unprecedented ways by human activities, with the ocean playing a central role in this disruption. More energy is entering the climate system as compared to the amount of energy leaving it. This unbalance is defined as the Earth Energy Imbalance (EEI). As a consequence, heat is accumulating in Earth climate. Most of this surplus heat is stored in the ocean, about 90%, and it is measured in terms of ocean heat content. The latest results indicate that global warming is accelerating (Minière et al., 2023; Storto et al., 2024).This, potentially accelerating, ocean warming alters the vertical structure of the ocean inducing a stronger stratification of the upper layers and might favor the genesis, intensification and duration of Marine Heat Waves together with changes in atmospheric ocean circulation drivers (Oliver, 2019). Indeed, the surface temperature of the oceans has been rising, with extreme periods occurring more frequently over the past two decades. These are known as marine heat waves, or MHWs (Frölicher et al., 2018). We do not yet know the extent and depth of such events, nor do we know their connection to the atmosphere in terms of drivers and impacts. Nevertheless, these extreme warming events have been documented to have significant impacts on marine ecosystems (Smale et al., 2019; Smith et al., 2023), as well as on human well-being and regional economies (Holbrook et al., 2022). In this PhD project, we will address this issue by focusing on the Atlantic Ocean which has been identified as one of the major regions of ocean warming (e.g., Cheng et al., 2023; Li et al., 2023) and where changes and extreme events have been observed to increase in frequency and intensity.The candidate will work within the framework of the Europe Horizon2030 project ObsSea4Clim (Ocean observations and indicators for climate and assessments : https://obssea4clim.eu). One of the main focus of ObsSea4Clim is to assess MHWs and with this provide a better framework for observing and predicting actionable indicators for sustainable development and climate change adaptation.The objectives are to:Analyze critical areas of regional heat accumulation and changes in stratification as well as MHWs impacted areas under global warming.Identify the most critical areas (e.g., structure of the ocean circulation, modes of internal climate variability, synoptic atmospheric circulation) how heat is redistributed into the deep ocean layers, and how this has changed the vertical ocean stratification.Understand the regional development of MHWs processes and decipher how these have changed with ocean warming and stratification together with the regional synoptic atmospheric circulation.The questions to be addressed are:What are the elements of the regional ocean system that are changing ? Are there key ocean processes that can explain the observed behavior ?What are the respective roles of the ocean warming and atmosphere circulation and their interactions in a warming climate in the observed changes in MHWs ?Do current climate models correctly represent these phenomena? What do large ensembles of climate simulations tell us about the processes in point (b)? Indicative work programDetailed characterization of regional ocean warming and marine heat waves based on analysis of analysis of historical data from observations and reanalyses.We will focus on the Atlantic OceanComposite study of periods of ocean warming, stratification and marine heat wavAnalysis of CMIP6 models using the methods defined in points (1) and (2). At the end of the thesis, based on the results obtained, we will be able to design sensitivity experiments using the IPSL global climate model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We are looking for GIS and remote sensing expert to work with data from drones with LIDAR and hyperspectral sensors and other spatial data processing and analysis within the new project:FORSOMICS: Research team and infrastructure upgrade to study the mechanism of conifer resistance to bark beetles in a changing climate: From Gene to Tree Level.And also partially within the project RESDiNET: NETWORK FOR NOVEL REMOTE SENSING TECHNOLOGIES IN FOREST DISTURBANCE ECOLOGY.https://resdinet.eu/The project job position ends on 30.6.2026</t>
+    <t xml:space="preserve">As part of its growth and acceleration plan, Kylii Kids is recruiting a Business Developer for the playground and leisure sector to continue promoting its interactive treasure hunt Kylii Quest in Germany, the Netherlands, Belgium and Nordic countries Kylii Kids is the leader in interactive children's play and spaces. We transform physical spaces into places for families to experience. We support our customers in the design and deployment of interactive games for children to attract, entertain and keep families coming back to their establishments. We have deployed more than 1,100 solutions in 20 countries in the leisure, restaurant, retail and petrol station sectors. YOUR PROFILE :   You have a minimum of 2 years' higher education (BAC + 2) with a commercial/sales background.  You speak German, English and French (not mandatory)  You have good listening and negotiating skills  You enjoy BtoB development and sales  You have professional written and spoken skills  You have a good command of office automation tools (CRM, google suite)  You have good interpersonal skills and are a team player  YOUR MISSION :  You will work under the responsibility of the CEO and will be responsible for the following tasks:   To promote and sell the Kylii Quest interactive treasure hunt to the leisure sector in Northern Europe.  Prospect and win new customers in the leisure sector (indoor and outdoor play parks)  Increase sales with existing and prospective customers by organizing on-site demonstrations with management support  Draw up sales proposals, negotiate contracts and renewals  Carry out regular reporting using CRM  Develop and participate in operational marketing initiatives  Job Type: Full-time Schedule:   Monday to Friday  Language:   English (Required)  German (Required)  Work Location: In person Expected Start Date: 09/09/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At Mango we inspire and we unite through our passion for style and culture. We are present in more than 115 countries and our online presence extends to more than 110 countries. Our team is made up of people of 112 nationalities and 78% of them are women.        We are looking for     ASSISTANT STORE MANAGER (35 hours - Anvers)     WHAT WOULD YOUR DAY TO DAY BE LIKE AT MANGO?        You will support the store manager in the effective running of the shop by delivering improved sales performance, ensuring excellent customer service and ensuring the team performs daily tasks in a positive environment.          We are hiring for our Flagship store in Belgium!              Must be eligible to work in Belgium.          Key Responsibilities:        Plan, implement, and monitor measures required to meet and exceed sales targets     To possess a good product knowledge and fashion awareness.     To know and apply the visual merchandising standards of the brand and of the season.     Ensure and collaborate in the implementation of merchandising standards and optimize sales space to maximize profitability     To act as a role model and promote effective communication within the sales team.     To recruit, train and ensure the seamless integration of new employees.          What are we looking for?        Relevant experience in managing and visual merchandiser in a dynamic shop within the fashion retail industry (At least 1 year)     Customer and image-oriented, having product awareness and commercial orientation     Excellent command of English - written and spoken     Motivation and passion for managing people by example     Sales oriented person organized and tenacious, problem solver, able to work well under pressure and adapt to change.          WHAT MAKES US SPECIAL?      Discount on all our lines (Woman, Man, Kids, Teen &amp; Home).    Uniform per season.    Meal vouchers.    Constant development opportunities with varied challenges that generate on-the-job learning.    Close, inspiring, and ambitious work environment.    You will be part of a leading company in the fashion industry, dynamic and in full innovation.     You got it?   We like you!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Who is Kadonation?        Kadonation was founded in 2016 and is today one of the fastest growing companies in Belgium.  Our scale-up is a dynamic player in the employee and corporate gifts market. Unwrapping the impact of gifting, that’s our motto. And it’s also the reason we built Kadonation Select: an intuitive platform that allows organisations to set up a well-thought-out recognition policy in no time. Our software takes away the administrative burden that comes with employee gift-giving. In short: more appreciation, less hassle!  Want to know more about our story, the core values we strive for and the mission we’re working on with around 40 talented individuals? Read more here.            We’re looking for…        … an Account Executive to approach prospects and convince them of the power of our Kadonation Select platform. You’ll take ownership of the Dutch-speaking market within the Benelux and focus on expanding the pipeline and closing deals.  What are your responsibilities?               You’ll be responsible for lead generation and sales of our B2B platform in Flanders and the Netherlands.       You’ll ensure your own stable flow of outbound leads, follow them up and also be responsible for closing the deals.       Even after the deal is closed, you’ll continue to maintain a relationship with the customers in your portfolio, focusing on up- and cross-selling to increase recurring revenue.  Clear communication and administration in the CRM.  You’ll be an ambassador for Kadonation, which means introducing yourself to the customer with pride!       Focus: B2B sales at companies in Flanders and the Netherlands with 100‑1000+ FTEs.       You’ll work from our office in Ghent (2d/w) and visit customers on site where necessary.                   What is your profile?          You’re a real hunter and get a thrill out of closing deals with new customers.  You’re a go-getter who is not easily discouraged. You know that your strength lies in a consistent approach.  You can tell a story with passion and conviction and have the necessary sales techniques to close a customer.  Strong team spirit, goal-oriented and transparent communication.  You have a proactive attitude and a results-oriented mindset.  You’re a team player and have a positive mindset.  You work independently and use your time efficiently.       You have at least 2 years of experience in B2B sales, preferably with proven successes in cold acquisition. Do you have more experience? That’s certainly something we’re interested in.       Your Dutch is perfect and your English is good.  You have a bachelor’s degree or equivalent experience.       Your experience in sales with HR or marketing as the target group is a big plus.               What can we offer you?             An enthusiastic team and a friendly office environment where even your dog is welcome.              The chance to experience the growth of a scale-up up close and to put your stamp on it.              A 38-hour week with 26 days of leave and, in addition to a competitive salary, a flexible salary package. Including, for example, a company car, meal and eco vouchers, training and workplace budget, plus hospitalisation insurance. And of course, there’s also an extensive gift policy for your professional &amp; personal milestones, but that probably doesn’t come as any surprise!              A good work – life balance, with flexible hours and the option to work from home (up to 3 days a week).               Why join Kadonation?        At Kadonation we connect the energy and ambition of a start-up to the expertise and know-how of a scale-up. You’ll be working in a dynamic tech company with an open feedback culture and space for your own initiative and ideas. And above all: we like to make you feel truly appreciated.  Do you also believe in our product? Apply now to join our sales team!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">About AppTweak    AppTweak is the trusted app store acquisition partner for mobile leaders worldwide; we provide innovative solutions that help apps and games optimize their app store presence and increase downloads. For 10+ years, companies including Uber, Adobe, and Zynga have trusted our unique metrics, actionable insights, and expertise to make informed decisions and achieve long-term success in the competitive mobile market.    Driven by data science and a human-centered approach, AppTweak is recognized for its innovative features and rapid growth. We have been awarded “ASO Tool of the Year” and “App Data Platform of the Year” by the App Growth Awards, and have been four times recognized as one of the fastest-growing technology companies by Deloitte Belgium.    Today we are a team of +100 people based in 8 offices around the globe (Brussels, San Francisco, Bengaluru, Tokyo, Seoul, London, Montreal and Beijing) supporting more than +2,000 customers worldwide. We’re gearing up for fast growth and are looking for ambitious individuals to join our team!      About the role      We are looking for a passionate and experienced Account Executive to join our second-stage rocket ship!  You’ll be responsible for helping AppTweak grow its customer base and revenue in EMEA, with a focus on Enterprise prospects. As an experienced AE, you will provide direction and perspective to the regional manager and leadership team to increase the business efficiencies, structure, and strategy to ensure team and individual success. If you have what it takes to help us grow, we’d love to hear from you!      Location: London or Paris. Access to co-working space.        What you will do:      Achieve the company’s sales goals for the EMEA market       Close deals consistently to achieve your individual sales target.    Build and grow your pipeline with accurate forecasting.    Conduct product demos to leads with a focus on value and business needs. You will own the full sales cycle from lead to close.    Prospecting ICP customers to generate opportunities, through inbound and outbound. Assess leads requirements, solve their problems and anticipate future needs to increase revenue.    Establish a deep understanding of AppTweak’s business operations, including App Store Optimization, competitive landscape, and internal tools &amp; processes.       Reinforce AppTweak’s presence and reputation in EMEA         Represent and advocate AppTweak’s brand during major mobile marketing conferences throughout the year in various locations such as Berlin, London, Barcelona, etc. (between 4 and 8 events per year).    Connect with C-level and senior executives in the mobile industry to grow AppTweak’s reputation across various verticals such as Gaming, Retail, Finance, Entertainment, etc.    Organize and host ASO-related networking events to increase brand awareness and reputation.      Actively participate in cross-department cooperation         Lead and contribute to team projects to develop and refine our sales processes.    Work with Marketing to ensure consistency in outreach/emailing campaigns and inbound initiatives.    Collaborate with various teams, including the Product and Customer Solutions Team, to better align client-facing efforts by taking the initiative to identify issues and find solutions.     Must-have       2+ years as an Account Executive selling B2B solutions    Perfectly Fluent in English, French or German is a plus!    Knowledge of the mobile marketing industry is mandatory    Consistent track record of (over) achieving targets    A problem-solving approach to the prospect's challenges    Entrepreneurial spirit: your pipeline is your business, you need to own it and embrace it    Bachelor's or Master’s degree in Business, Communication, Marketing, Sales or any relevant field       What's in it for you?         Onboarding journey in our amazing offices in Brussels, then invitation to join the Global meeting in person once every quarter.    Bi-yearly company-wide team building to connect with all your colleagues.    A diverse team within a flat hierarchy: altogether we speak more than 15 languages.    Opportunity to connect with a variety of exciting mobile businesses cross different verticals.    An exciting and fast-growing company with a people-first culture. “Diversity” and “work-life balance” are not just buzzwords at AppTweak.    Flexibility in your work and opportunities for continuous learning and creative thinking.    Regular general team meetings and demo days to make sure everyone is aligned with AppTweak's growth path    Chance to discover new food recipes, because yes, we love food!     ✨Our recruitment process✨         A first video call with Madeleine from the HR team to get to know each other and tell you more about AppTweak.    A video interview with the manager to deep dive into your past experience and learn more about your aspirations    The Assessment part, to test your skills related to the position    Final call with a C-level or the CEO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOVABLE VISION: ENABLE INNOVATION THROUGH STARTUP RELATIONS   Novable is a tech startup active in the corporate innovation space, providing a startup scouting solution made of advanced technology software and dedicated analyst reviews. In particular, Novable develops an advanced AI-based technology to scout and match startups.   Startups have the innovation power - We believe that startup ecosystems (entrepreneurs, startups, scaleups, hubs, accelerators, venture capital funds) are a glimpse of the future, as they crystallize the forefront of technology innovation everywhere in the world. They are the crystal ball to anticipate future industry trends.   Corporations have the industrial power - On the other side, we believe that corporations have the necessary resources to get things done and to put the best ideas at work on a global scale. In that sense, it is critical that they collaborate with startups, not only for themselves, not only for their survival but also for the greater good of humanity on this planet.   Bring the best of those two worlds together - We are technology optimists. We believe that tech innovation can contribute to solving major societal issues and world problems, provided that enough industrial power is injected into the process. We envision a world where innovation and industry powers connect seamlessly and globally, to speed up the world’s transformation.   Novable mission is to enable innovation through startup relations, by connecting the brightest minds from the startup ecosystem with the strong industrial ambitions of the business world. We allow corporations and companies to identify the most suitable, enterprise-ready innovations matching their strategic agenda.     Novable is a fast-growing tech startup working in the field of corporate venturing &amp; innovation scouting. We are now looking for a Growth Hacker Intern who is willing and ready to support the team in daily activities for at least 3 months.   Here are the main tasks that you will be involved with      Execute our growth hacking strategy: feed the sales team by building lists of leads through social engagement, SEO hacks, and HubSpot management    Engage in outbound activities: Design, set up, monitor and refine email and social media outbound campaigns    Use data &amp; analytics to support decision-making and growth strategies.    Creation of landing pages     Your Profile      Keen interest in digital selling, conversion, funnels, measures, with a data-driven mindset.    Knowledge of tools such as HubSpot, Lusha, Apollo, LinkedIn Sales Navigator, Google Analytics, etc. will be a strong plus.    Open-minded, eager to learn and try out new things, while also being autonomous.    Fun to work with! We take the sense of humour very seriously.    Fluent in English (C1), any other language is a plus     We'll only consider candidates located in Belgium who can regularly be in Brussels (2 days at the office is a must).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to build a high-quality data platform that will innovate financial markets? Do you want to work for a company that uses modern techniques to achieve the best results for its clients while empowering and supporting you to realize your full potential?    We are an experienced team of Spring committers, Kafka contributors, ex-Pivotal, and ex-Google engineers. If you want to know more, keep reading or reach out for a chat.    About us    We are a VC-backed fintech with a live product in the regulatory trade reporting space and a growing list of institutional clients (B2B). Our product journey has started in the US with a roadmap into Canada, UK, EU, Australia, and Singapore over the next twelve months. We are a start-up on a fast paced journey to scale-up.    KOR is built on leading edge cloud technology by industry domain experts and world class in-house engineering. We're on a mission to innovate B2B trade servicing starting with regulatory reporting in time for a global wave of mandated changes hitting all segments of market participants across OTC derivatives transactions. We’re solving the most challenging problems around by bringing fresh designs and solutions to data utility, quality, and processing inefficiencies. . . while unlocking insane value for clients.    Teamwork and laser focus are central to everything we do at KOR. With the right support, we believe small independent teams with deep expertises achieve better results and encourage skilled people to take responsibility and grow their careers. We live by the mantra of work humble, work smart, and work together.    About you    You have a passion for high-quality, reliable, and maintainable code. You're comfortable working with product managers, designers, and clients, making decisions to deliver valuable working software to clients and their users quickly. You're agile and retrospective and not afraid to identify what we're doing wrong so we can fix it and what we're doing right to improve on it. Above all, you judge your success by the success of your team and the happiness of our customers.    Responsibilities    As a Back End Engineer at KOR, you get to own parts of the KOR Platform. We value your ideas, and you'll play a key role in developing products that our customers will love using. Of course, we don't expect you to know it all, but your natural desire to learn will help you overcome new challenges and prove yourself as a valuable member of the KOR team.    Day to day, you'll be:&gt;      Designing and implementing the streaming data platform engine and SDK.    Implementing new features for our range of web and streaming applications and data reporting capabilities.    Be an active voice in the platform's build-out in regards to the technical choices and implementations.    Working closely with the broader team to embrace new challenges and adapt requirements as we continue to grow and adjust priorities.    Paired programming with a growing team of Back-end, Data, and Front-end Engineers.     Experience and attributes      A minimum of 5+ years of experience as a Back End Engineer.    Experience with Java and Spring Boot Framework.    Experience with building and running applications on public cloud vendors like AWS.    Experience profiling, debugging, and performance tuning complex distributed systems.    A firm reliance on unit testing and mocking frameworks with a TDD (Test Driven Development) mindset.    Knowledge of OOP principles and modern development practices.     Plus to have      Experience with event data modeling in event store/sourcing systems.    Experience with horizontally scalable and highly available system design and implementation, focusing on performance and resiliency.    Bachelor's Degree or higher in Engineering, Computer Science, or Information Technology.     The main tools and frameworks we use daily      K8s    AWS     OSX (Mac)    IntelliJ    Github (Actions)    DataDog    Confluent Cloud    Argo CD      We're still in the build stage, so introducing new tools and approaches are entirely on the table.    At KOR, the company culture is essential to us. Therefore, we are looking for an open-minded, humble, driven, communicative team player to join us.    What we have to offer    Depending on you and your priorities, we offer the following:       Culture of trust, empowerment, and constructive feedback.    Competitive salary, great IT equipment, and expense allowance.    Flexible working times.    Fully Remote    A span of control that matches your ambitions and skills.      Above and beyond this, we will provide a commitment to a genuine, balanced relationship. We will listen to you, take your needs and wishes seriously, and work to help you grow professionally.    So, if you're a Back-End Engineer who wants the chance to grow, maybe it's time to join a company that values what you do and helps you achieve your goals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business Developer Intern About Staizen At Staizen, we live and breathe transformation. We support and guide our clients through the toughest and nitty-gritty parts of building, modernizing, and running digital products and platforms. Transformation is not easy and to be the best partners, we challenge ourselves to constantly practice what we preach in the way we do, build and lead. The name Staizen is short for “State of Kaizen”, inspired by the Kaizen philosophy of continuous improvement. We are all about getting 1% better every day because sustainable transformation is not about the big bang but manifests in the daily choices that we commit to do every single day. What we offer   Get the chance to work on transformation at scale missions for complex industries such as banking, e-commerce, insurance  Be part of our internal product development and build the next generation of productivity tools for customers  Be part of exciting communities where you can collaborate, grow and learn across the board  We are remote-first with global operations across Belgium, Luxembourg, France, the Philippines, Singapore, and Cyprus, with optional co-working spaces for the team  The winning recipe Social Chameleon - Active Listener - Timely Delivery - Organizational Skills - Team Player - Solution and data Oriented Responsibilities Working in close collaboration with our Business community and you will have the opportunity to:   Identify account names per industry and build a priority list;  Identify leads (contact names, email address, LinkedIn contact);  Propose action plans;  Schedule prospection meetings;  Contribute to the CRM enrichment and data quality;  Support senior business manager in building customer offers;  participate to client meetings and project delivery sync-up;  Part of the business community and contribute to the business process improvement;  Requirements   A minimum internship duration of 6 months is required, and must be in business school.  On top of everything, you love to think, act smart and understand who you are addressing and why.  Strong ability to listen and accompany customers in the smooth deployment of new tools and teams.  Enthusiastic about using innovative technologies, collaborative tools and their possible applications.  Charismatic communicator, willing to be the driving force in sustainable collaborations.  High-level command of English and Dutch is required as you will collaborate closely with Dutch clients within a diverse team.  Dynamic individual with an interest in IT/Digital Transformation.  Previous internship experience in the IT/Digital industry is advantageous.  Benefit   Attractive internship compensation  Be part of a dynamic and senior Business community  Learn digital and IT industry market  Create a long-term lead portfolio  Potential long-term employment after the internship.  So, what do you think? Are you ready to drive impact and grow with us? We’re looking for forward thinkers who thrive in an international environment. We have openings across our various communities - Frontend, Backend, DevOps, UX/UI, Quality Assurance, Data &amp; Analytics, and Engineering Management. We can’t wait to meet you, drop us a message, and let’s chat! Job Type: InternshipContract length: 6 months Pay: Up to €500,00 per month Benefits:   Work from home  Schedule:   Day shift  Supplemental Pay:   Commission pay  Language:   English (Required)  Dutch (Required)  French (Preferred)  Work Location: Hybrid remote in 1050 Brussels</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Job Title: Business Development &amp; Sales Manager          Location: Belgium          Job Type: Full-time                   Looking for an opportunity to channel your inner Business Development ninja?          Look no further. We are seeking a Business Development Manager who is passionate about the latest high-tech innovations in world leading companies, who can drive new business opportunities and manage the sales funnel end to end. Join our team and help shape the future of Caeleste, and beyond.                   Who We Are          Caeleste is a dynamic team of engineers, scientists and enthusiasts who develop exceptional CMOS image sensor solutions. Our collaborations with top global companies in the space, scientific, medical, industrial and life science industries result in extraordinary and innovative solutions that give them a competitive edge in their respective fields. Our expertise in designing and delivering high-speed, ultra-low noise, ultra-high dynamic range and extreme radiation-hard sensors make us a one-stop solution provider for our customers.          Join our team at Caeleste and experience the direct impact of your ideas and actions, regardless of your role or seniority. Our team is not only proud of their achievements, but also knows how to have fun.          Excitement awaits!                   What We Look For          As a Business Development Manager at Caeleste, you are responsible for generating new business by connecting with potential customers and translating their high-tech needs into successful projects. This includes identifying new leads, creating the business case, and driving qualified leads into signed proposals in collaboration with the engineering team. You will also be responsible for defining the go-to-market strategy and driving marketing activities. You will contribute to Caeleste's imaging offering in close collaboration with the engineering teams by mapping research and solution roadmaps to market needs. You will formulate business recommendations for the management team and report directly to the Business Development &amp; Sales Office Leader.                   You Are The Perfect Candidate If You                    have a technical Bachelor or Master's degree, combined with a strong business acumen,           share a customer-centric focus with the ability to identify and meet customer needs,           bring a track record of success in driving sales and business development in a high-tech B2B sector or have similar experience through managing customer facing projects,           show excellent interpersonal and communication skills to build and expand your professional network and confidently represent the company at conferences and trade shows,           demonstrate proficiency in effectively persuading peers on technical, legal and business-related matters,           enjoy traveling globally, to wherever business opportunities arise (between 10-30%),           are fluent in English.                            We'll be blown away if you also have:                    an understanding in the areas of CMOS technology, digital and analog design, test electronics, electro-optical instrumentation, photonics, etc.,           experience in the imaging technology market,           a good understanding of public funding mechanisms (local and European),           have a relevant network in the image sensor industry and/or in any of our target markets (industry, medical, space, life-science)           have experience with Business with Space Industry, e.g. with ESA or New Space.                            We Offer:                    a mandate to have a long-term impact in the successfully growing semiconductor company           competitive compensation and benefits package           a bonus in line with Caeleste's performance,           the opportunity to work on cutting-edge technology projects with world-leading companies,           a technological playground with a mixed-skilled, multi-cultural team of experts,           a flexible and dynamic work environment,           a continuous focus on learning at Caeleste University                            For application and questions, please contact us at </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">jobs@caeleste.be</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">About Oxygen         The insurance industry is gasping for breath. The work environment is becoming increasingly digital, legislation is changing, clients expect more and the call for efficiency is getting more prominent. Our passionate team of experts offers an answer. Bringing oxygen and building the insurance industry of tomorrow : that’s what we’re all about!         We make impact by approaching industry challenges from different angles. We fill in project roles, support in day-to-day administration, provide total solutions and offer an answer to complex challenges by offering end-to-end automations.         At Oxygen, it’s all about people. We believe that passionate people with ambition can make the difference. Growth through the growth of people, that’s how it works.         What will you be doing?         As a business analyst you represent Oxygen at our clients. Together with the team you work on various projects, always with the aim of making the insurance sector more efficient and more customer-oriented.         You review existing processes and structures with a critical eye. You detect bottle necks and think about how these can be eliminated. Besides analyzing you also support in implementing new processes or optimizing existing procedures. To do so you form the bridge between business and IT and involve the different stakeholders throughout the process. In addition, you help facilitate changes in the organization and make sure that everyone embraces the transformation.         What can you expect?                  Building the insurance industry of tomorrow : challenging projects with impact          Growth through the growth of people : extensive training and development opportunities, training budget, personal coaching sessions, space to shape your own growth path,…          Join a scale-up in full development and with a strong personal approach          Broaden your horizons and choose a career full of variety : working for different insurers and brokers with a good reputation          Interesting remuneration package: competitive salary supplemented with company car, hospitalization insurance, pension plan, meal vouchers, bonus plan, expense allowances, …                          Who are you?                  A must: You recognize yourself in the Oxygen core values : Collaborative – Positive – Hands-on – Open-minded – Deliver          You have a first experience in a project role in the insurance industry (business analyst, project manager,…)          Analytical mind combined with strong communication skills          Someone who is flexible and can adapt quickly to new environments          Languages. You have good knowledge of Dutch and French                                                  Does this job appeal to you? Then don’t hesitate to apply and send an e-mail with your motivation and your CV to dieter.kennes@oxygen.be.                                                                             APPLY NOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you know Club Med?   We have nearly 70 Resorts, open year-round in 26 countries. We offer luxury vacations in both mountain and seaside settings. Our clients seek happiness and freedom.   Why are you reading this job posting? Because you want to become a part of that extra something that sets us apart. You possess sought-after human and professional skills. We offer you the opportunity to develop and grow rapidly by joining our brilliant teams. You'll be able to travel the world.      Your Workspace   Welcome to the Alps, where our Exclusive Collection Chalets offer a unique working environment that blends luxury and practicality. Each chalet, with its elegant spaces and warm atmosphere, creates an unforgettable experience for our clients. Like our Chalet-apartments, these exclusive areas strengthen our relationships with our clients. Every detail is carefully thought out, from personalized welcomes to spaces designed by renowned designers, to enrich your daily life.   Your role is essential in providing memorable experiences, whether it's family moments or exclusive Club Med activities. Meanwhile, our kids' clubs take care of the little ones. Our working environment goes beyond conventional standards by combining luxury, well-being, and a unique experience. Additionally, we provide quality professional equipment for optimal working comfort. Our pioneering spirit encourages us to adopt innovations that enhance our teams' working comfort and allow them to focus on the essentials: the relationship with our clients.      You Are        Curious: You can share interests based on what others like. You are open to new ideas and have good general knowledge.   Attentive: You ask questions and listen carefully. You adjust your energy according to the situation, react sensitively, and show empathy.   Elegant: You communicate well and handle conversations with grace. You are authentic in both your communication and demeanor.   Charismatic: You have a natural and sincere presence. You inspire others by being yourself and remaining simple.   Proactive: You anticipate needs, overcome obstacles, and find solutions proactively. Autonomous: You work independently, make sound decisions without constant supervision, thus enhancing your efficiency and self-confidence.   Unifying: You effectively connect departments, mobilizing teams toward common goals, positioning yourself as a powerful driver for task accomplishment.     You Will        Ensure a worry-free stay in the Chalet and the resort by being the preferred point of contact for the client.   Carefully prepare the client's stay by highlighting included and à la carte services, as well as resort activities.   Facilitate the client's stay by coordinating the various services involved, ensuring the follow-up of all specific client requests, whether related to the Chalet or the Resort.   Ensure the quality of services offered to the client by verifying their compliance with established quality standards for Chalets.     By joining Club Med Exclusive Collection, you will experience a new kind of luxury. One that combines refinement, attention to detail, consideration for each of our clients with the kindness, simplicity, authenticity of relationships, and the legendary conviviality of Club Med. Luxury centered, above all, on humanity and experiences.      Club Med Exclusive Collection includes: 100% Club Med Exclusive Collection Resorts, Club Med Exclusive Collection Spaces in our 4 Trident Resorts, Villas, Chalets, and our legendary 5-masted sailboat.      All our positions are open to individuals with disabilities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">About Accenture     We are a leading partner to the world's major cloud providers, including AWS, Azure, and Google. The formation of Accenture Cloud First, with a $3 billion investment over three years, demonstrates our commitment to deliver greater value to our clients when they need it most. Our Cloud First multi-service group of more than 70,000 cloud professionals delivers a full stack of integrated cloud capabilities across data, edge, integrated infrastructure and applications, deep ecosystem skills, the culture of change along with deep industry expertise to shape, move, build and operate our Client's businesses in the cloud. To accelerate our customer's transformation by leveraging the cloud, we combine world-class learning and talent development expertise; deep experience in cloud change management; and cloud-ready operating models with a commitment to the responsible business by design — with security, data privacy, responsible use of artificial intelligence, sustainability and ethics and compliance built into the fundamental changes Accenture helps companies achieve.     Last year, Accenture acquired Sentia's businesses in the Netherlands, Belgium and Bulgaria to strengthen local infrastructure engineering and public cloud-managed services with 310 cloud specialists. The Sentia group is a leading cloud consulting company that manages private and public cloud migrations and provides digital experience monitoring services.     The Cloud Infrastructure Sales Specialist (Senior Manager) is focused on growing Accenture Cloud First Business in the public and private cloud domain and manages opportunities through all phases, including qualification, sales pursuit and close by applying deep sales process and offering expertise. Develop relationships &amp; engage in content-driven conversation with essential buyers and decision-makers at new and existing clients to solve their problems.     #LI-EU       Your profile      Minimum 5 years selling &amp; closing enterprise deals in the professional services space in one or more of the following areas: Infrastructure Outsourcing, Cloud enablement migration and modernization, Private or Public Cloud managed services    Minimum of 10 years of Sales Pursuit Management experience    Minimum of 5 years experience in direct sales with a quota of $10M+    Experience with C-Level client relationship building and relationship management    Strong understanding of cloud computing technologies and services, as well as the ability to explain complex technical concepts in a clear and straightforward manner to customers    Cloud certification in Azure, AWS or Google    A Degree in Computer Science, Engineering or Technical Science.       Bonus points if you have      Previous experience in conceptualizing, planning, and implementing cloud migration, modernization, cloud-native development, or cloud-managed services.    Industry experience in Banking, Insurance, Utilities, Telecom or Manufacturing.    Proven ability to operate within a team-oriented environment.    High energy level, decisiveness, and ability to work well in demanding environments.    Excellent communication (written and oral) and interpersonal skills.    Strong leadership, problem-solving, and decision-making abilities.       Our offer   At Accenture, we are committed to creating an inclusive and supportive workplace that values diversity and promotes growth for all. As you join our global company with a world-class brand and reputation, we want to assure you that you will be part of a vibrant, diverse workplace culture. We firmly believe in openness and honesty, fairness and equality, and we celebrate the unique contributions of every individual. We are dedicated to getting to know the real you and supporting your personal and professional growth, so you can excel in whatever you're great at. At Accenture, learning is a continuous journey, and we provide numerous learning opportunities, both formal and informal, to enhance your role-specific skills and expertise.   Beyond the impactful work we do for our clients and the nurturing work environment we provide, we offer a range of excellent employee benefits designed to cater to your diverse needs and well-being. These benefits include:      13th month + holiday allowance: Ensuring financial stability and recognition for your hard work.    20 + 12 holidays: Providing ample time to recharge and spend quality moments with loved ones.    Laptop and smartphone: Equipping you with the necessary tools to excel in your role, regardless of location.    Hospitalization insurance and extensive group insurance package: Prioritizing your health and well-being, so you can focus on what matters most.    Bonus program: Recognizing and rewarding your exceptional contributions to the team's success.    Training &amp; learning opportunities: Encouraging continuous growth and skill development to reach your full potential.    Green mobility program: Supporting environmentally-friendly commuting options like e-bikes, public transport, bike 2 work allowance, and more.    Flexrewards: Empowering you to customize your rewards package with our flexible benefits tool to suit your individual needs.    Discount program: Offering discounts at your favorite (online) shops, so you can enjoy life outside of work.    Employee shares purchase plan: Providing an opportunity to become a stakeholder in the company's success.    Eco-cheques: Promoting sustainable living and environmentally-conscious choices.    And many more!       At Accenture, we understand that a diverse and inclusive workplace fosters innovation, creativity, and a sense of belonging. We are committed to building a workforce that reflects the richness of the communities we serve. By offering these inclusive benefits, we aim to attract and retain talent from diverse backgrounds and create an environment where everyone can thrive and succeed together. Your unique experiences, perspectives, and talents are what make Accenture a great place to work, and we look forward to having you join our team and contribute to our shared success.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job ID: 239756   Date posted: 22/07/2024 Who you are      '- You have an interest in interior design and the daily life of people's homes.         You already have several years of professional leadership experience and love working with people.    You have already proven to be a real problem solver and able to make decisions in a rapidly changing retail environment.    You are business-minded, results-oriented and focused on the customer.    You involve your colleagues and create commitment for your plans.    You continuously challenge your colleagues and yourself to exceed our customers' expectations and optimize the way we work.    You are energized by the IKEA values and they are a reflection of your own values.    You speak and write (one of) the store's regional languages and English.    You will gladly come to work on Saturdays in exchange for a day off during the week.      Your responsibilities      You will drive the commercial calendar both online and throughout the store to create vitality, encourage customers to visit us more often and to buy more. You will do all this in close collaboration with your colleagues and the local marketing manager.            You translate the store's business plan into a clear action plan for your department and implement the various actions. In this way you contribute to the positioning of the IKEA store as the leader for interior design in the local market.    You inspire, motivate and engage your team to achieve the goals and thus create long-term growth and profitability.    You motivate your fellow managers to take responsibility in achieving store vitality goals.    You react quickly to commercial opportunities, changes in stock availability and customer feedback.    You will focus on opportunities to drive impulse buying    You analyze the results delivered: identify successful activities, solutions and ideas and use this information in planning future actions.      Our team within IKEA      We are the ones meeting our customers – in our stores, online, in our catalogue and beyond. We have knowledge of the IKEA product range, local markets and customer needs and we constantly find new ways of making real connections with our customers to maximize sales and profitability. Together with thousands of colleagues around the world we’re a diverse team working for the continued global success of the IKEA Concept – a concept that helps millions of customers create a better everyday life!      Apply now!      At IKEA, we like to give you the space to take control of your own development and growth. We believe in entrepreneurship and initiative and want to make it easy for you. In the first few weeks/months, you will be offered a 5-step development plan to get you started, with enough personal space to create the learning moments you need.    We offer this structure and a supportive network of colleagues who will make sure you feel comfortable in this situation and give you time to learn, make mistakes and develop.       In addition to a competitive remuneration, we offer:            Eco-vouchers    End-of-year bonus, holiday pay and sector premiums    A commuting allowance with an additional allowance if you come by bike    Private leasing of an electric bike, we are happy to give you a boost    Comprehensive hospitalization insurance    A private accidents insurance    Pension savings    A leave savings plan: choose how you want your late/early hours (before 7h and as of 19h) to be paid out: a supplement on your salary or in holiday hours    We also offer extralegal holidays, seniority holidays and for full-time colleagues 6 extra days off    A canteen where you can eat delicious food at very democratic prices    IKEA Tack! Loyalty reward, an additional deposit into your retirement savings based on our global results and your loyalty to IKEA    ONE IKEA Bonus: an additional bonus based on your shop's results    IKEA Benefits at work: a portal offer you great discount for well-known stores and brands    IKEA staff discount 15% on all your purchases    Team outings &amp; staff parties, because togetherness is very important to us    A nice extra in case of legal cohabitation/marriage/birth/retirements to celebrate these beautiful moments    We offer you a schedule 6 weeks in advance to better plan your work-life. Our shops close at 8pm (Friday 9pm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company Description   Our Mission   At Palo Alto Networks® everything starts and ends with our mission:   Being the cybersecurity partner of choice, protecting our digital way of life.   Our vision is a world where each day is safer and more secure than the one before. We are a company built on the foundation of challenging and disrupting the way things are done, and we’re looking for innovators who are as committed to shaping the future of cybersecurity as we are.   Our Approach to Work   We lead with flexibility and choice in all of our people programs. We have disrupted the traditional view that all employees have the same needs and wants. We offer personalization and offer our employees the opportunity to choose what works best for them as often as possible - from your wellbeing support to your growth and development, and beyond! Job Description   Your Career   Our Commercial Sales Team is an important driver of company revenue and growth. As an experienced and dynamic sales professional, you will be responsible for leading and driving sales engagements into assigned commercial accounts. In this role, you are motivated by the desire to solve critical challenges facing our customer’s secure environment, so you’re prepared to connect them with a solution for every stage of threat prevention.   You will be responsible for meeting and exceeding your quota by crafting and implementing strategic and tactical sales plans targeting deployments of the Palo Alto Networks Next-Generation Security Platform. This is a unique opportunity for a closer with a self-starter mentality to win business and market share by actively displacing competing technologies and further improving the security posture of existing customers. Oh, and did you say you love to sell? Because selling is what gets you out of bed every morning. This is not just a career – it’s a meaningful challenge that impacts our lives in the digital age.   Your Impact      Prospect and sell into assigned commercial accounts, create and execute a robust sales strategy to penetrate into new accounts and expand into existing accounts    Be the primary sales driver, managing a sales pipeline to deliver to quarterly/annual quota    Strong discipline around managing sales stages and SFDC hygiene    Deliver accurate weekly and quarterly forecast    Stay updated on industry news and trends, and how they affect Palo Alto Networks products and services    Communicate value propositions to clients and partners that speak intimately to their needs and requirements    Generate velocity to deliver a predictable book of business and drive forecast accuracy utilizing channel ecosystem    Develop and deploy marketing activities and plans to end users through our channel sales partners    Engage a programmatic approach to demand, to generate, develop, and expand your territory    Work collaboratively with all cross-functional resources to achieve your quota - inside sales, channel systems engineering, field marketing, cybersecurity sales specialists, the services team, sales ops (including deal desk and the response team), and others      Qualifications   Your Experience      Proven track record of success in achieving sales quotas    Experience working with channel partners and understanding of a channel-centric go-to-market strategy    Have and able to lead all aspects of the sales cycle with the ability to uncover, qualify, develop, and close new, white-space territories and accounts    Technical aptitude for understanding how technology products and solutions solve business problems    Excellent time management skills, and work with high levels of autonomy and self-direction    Proficiency in French and/or Dutch language skills      Additional Information   The Team   Our sales team members work hand-in-hand with large organizations around the world to keep their digital environments protected. We educate, inspire, and empower our potential clients in their journey to security.   As part of our sales team, you are empowered with unmatched systems and tools, constantly updated research and sales libraries, and a team built on joint success. You won’t find someone at Palo Alto Networks that isn’t committed to your success – with everyone pitching in to assist when it comes to solutions selling, learning, and development. As a member of our sales team, you are motivated by a solutions-focused sales environment and find fulfillment in working with clients to resolve incredibly complex cyberthreats.   Our Commitment  We’re trailblazers that dream big, take risks, and challenge cybersecurity’s status quo. It’s simple: we can’t accomplish our mission without diverse teams innovating, together.  We are committed to providing reasonable accommodations for all qualified individuals with a disability. If you require assistance or accommodation due to a disability or special need, please contact us at accommodations@paloaltonetworks.com.  Palo Alto Networks is an equal opportunity employer. We celebrate diversity in our workplace, and all qualified applicants will receive consideration for employment without regard to age, ancestry, color, family or medical care leave, gender identity or expression, genetic information, marital status, medical condition, national origin, physical or mental disability, political affiliation, protected veteran status, race, religion, sex (including pregnancy), sexual orientation, or other legally protected characteristics.   All your information will be kept confidential according to EEO guidelines.     Please note that we will not sponsor applicants for work visas for this position.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">About Wintercircus:Wintercircus is a dynamic tech hub and innovation ecosystem located in the iconic building in Ghent. Home to over 300 residents, including early-stage tech startups, Wintercircus offers a vibrant space where work, collaboration, and creativity thrive. With its startup campus, cool bars, cozy eating spaces, and art experiences, Wintercircus is a place to connect, unwind, and recharge. Job description:We are seeking a talented and creative designer to join our team. As a Designer, you will create visually compelling designs that convey our brand's vision and values to different audiences. Your responsibilities include developing graphics for digital, print media, and on-site assets. You'll collaborate with various teams to ensure our visual communications are consistent and engaging. Key responsibilities: Visual design:   Create visually appealing graphics for digital platforms, including websites, social media, and email campaigns.  Design print materials such as brochures, flyers, posters, and event collateral.  Brand identity:   Ensure consistency in Wintercircus' visual identity across all design projects.  Develop and maintain brand guidelines to support a cohesive look and feel.  Collaborative projects:   Work closely with the marketing, events, and startup teams to understand project requirements and deliver high-quality designs.  Participate in brainstorming sessions to generate creative ideas and concepts.  UI design:   Assist our dev team in creating intuitive and user-friendly interfaces for web and mobile applications.  Conduct user research and gather feedback to improve design solutions.  New media and installations:   Create custom illustrations and multimedia content to enhance visual storytelling.  Assist the team in producing &amp; editing videos, animations, and interactive content as needed.  Community engagement:   Create engaging designs to support the social media team in promoting Wintercircus activities.  Develop visual content for music, art, and technology events to enhance community interaction.  Qualifications and skills:   Proven experience as an interactive designer, preferably in a similar setting.  Strong portfolio showcasing a variety of design projects and styles.  Proficiency in design software such as Adobe Creative Suite (Illustrator, Photoshop, InDesign, etc.), Figma, and Canva.  Excellent understanding of typography, color theory, and layout design.  Strong communication and interpersonal skills, with the ability to collaborate effectively with diverse teams.  Creative thinker with a keen eye for detail and a problem-solving mindset.  Ability to manage multiple projects simultaneously and meet deadlines.  Knowledge of print production processes and requirements.  3D design, editing, and film capabilities are nice to have.  An interest in music, art, AI, technology, and urban culture is a big plus.  Why join Wintercircus?Wintercircus provides a unique opportunity to work in an iconic building filled with rich history that triggers inspiration. Backed by top entrepreneurs and renowned knowledge institutions, Wintercircus offers you an exciting network, personal development, and lots of fun. It’s a spot where your creative talents and ambitions are encouraged and nurtured. Join us in our mission to create a vibrant, interdisciplinary community for changemakers. To apply, please submit your resume and a portfolio of your work, and send us a short message detailing how you can contribute to our creative team. Dienstverband: Voltijds Werklocatie: Fysiek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">About us    The Interchain Foundation stewards a vast ecosystem of decentralized technologies. We develop and maintain foundational protocols, and fund organizations to create an internet of shared resources, security, and value creation. Through our grants, investments, and ecosystem stewardship, we are shaping a new technological paradigm that is open-source, interoperable, and community-owned.    About the role    As Managing Director of the Interchain Foundation, you will step into the heart of a vibrant and innovative environment, using your influence and vision to guide the strategic direction and culture of our cutting-edge open-source ecosystem.  The Interchain Foundation is a dynamic organization, leveraging a distributed development environment to deliver state-of-the-art open-source software for building blockchains while fostering a thriving community of builders.  Our core mission is to support the development and adoption of the Interchain Stack. You will lead a Board of Management composed (today) of a Chief Product Officer and Chief Marketing Officer, and report to a Board of Directors. You will oversee the operations of the ICF and its subsidiaries, Interchain AG and Interchain GmbH, which together consist of 25 employees across key functions such as Finance, Marketing, Product, Developer Relations, and Operations.  In addition to our internal teams, you will collaborate closely with external development teams responsible for maintaining different components of the Interchain Stack. These teams, which we refer to as stewards, manage specific parts of the software stack such as IBC, CometBFT, the SDK, and CosmWasm, while also operating their own businesses within the crypto space.  The Interchain Foundation has an annual operating budget of approximately $40 million and a total treasury of roughly $300 million. This is an exciting opportunity for a visionary leader who thrives in innovative environments and is eager to take on the challenge of steering an impactful organization at the cutting edge. We are looking for someone with a proven ability to navigate complexity, forge strategies from diverse viewpoints and inputs, and make a significant long-term impact.  This person excels at recognizing opportunities that others may miss and securing buy-in from a wide range of stakeholders. They are committed to maximizing value for the organization and the ecosystem, knowing when to empower others and when to take the lead themselves. They understand that their legacy will be defined by creating sustainable and resilient structures.  This transformative leader will enhance good teams by recognizing and building on their strengths. Ultimately, this person is comfortable being the face of the organization, leading by example and embodying the values that will shape our culture.     Your responsibilities will be:       With guidance and support of the Foundation Council, set the strategic direction for the Interchain Foundation, ensuring alignment with the broader goals of the ecosystem.    Lead and manage the Interchain Foundation, executing on the strategy you set above, fostering a culture of collaboration, innovation, and impact.    Work within the interchain beyond the Interchain Foundation, interfacing and collaborating with diverse, distributed participants in the ecosystem and beyond.    Cultivate and expand the interchain community, attracting developers, builders, and users.    Drive the growth and adoption of the interchain.    Build strong narrative and strategic alignment through public appearances — with a consistent focus on the strategy you’ve set     Ideal but not prerequisite qualifications:       Deep experience in complex environments (dynamism of open source, and coordinating across diverse &amp; distributed stakeholders).    Comfortable with soft influence (not a BDFL type).    Proven experience fostering strategic alignment with a board.      Who you are:       Proven experience in leadership roles at an organization that successfully delivered a product to market, preferably within open-source software, or a similar environment managing multiple engineering projects in parallel with varied, complex dependencies.    Interest (and understanding) of the crypto industry at large.    Embody the values of free and open source software.    Able to see the big picture and deftly understand the interplay of a complex ecosystem.    Strong interpersonal and communication skills, committed to collaboration and community engagement.    Capable of articulating a compelling long-term vision and inspiring others to rally around it.    Capable of making tough decisions, and knowing when and how to decide; capable of disagreeing but committing when compromise is necessary.    Puts the mission and the team first, and oneself second.    Located in or able to relocate to Switzerland.     Is a plus:      Already domiciled in Switzerland, or admission to an EU country via residency.      Not sure if you're a fit? Please feel free to apply anyways, and we'll take it from there.  Interchain believes that great people come from a broad range of backgrounds, and that the diversity of our team is one of our strengths. Discriminatory behavior has no place at Interchain—we do not discriminate on the basis of race, colour, gender, gender identity, national origin, age, religion, disability, or sexual orientation. We are committed to fighting bias in our workplace and our communities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kapsch TrafficCom develops smart solutions to make mobility safer, more sustainable and efficient for everybody. We design, build and operate traffic management systems including connected vehicles technology and mobility demand management as well as tolling services for cities, roads, tunnels and bridges around the world. We develop data and video analytics platforms, building on state-of-the-art technologies including AI, machine learning, big data and cloud services to enable the digitalization of mobility.                    Your Responsibilities              You translate complex requirements into functional, secure, reliable, serviceable and cost-effective architectures and designs.        Design a System Architecture for data centers (DC), LAN and WAN for specific projects be it on premises or in the cloud        Support international bids with the elaboration of operational concepts and cost calculation        Interact with our system integrators for ascertaining that your system architecture intention is fully understood, check and release their low level designs        You work closely with supply chain to get optimized commercial offers from vendors, integrators and operational partners        Control the project implementation costs for DC &amp; WAN and interact with our other solution specialists to build a large and complex system        Support the operations teams of production systems with your knowledge of the systems architecture        You build and lead a community of practice by driving active knowledge and best-practice sharing             Your profile              You bring a high sense of commercial awareness, balancing between technological rich and commercially feasible architectures and designs        You know your way around all architecture patterns, be these RPO=0 systems or lambda architectures or cloud implementation (SaaS and PaaS) of current software stacks        You have a profound knowledge of current IT technologies, be this virtualization, heterogenous database landscapes, microservice architectures or SaaS strategies or what else is currently in vogue        You know the existing vendor landscape well and keep monitoring their current and future offerings and products        You have a passion for mentoring and sharing your knowledge and passion with others        You have the ability to talk to C-level and engineers alike.        A structured and independent way of working with excellent communication skills        Willingness to travel (up to 25%) and work in international teams        Fluent in English verbally and writing             Our offer:              You you will be part of an exciting endeavor in an international company with European roots        We have a unique corporate culture, driven by family tradition since 1892. We strive to create a work environment conducive to personal growth, satisfaction and achievement.        A hands-on onboarding with an experienced team to get familiar with the business and domain-related processes        Possibility to participate in regular trainings (technical and personal development)        Space for creating innovative solutions and ideas within a professional team practicing Agile methodologies        Social benefits of a modern company, e.g. Homeoffice, mobile devices, flexible working hours, operating restaurants, meal discount, bridge day regulation etc.        Working in our Global Services ambitioned team, brave to try out new technologies        A market-compatible gross salary of € 70.000 p.a. – which can be adapted according to your qualification and relevant experience             Kapsch is proud to be an equal opportunity employer. We attach great importance to a balance in the diversity of our employees. Therefore we welcome all applications without regard to gender, age, religious beliefs/ideology, sexual orientation, ethnicity or national origin.       Your contact person for this position: Tatiana Rezan-Sirotinskis. T: +43 50 811 1906</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terma is a leading provider of mission-critical solutions for the defense and aerospace industry, dedicated to delivering security for nations, allies, and individuals. We operate across various sectors, with security being a central focus. Our advanced technologies are designed to ensure the safety of people during both peaceful and conflict situations. Our systems offer security on land, at sea, and in the air. Terma places a strong emphasis on diversity, fostering an environment that brings together individuals with different cultural and professional backgrounds who are passionate about what they do. Your new Role Join our dynamic team responsible for the Manufacturing, Assembly, Integration, and Test (MAIT) of satellite test equipment. As a Warehouse Operations Specialist, you will play a pivotal role in logistical support and front office reception. Key Responsibilities:   Manage warehouse operations including booking in and out, replenishment, and reorders.  Conduct incoming inspections, verifying ordered components and document scanning.  Handle shipping of packages and containers, including parts list creation and coordinating delivery notes and transport.  Provide reception support, welcoming guests, managing check-ins and check-outs, and maintaining access control.  Requirements:   Apprenticeship qualification in work areas like logistics, warehouse management, office administration, or related fields.  Proficiency in any warehouse management systems is beneficial;  experience in parcel delivery is advantageous.  Excellent problem-solving skills and adaptability to new challenges.    Fluent in both German and English, with good verbal and written communication skills.  Strong team player with excellent communication skills.What We Offer:    A collaborative and innovative work environment that encourages creativity and personal growth.  Opportunities for professional development and continuous learning.  Competitive salary and comprehensive benefits package.  Why Terma? We are an international company representing world class expertise, delivering complex and high-tech products. We value our colleagues and our meaningful contributions to securing people through advanced technology. During your onboarding in Terma you can expect a thorough introduction and training in our systems and processes, as well as a strong focus on teaching you useful new competences and further strengthening current ones, both professionally and personally. Our company culture is autonomous and engaging, and we acknowledge the importance of flexibility in a great working environment. On our different locations, we offer various social activities to bring all our colleagues together. For further information, please contact Mrs. Raluca Moise by telephone [+49 6151 860050] or by email [ta.space@terma.com]. We look forward receiving your application and CV. To ensure that your application reaches us and is properly processed, please upload your application and CV via our recruitment system. Please use the Apply-button below. Based on full employment we offer you a yearly gross salary of 37.000 Euro (collectively agreed minimum salary - overpayment possible) depending on your qualification and experience. The high-tech and innovative Terma Group develops products and systems for defense, non-defense and security applications, including command and control systems, radar systems, self-protection systems for aircraft and vessels, space technology, and aerostructures for the aircraft industry. Terma is headquartered at Aarhus, Denmark. Internationally, Terma has subsidiaries and operations in The Netherlands, Germany, France, United Kingdom, Austria, Czech Republic, Romania United Arab Emirates, India, Singapore, and the U.S. The Space Business Area contributes with mission-customized software and hardware products including power systems and star trackers as well as services to support several in-orbit pioneering European scientific and Earth observation satellite missions. Additionally, Terma is contracted for the development and delivery of software and hardware systems and services for numerous ongoing and future European, and international missions. Terma Space operates out of Denmark, The Netherlands, Germany, France, the UK, Austria, Czech Republic, and Romania. Lager Logistiker (M/W/D), Österreich, Wien Terma ist spezialisiert auf die Bereitstellung missionskritischer Lösungen für die Verteidigungs- und Luft- und Raumfahrtindustrie. Unser Hauptziel ist es, Sicherheit für Länder, Verbündete und Einzelpersonen zu gewährleisten. Wir sind branchenübergreifend tätig, wobei Sicherheit im Mittelpunkt steht. Unsere fortschrittlichen Technologien sind darauf ausgelegt, die Sicherheit der Menschen sowohl in friedlichen als auch in Konfliktsituationen zu gewährleisten. Unsere Systeme bieten Sicherheit an Land, auf See und in der Luft. Terma legt großen Wert auf Vielfalt und fördert ein Umfeld, das Menschen mit unterschiedlichem kulturellen und beruflichen Hintergrund zusammenbringt, die mit Leidenschaft bei der Sache sind. Ihre neue Rolle Sie sind hauptsächlich für logistische Belange und die Unterstützung in unserem Frontoffice/Rezeption zuständig. Sie werden Teil des hochdynamischen Teams, das für MAIT (Herstellung, Montage, Integration und Test) von Satellitentestgeräten verantwortlich ist. Hauptverantwortlichkeiten:   Verwaltung des Lagers (Ein- und Ausbuchungen, Auffüllen des Lagers sowie eventuelle Nachbestellungen etc.)  Eingangskontrolle (Prüfung bestellter Bauteile, Scannen von Dokumenten)  Versand von Paketen und Containern (Erstellen von Stücklisten, Anfordern von Lieferscheinen und Transport)  Rezeptionsunterstützung (Begrüßung, Check-in und Check-out der Gäste, Zugangskontrolle usw.)  Anforderungen:   Lehrabschluss in einem der Bereiche Logistik, Lager, Büro, Verwaltung o. ä.  Kenntnisse in der Lagerverwaltung wären von Vorteil.  Hervorragende Fähigkeiten zur Problemlösung, flexible Herangehensweise an unerwartete Situationen und Herausforderungen.  Fließende Deutsch- und Englischkenntnisse in Wort und Schrift  Starke Kommunikationsfähigkeiten und die Fähigkeit, in einer teamorientierten Umgebung zusammenzuarbeiten  Was wir anbieten:   Ein kollaboratives und innovatives Arbeitsumfeld, das Kreativität und persönliches Wachstum fördert.  Möglichkeiten zur beruflichen Weiterentwicklung und zum kontinuierlichen Lernen.  Wettbewerbsfähiges Gehalt und umfassendes Leistungspaket.  Warum Terma? Wir sind ein internationales Unternehmen, das erstklassiges Fachwissen vertritt und komplexe und hochtechnologische Produkte liefert. Wir schätzen unsere Kollegen und unseren sinnvollen Beitrag zur Sicherheit von Menschen durch fortschrittliche Technologie. Während Ihres Onboardings bei Terma erwartet Sie eine gründliche Einführung und Schulung in unsere Systeme und Prozesse sowie ein starker Fokus darauf, Ihnen nützliche neue Kompetenzen zu vermitteln und bestehende Kompetenzen weiter zu stärken, sowohl beruflich als auch persönlich. Unsere Unternehmenskultur ist autonom und engagiert und wir wissen, wie wichtig Flexibilität in einem großartigen Arbeitsumfeld ist. An unseren verschiedenen Standorten bieten wir verschiedene soziale Aktivitäten an, um alle unsere Kollegen zusammenzubringen. Für weitere Informationen kontaktieren Sie bitte Frau Raluca Moise telefonisch [+49 6151 860050] oder per E-Mail [ta.space@terma.com]. Wir freuen uns auf Ihre Bewerbung und Ihren Lebenslauf. Um sicherzustellen, dass Ihre Bewerbung uns erreicht und ordnungsgemäß bearbeitet wird, laden Sie bitte Ihre Bewerbung und Ihren Lebenslauf über unser Rekrutierungssystem hoch. Bitte nutzen Sie den unten stehenden „Bewerben“-Button. Bei Vollbeschäftigung bieten wir Ihnen abhängig von Ihrer Qualifikation und Erfahrung ein Jahresbruttogehalt von 37.000 Euro (kollektivvertragliches Mindestgehalt – Überzahlung möglich). Die hochtechnologische und innovative Terma-Gruppe entwickelt Produkte und Systeme für Verteidigungs-, Nichtverteidigungs- und Sicherheitsanwendungen, darunter Befehls- und Kontrollsysteme, Radarsysteme, Selbstschutzsysteme für Flugzeuge und Schiffe, Raumfahrttechnik und Flugzeugstrukturen für die Flugzeugindustrie. Terma hat seinen Hauptsitz in Aarhus, Dänemark. International verfügt Terma über Tochtergesellschaften und Niederlassungen in den Niederlanden, Deutschland, Frankreich, Großbritannien, Österreich, der Tschechischen Republik, Rumänien, den Vereinigten Arabischen Emiraten, Indien, Singapur und den USA. Der Geschäftsbereich Raumfahrt trägt mit auf Missionen zugeschnittenen Software- und Hardwareprodukten, einschließlich Stromversorgungssystemen und Sternverfolgungssystemen, sowie Dienstleistungen zur Unterstützung mehrerer wegweisender europäischer wissenschaftlicher und Erdbeobachtungssatellitenmissionen im Orbit bei. Darüber hinaus ist Terma mit der Entwicklung und Lieferung von Software- und Hardwaresystemen und Dienstleistungen für zahlreiche laufende und zukünftige europäische und internationale Missionen beauftragt. Terma Space operiert von Dänemark, den Niederlanden, Deutschland, Frankreich, Großbritannien, Österreich, der Tschechischen Republik und Rumänien aus. Application deadline:As soon as possible Job Type: Full-time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your assignment:      You ensure that our space instruments can be assembled, aligned and tested according to the specifications.    You are responsible for the test- &amp; assembly procedures and consult with the design office for the development of tools (hard-&amp; software) for our space projects.    You take care of the Assembly, Integration and Tests of our space projects (ao in the cleanroom).    You support quality reviews and Root Cause Analysis.    You participate in test campaigns, responsible for all assembly related issues during the test campaign.    You document and Report progress with internal and external partners.    You ensure that test instruments and facilities are in accordance to requirements for existing and upcoming projects.    You standardize maintenance and calibration routines and document equipment and facilities.     Your profile:      You have a degree in Industrial Engineering, Aerospace Engineering,… and/or relevant technical experience in aerospace sector.    You are familiar with a high-tech working environment.    You are quality minded and work very accurately.    You fluently speak and write English.     We offer you:      The possibility to take part in the development of high technological products.    Employment in an enthusiastic team driven by new technology.    A competitive salary, supplemented with interesting extra-legal benefits (group and hospitalisation insurance, meal vouchers, internet allowance, and lots of learning possibilities).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our cities are changing. The shift towards sustainable mobility coupled with an ever increasing density is shaping the new urban landscape. Key challenges are arising such as:      How can we free-up space in our streets and give it back to pedestrians and cyclists without ignoring the impact on drivers?    How can we enable the electrification of vehicles with the suitable charging infrastructure?    Where should all the bicycles, cargo bikes, and scooters go at the end of the ride?     BePark aims to provide a better mobility experience to this generation and the next. In short, we hunt for unused private parkings and open them to the crowd for various uses: car park (keeping cars off-street), bicycles, EV charging, Last-mile delivery...   Our goal is ultimately to generate a network of mobility hubs throughout cities in France, Belgium and Luxembourg.   Today we are a team of 25 delivering mobility services across 500 parking lots for our community of 16k active users. Let's grow this network together !   Requirements   As a Sales Development Representative, you will integrate the B2B sales team focused on corporate users. Parking can be a real headache for companies, and your job is to find the right solution fitting their specific challenge. BePark can provide corporates with external parking solutions, flexible contracts and software solutions to better manage their parking usage and implement their own mobility policy at the parking level.   Your main responsibility is to hunt for new prospects in pain, understand their situation and bring them to a discussion with an Account Executive with whom you work in perfect pairs!   About you      You are fluent in French and proficient in Dutch ( mandatory)    You enjoy social contact and meeting new people    You are solution-oriented and proactive, with an entrepreneurial mindset    You are customer-centric, obsessed with your clients’ pains to generate leads    You show resilience in your contacts with prospects and be extremely attentive    You are organized, rigorous and independent in your work     Benefits      Competitive package, in line with your sales performance (we do not cap commissions)    Work with top-tier tools (CRM, Automated prospection, Project Management tools)    Build/Develop a deep knowledge of Mobility and Real Estate sectors    Be a part of a young, innovative and fast growing SME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VITO develops technology to facilitate the transition to a more sustainable society and economy. One of the key technologies applied in this context is Remote Sensing. With the increasing number of satellites, drones, processing facilities and technologies like artificial intelligence, the opportunities with remote sensing are larger than ever.             Meanwhile the Remote Sensing team of VITO counts more than 100 motivated scientists, IT engineers and project managers. To facilitate the growth of our ambitions we are looking for an extra colleague, more specifically a Business Developer with focus on the institutional market.             Your tasks:              You will be full time employed as Business Developer in VITO’s Remote Sensing team. This means that you will scout opportunities in the institutional market. The main clients will be European Institutes like the European Commission, EC’s Joint Research Institute, the European Space Agency, the European Centre for Medium-Range Weather Forecasts, the European Environment Agency, etc. While the focus will be on these European clients, also international Clients like the United Nations might be targeted.        You will scout interesting opportunities that fit our strategy and goals and manage the entire bid process.        You don’t have to be an expert in remote sensing, GIS or data science. But a sound understanding of these domains and knowledge of the ecosystem in which we operate is a strong asset.        Outside VITO you will communicate frequently with clients and partners. Hence, excellent writing and presenting skills are key.                                                 You hold a Master or PhD degree related to bioscience engineering, engineering science, or environmental sciences;       You have proven knowledge and expertise in the management of large tenders, involving many partners. Experience in all core bid duties like consortium building, financial negotiation, strategy development, and coordination of the writing;       Knowledge of the European funding landscape is key;       A project management certificate is an asset but not a strict requirement;       You have strong customer focus and you are a born negotiator;       You have the ability to make decisions, act on your own initiative and operate in a pro-active way;       You have excellent writing and presentation skills in English.                Offer            We work 'activity-based', our activities bring us to our location. Our headquarter is in Mol. Hybrid work arrangements and/or working in a satellite office in Antwerp-Berchem, Ghent, Ostend or Genk is possible.       A competitive salary with a range of benefits, including allowances, insurance and a modular package of holidays.       Innovation is our asset, so it goes without saying that we give our employees the opportunity to take additional training courses and stay up-to-date in their field. You will always have the opportunity to broaden your knowledge and discover new technologies.       You will have the opportunity to be part of an organization with an international reputation, known for its cutting-edge technological research and scientific consultancy.       With us, you will contribute directly to sustainable developments at local, national and global level through your innovative applications. You provide answers to contemporary societal challenges.       Moreover, we highly value a good work-life balance at VITO! This is achieved by adopting a flexible attitude depending on your specific needs.            Are you the experienced, highly motivated candidate we are looking for? Don't hesitate and apply now!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">About Antwerp Space    Antwerp Space is a leading Belgian space engineering company and an industrial player well-recognized by the European Space Agency and the European Commission. Antwerp Space has an established presence in the European space market and in several cases is taking the lead in technically complex space projects, supported by a consortium of partners from all over Europe.    The company employs around 50 highly skilled engineers and technicians from all over the world, the majority of whom hold an engineering degree, with strong expertise in the areas of digital signal processing, hardware and software design, as well as in project management and technical leadership.    OHB SE Group    Antwerp Space is part of the OHB SE group, one of Europe’s success stories in the field of contemporary space. Today it can call itself the third largest space group in Europe.    The OHB SE group has been growing at a steady pace over the last three decades and its footprint in Europe has continuously expanded. Nowadays, there are subsidiaries in Austria, Germany, Italy, Sweden, Luxembourg, Greece, the Czech Republic and Belgium. Despite its size, OHB SE is still a family business, run by the Fuchs family.    Who are we looking for?   Required technical competences      Master’s degree in Electronics, Space Engineering, or equivalent expertise.    At least 2 years of relevant work experience in the aerospace sector.    Eligible to obtain a National and EU security clearance is mandatory.    Proficiency in LabVIEW and Python development is essential.    Basic understanding and a high interest in digital communications theory and signal processing in the RF communications domain.    Basic understanding and a high interest in Global Navigation Satellite Systems (GNSS).    Basic knowledge of electronics (schematics, EMI, testability)    Ideally some experience with RF test equipment such as a spectrum analyzer, signal generator, power meter, etc.    Your home base location allows working on a regular basis at the Hoboken office and sporadic at the Leuven office.    Occasional business trips mean a welcome change from your daily work.     Expected soft skills      Open-minded towards new ideas and willing to learn    Effective interpersonal and teamwork skills    Strong analysis and problem-solving skills    Good verbal and written communication skills in English (mandatory)     Where do you fit in?    The AIT team is responsible for assembly, integration and verification of the challenging communication and navigation products of Antwerp Space. Within the AIT team, you are mainly responsible for the verification of the RF products. Product testability starts with the requirements definition followed by model philosophy, test bench design, AIV plan and procedures and finally the performance and compatibility verification. You will work closely with all the engineering teams, product assurance, and our international customers. As a member of the Antwerp Space AIT team, you will contribute to the many fascinating international satellite communication and navigation projects.  Your main responsibilities will be:       Developing test benches for RF communication and navigation products    Work closely with all the engineering teams to design an efficient system architecture and bring new products from prototype to production, with a strong focus on testability.    Shape the technical requirements and define the test strategy for our projects.    Take ownership of all test related documents, test execution and post processing of the results.    Conduct environmental compatibility verification (Thermal vacuum, EMC, Vibration, Shock) of the RF products, including testing at external facilities in Europe.    Verify interfaces typical to space products, such as MIL-STD-1533, Space Wire, SPI, RS422.    Engage in hands-on debugging and testing within our labs.    Utilize high-end RF test equipment, such as a spectrum analyzer, signal generator, power meter, and constellation simulator.     What we can offer you?       A multicultural environment. You’ll be working in an international environment with colleagues from all over the world.    A strong corporate culture. Our company is based on strong values: respect, trust, personal development and well-being.    Professional development. You’ll get the chance to learn, to share your expertise, to develop your skills and contribute to high-level, international projects in a high-tech environment.    Salary package. A very attractive salary package including numerous fringe benefits. The main job location is Hoboken, though, short-term missions abroad are part of this challenging job environment.     Come and explore Antwerp Space    At Antwerp Space we treasure our human capital. From the moment you get on board until retirement, we will be at your side to make sure you feel at home and you get the chance to travel all the way through Antwerp Space, developing yourself and growing together.    As a company with a passion for innovation we want to create a dynamic, open and enriching environment for people, where people are passionate about their work and exchange ideas &amp; expertise.    Moreover, we understand the need for a healthy working environment and we focus on the employee’s well-being, offering amongst others fruit@work, ergonomic advice and many other initiatives. We also focus on a good work-life balance, offering flexible working hours and additional holidays. Each year a number of events are organized to emphasize that it is important to have fun, relax and create a good team spirit.    Eager to join us? Get in touch!    Apply now by clicking the Apply button below and send us your motivation letter and CV. We will be get back to you soon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Joint Venture between Thales (67%) and Leonardo (33%), Thales Alenia Space is a global space manufacturer delivering, for more than 40 years, high-tech solutions for telecommunications, navigation, Earth Observation, environmental management, exploration, science and orbital infrastructures. Thanks to our diversity of skills, talents and cultures, our customers (governments, institutions, space agencies, telecommunications operators), therefore have Space to Connect, Secure &amp; Defend, Observe &amp; Protect, Explore, Travel &amp; Navigate.     We say HI* ̶ Welcome to the Thales team!     Human Intelligence     Thales in Switzerland is part of a world-leading technology group in the area of Defense &amp; Security, Training &amp; Simulation, Space and Digital Identity &amp; Security. In a world full of uncertainties, we ensure that our customers, partners and employees can break new ground with confidence and in security. For a future we can all trust.     Say HI* to your career as a   PCB Layouter/Hardware Solution Engineer 80-100% (m/f/d)   in Zürich #LI-HYBRID (Ref. Nr. R0231121)     In Zurich awaits you a center of excellence for optical, quantum-based communications and opto-electronic observation and communication systems used in satellite and space technology. This is the place for you if you don't just dream of space travel, but want to work on the development, operation and deployment of satellite-based systems that help position and connect everything and everyone everywhere, observe our planet and optimize the use of Earth's resources - and of our solar system. Join the team of experts at Thales Alenia Space, a key partner for governments, institutions and businesses. We look forward to meeting you!     Your mission     As PCB Layouter/Hardware Solution Engineer role at Thales Alenia Space, you will:      Layout of printed circuit boards (PCB) including component placement and signal routing for space applications, prototypes and test equipment    Layout of printed circuit board (PCB) for circuit card assemblies (CCA) according to ECSS/MIL/IPC standards    Close collaboration with design engineers    Maintenance of component library    Capture schematics symbols and footprints for EEE components    Documentation of the activities and results    Generation and release of manufacturing files including assembly drawings, Gerber files and parts lists    Participation in internal and external design reviews    Interdisciplinary collaboration with mechanical, thermal and test engineering    Ability to follow internal design guidelines and contribution for continuous improvement       We look forward to that      Technical education (university degree) in electrical engineering or similar    Practical experience in PCB layout for electronics hardware (minimum 5 years industry experience)    Experience with PCB layout of rigid, flex, rigid-flex and similar PCB technologies    Experience in PCB design for analog, digital, mixed-signal and power conversion (applications like control boards, power converters, communication electronics)    Experience in Design for Testing (DfT) and Design for Manufacturing (DfM)    Good knowledge of eCAD design tools like Mentor Graphics Xpedition    Experience with RF design, signal and power integrity simulation is an advantage    Fluent in English, German (spoken) and/or French is an advantage    Experience with SAP is an advantage    Good team player also within interdisciplinary teams    Strong communication and collaboration skills    A structured, methodical working method    Ability to proactively find solutions       What awaits you at our location in Zurich   For our 77,000 employees in 68 countries, we open up forward-looking perspectives, realize individual career paths and enable creative freedom. We achieve this through courage, diversity, and the determination to make the demanding challenges of our time safer and more inclusive. With our sustainable, value-oriented employee management, we actively advocate diversity.     Say HI* – Your way to us   When the writing is on the wall, our international teams are there to tackle today's complexity with tomorrow's industry-leading technologies. Are you in? Your contact Frederic Martin is looking forward to receiving your online application via our career portal.     Frederic Martin   Talent Acquisition Partner   #LI-FM1     Notice for recruitment agencies:   Unfortunately, due to unforeseen circumstances, we regret to inform you that the CVs submitted by recruitment agencies are not processed. We will take into consideration only the CVs submitted by the candidates.   We appreciate your understanding to Thales recruitment processes.   At Thales Alenia Space we provide CAREERS and not only jobs. With Thales Alenia Space employing around 8,900 employees in 10 countries with 17 sites in Europe and a plant in the US, our mobility policy enables employees each year to develop their careers at home and abroad. Thales Alenia Space sees space as a new horizon, helping to build a better, more sustainable life on Earth #SpaceForLife. Great journeys start here, apply now!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLM PROJECT MANAGER (f/m/d)  PLM PROJECT MANAGER (f/m/d) : CAx/ custom engineering tools/ international matrix organization/Stakeholder Management / Communication skills / English/German/French  Project: For our customer based in Zurich we are looking for a highly qualified PLM PROJECT MANAGER (f/m/d).  Background: Our Client, headquartered in Zurich, Switzerland, is the first startup to combine agility, speed and innovation with decades of experience and p ro v e n q u a l i t y . Around 1600 e m p l o y e e s at 12 locations in six countries (Switzerland,Sweden, Austria, Germany, USA and Finland) develop and manufacture products for satellites and launch vehicles with the goal of advancing humankind and enabling the exploration of the world and beyond. Our Client is the preferredsupplier of structures for all types of launch vehicles and a leader in selected satellite products and for constellationsin the New Space sector. Our Client also uses its space knowledge for applications outside of space technology:The high-precision products have already been used in the semiconductor industry for more than 20 years. Job description: We have recently launched a major PLM and engineering transformation initiative, taking the company to the next generation, and are looking for the right person to drive the project. A person with key skills in project management and operations of complex PLM projects including system introduction and support as well as being able to drive change – to bring our colleges along on the journey. Focus of your work is change management and the management of the PLM implementation, external partners collaboration, engineering application landscape simplification, related projects, and introduction/ consolidation of new/existing processes.  The Perfect Candidate: As project manager, you are responsible for the planning, implementation, and documentation of related initiatives. You will guide the project team in the creation of requirements and functional specifications, be responsible for solution design and the implementation. You further ensure that the project targets are achieved within time, budget, and quality.  Tasks &amp; Responsibilities: * Partner to business for successful implementation and organization change management * Lead PLM system (Teamcenter) implementation and participate in end-to-end Digital transformation * Define strategies for Data migration, Design data management, BOM management, Change Management, MES, ERP &amp; downstream system integration * Developing architectural blueprints for PLM, CAD, PLM-ERP interfaces &amp; downstream systems * Further optimization of applications landscape for Multi-PLM, MES, M-CAD, E-CAD, FEM systems and future R&amp;D tools * Evaluating business problems, their financial impacts, proposing solutions and driving change for key results * Own decommissioning strategies for PLM / CAD systems * Manage and train the Power User organization and create, review, and validate work instructions and training materials  Must Haves: * Min. 7-10 years of working experience in a similar role and proven strengths in PLM and CAx technologies * Operational experience in CAx and custom engineering tools e.g. Siemens Teamcenter, NX, CATIA, SAP, IFS, Windchill, 3D experience. * Very good functional understanding and usage of various Teamcenter modules like BMIDE, Structure Manager, Workflow Designer, Change Management, BOM Configuration methodologies, Active Workspace, ERP interfaces ( e.g T4S) , OpsCenter and MES * Ability to work in an international matrix organization and manage stakeholders and facilitate decision making in an international group organization * Strong communications skills in English; French nice to have  Reference Nr.: 923402SDA Role: PLM PROJECT MANAGER (f/m/d) Industrie: Space Research Workplace: Zurich Pensum: 100% Start: ASAP Duration: 3++  Job Type: 100%  Schedule:  8 Hour Shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">About us:       One team. Global challenges. Infinite opportunities. At Viasat, we’re on a mission to deliver connections with the capacity to change the world. For more than 35 years, Viasat has helped shape how consumers, businesses, governments and militaries around the globe communicate. We’re looking for people who think big, act fearlessly, and create an inclusive environment that drives positive impact to join our team.   What you'll do:    As a Payload Systems Engineer, you will join a team focused on the forefront of technology for innovative satcom architectures. You have hands-on experience in designing sophisticated communication space payloads. This also includes knowledge of communication chains, transponders, onboard processing units for digital regenerative applications, beam forming, distribution units and power management.   You thrive in an R&amp;D framework environment and are passionate about continuous improvements. The ideal candidate will enjoy working on a variety of workflows from system definition to requirements downflow, reviewing subsystem design/co-design. Additionally, experience of manufacturing, integration, testing, and qualification is also a plus! The day-to-day:    Together with the team, you will lead the mission analysis for communication space system requirements and down-flows. You will being responsible for the SWaPC analysis and defining interfaces (digital, electrical, RF, optical, mechanical/thermal, etc.) and help to drive and facilitate discussions with subcontractors/partners as needed.   As the SME, you will work and challenge external contractors on technical matters. Together with the team, you will assist with reliability analysis including simulations and design choices with supporting space qualification activities such as bus selection and components. You will also assist with program management and B&amp;P, including collaborating with customers on programmatic and schedule matters. Finally, you will help to support test procedures, participate in the integration, launch, and in-orbit commissioning, and be involved in preparing presentations and reports for the full development (design reviews, test activities, manufacturing, qualifications, progress review, etc.) What you'll need:       The successful candidate should meet the following requirements:          MS/PhD in Engineering (SatCom system, Telecommunications, Electronics, Digital Systems, Automation, etc.)      8-10 years of proven experience in the following areas:      SatCom and communication Payload architectures for LEO/MEO/GEO/HEO      HW/SW design, development, and integration for space applications      Digital design for space communications and Digital regenerative payloads      Inter-satellite links and digital phased array antennas      Experience with orbital analysis tools, Telemetry, Tracking, and Control (TT&amp;C) platform, and Ansys Systems Tool Kit (STK).      Experience with operations, including satellite TT&amp;C operations, payload operations, users, and network management facilities      Swiss or EU (27) Citizenship or valid Swiss working permit       What will help you on the job:      Previous experience working with ESA/NASA in Telecoms programs is a plus!    A proactive person who enjoys working being challenged and working as part of a diverse international team.     ___________   #LI-EMEA : At Viasat, we consider many factors when it comes to compensation, including the scope of the position as well as your background and experience. Base pay may vary depending on job-related knowledge, skills, and experience. Additional cash or stock incentives may be provided as part of the compensation package, in addition to a range of medical, financial, and/or other benefits, dependent on the position offered. Learn more about Viasat’s comprehensive benefit offerings that are focused on your holistic health and wellness at https://careers.viasat.com/benefits. EEO statement:       Viasat is proud to be an equal opportunity employer, seeking to create a welcoming and diverse environment. All qualified applicants will receive consideration for employment without regard to race, color, religion, gender, gender identity or expression, sexual orientation, national origin, ancestry, physical or mental disability, medical condition, marital status, genetics, age, or veteran status or any other applicable legally protected status or characteristic. If you would like to request an accommodation on the basis of disability for completing this on-line application, please click here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">good food, healthy environment    The 'Digital Production' Research Group makes use of information and communication technologies to solve a wide variety of challenges in the agricultural sector. The Group develops new data-based solutions for improving the efficiency and sustainability of production systems. In addition to the understanding of agricultural production processes, our core competencies lie in computer vision, demanding data analyses and modelling.        Nitrogen fertilisation can be made more efficient with site-specific technologies. This project aims to optimise the individual fertiliser applications by taking into account soil mineralisation. Mineralisation models and innovative nitrate sensors will be evaluated for their suitability for practical application.                 Your tasks            Validate and further develop existing mineralisation models with regard to their practical suitability       Analysing data sets from field experiments and linking them with other data sources (e.g. weather data, satellite data).       Planning and conducting field experiments on N-mineralisation in soil       Writing scientific publications       Participation in scientific conferences and earning the required ECTS credits                             Your profile            University degree in agricultural sciences, biology, environmental sciences or equivalent qualification       Interest in mechanistic and statistical modelling of the soil-plant system       Good knowledge of R or Python       Experience in analysing spatial data with ArcGIS or QGIS is an advantage       Knowledge of two official Swiss languages and a very good command of written and spoken English                    Additional information    If this position interests you and you meet the requirements profile, we look forward to receiving your online application.    (English is not an official Swiss language, please choose German, French or Italian as correspondence language).        Additional information can be obtained from Thomas, Anken, in charge of the Group Digital Production by e-mail at or by phone on N° +41 58 480 33 52 (please do not send applications to this e-mail address).        Starting date: 01.10.2024 or by agreement. The position is limited until 30.09.2027.        Reference number: JRQ$540-11538           Apply now           About us    The 'Sustainability Assessment and Agricultural Management' Research Division develops decision-making bases to help policy-makers create optimal framework conditions for a competitive and multifunctional Swiss agricultural sector. The analysis of a wide range of data from the agriculture and food sector enables the identification of promising operating strategies and policy measures. The Research Division deals with issues concerning digitalisation in agriculture.        Agroscope is the Swiss federal centre of excellence for research in the agriculture and food sector. Its researchers work at a number of sites in Switzerland. Headquartered in Bern-Liebefeld (as of 2026: Posieux), Agroscope is attached to the Swiss Federal Department of Economic Affairs, Education and Research EAER.        We offer you a varied job in an interesting work environment as well as thorough training and a modern research infrastructure. Flexible working hours and good employee benefits are additional perks of the job.        + more           The Federal Administration is attentive to the different needs and backgrounds of its employees and promotes diversity. Equal treatment is a top priority.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Space Research and Planetology Division at the University of Bern is seeking a highly motivated PhD student to join its esteemed Space Science Group. Our group specializes in studying the composition of tenuous gases near solar system objects using time-of-flight mass spectrometers and determining surface compositions with advanced laser ablation techniques. Notably, we developed and built the mass spectrometer for ESA's JUICE mission and are responsible for the preparation and analysis of the measurements it will conduct once the mission arrives in the Jupiter system in July 2031. To support the missions we are involved in, we have developed a sophisticated computer model for simulating planetary atmospheres, which has been successfully applied to various solar system bodies, including Mercury, the Moon, Venus, Titan, Europa, Callisto, Ganymede, and comet 67P/Churyumov-Gerasimenko.   This research project focuses on preparing measurements by the mass spectrometers on board ESA's JUICE and NASA's Europa Clipper missions to study the plumes tentatively observed on Europa, one of Jupiter's icy moons. Investigating Europa's plumes is particularly exciting because these geysers offer a rare opportunity to sample subsurface liquid reservoirs that might harbor life, without needing to drill through kilometers of ice. Analyzing these plumes could provide unprecedented insights into the moon's oceanic environment, its chemical composition, and its potential habitability.  Research Project: This PhD project will focus on modeling the complete gas phase of Europa's plumes, a critical component in determining the habitability of this ocean world in the Jupiter system. The project involves developing a physical simulation model to quantify changes in the chemical composition of Europa's plumes from their liquid reservoirs to their gas phase. The successful candidate will work with existing Monte Carlo models and newly acquired DSMC models, aiming to provide valuable insights for ESA's JUICE and NASA's Europa Clipper missions. This research is poised to significantly enhance our understanding of Europa's potential to support life and will be an integral part of the science preparation for the measurements conducted by the mass spectrometers on the JUICE mission (JUICE / NIM) and the Europa Clipper mission (Europa Clipper / MASPEX). The selected PhD student will work closely with the JUICE / NIM team and the Europa Clipper / MASPEX team, including the potential for a research visit with our US counterparts to foster collaboration and share expertise.      Key Responsibilities:        Develop and extend existing Monte Carlo and DSMC models to simulate Europa's plumes.   Analyze the chemical modifications occurring within the plume's gas phase.   Work closely with senior geochemists and DSMC modelers to integrate new chemical reaction modules into the models.   Collaborate with the JUICE/NIM and Europa Clipper/MASPEX teams to optimize plume detection and maximize the scientific return of plume measurements.   Prepare and publish at least three scientific papers based on the research findings.   Present research results at international conferences and workshops.     Qualifications:      MSc in Physics, Astrophysics, or a field related to the research project.   Proficient English language skills, both written and spoken; German language skills are a plus.   Experience in programming is highly desirable.   Strong motivation and ability to work independently as well as in a collaborative research environment.     Why Join Us:      The University of Bern offers a vibrant research environment with a rich history of contributions to space missions, including ESA's JUICE, ExoMars, CHEOPS, BepiColombo, Rosetta, Comet Interceptor, and NASA's IBEX and Artemis missions. Our Space Science Group provides an excellent opportunity to work on cutting-edge research projects with a team of experienced scientists and engineers.     Position Details and Application Instructions:      Starting Date: Flexible, but not before September 2024   Location: University of Bern, Switzerland   Salary: In accordance with the personnel regulations of the Canton of Bern   Application Deadline: 31 July 2024     Application Instructions: Submit your application as a single PDF file consisting of: 1. Cover letter describing your motivation and qualifications for the position 2. Curriculum Vitae (CV) 3. List of publications (if applicable) 4. Names and contact information of three references  Please send your application to the contact given below by 31 July 2024. For further information, visit our website: www.space.unibe.ch  Applicants should contact: PD Dr. Audrey Vorburger +41 31 684 44 16 audrey.vorburger@unibe.ch                   www.karriere.unibe.ch              Rechtliche Hinweise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applications are invited for one research assistant position (Postdoctoral fellow) at the University of Bern (Dept. of Space and Planetary Sciences) to work under the supervision of Prof. Jonas Kühn on novel instrumentation techniques for direct imaging of exoplanets. The successful applicant is expected to lead the implementation of new exoplanet imaging techniques using pixelated “Spatial Light Modulators” (SLMs) display panels. The latter can be used as “programmable focal-plane phase mask coronagraphs”, to mask the unwanted light from the host star, in order to reveal faint off-axis astrophysical sources of interest (exoplanets, circumstellar disks).   This position is part of the ERC Consolidator “RACE-GO” project (Rapid Adaptive Coronagraphy of Exoplanets from a Ground-based Observatory), which aims at investigating how SLMs could be used as “active coronagraphs” to adapt to various observing conditions, target types (binary stars, giant stars) or to implement coherent differential imaging (CDI) techniques at high-speed. The RACE-GO project team will be allocated 60 Guaranteed Time Observing (GTO) nights spread over 2 years on the new Turkish 4-m DAG Telescope, to implement, validate and scientifically exploit the approach on-sky, and the applicant is expected to technically prepare and lead the initial phase of the observing campaign.        In particular, the postdoctoral fellow will work both on instrumental aspects of adaptive coronagraphy and CDI in the optical laboratory (high-contrast imaging testbed), and will participate in the installation and on-sky commissioning of the new Programmable Liquid-crystal Active Coronagraphic exoplanet Imager for the 4-m Turkish DAG telescope (PLACID) instrument. In consequence, the applicant is expected to travel to Turkey (Erzurum province) a few times per year, and spend at least a dozen nights observing at the summit (3,100m ASL). The candidate will be able to set up his own observation program towards the end of the position, if conditions allow. Overall, she/he will also play a key role in a small team of four people, notably helping to supervise and mentor two PhD candidates in their 2nd thesis year, but also running a practical lab experiment for Physics MSc students; hence team player and teaching qualities are crucial to this position.     Requirements      A PhD degree in Physics, Astrophysics or Engineering (with specialization in astronomical instrumentation or adaptive optics), obtained within the last 2 years. Prior experience in astronomical instrumentation, observational astronomy, Python programming and/or benchtop optics is a plus.     We offer      This is initially a 1-year position, with a 2nd year extension available upon mutual agreement.        The salary starts at 90'000.- CHF/year gross salary, commensurate with experience and with 5-week paid holidays per year, according to rules of the University and Canton of Bern. Childcare allowance is available.        The University of Bern is an equal opportunity employer committed to diversity in its workplace, and applications from under-represented minorities are strongly encouraged.        The University of Bern is a vibrant center of space and (exo)planetary research. It leads the National Center for Competence in Research PlanetS (www.nccr-planets.ch), a Swiss research network focused on planetary science, which includes more than 130 scientists from the Universities of Bern, Geneva , Zurich and ETH Zurich. The University of Bern also hosts the Center of Space and Habitability (www.csh.unibe.ch), and is the leading house of the ESA exoplanet transit satellite CHEOPS. The city of Bern offers an excellent living environment, with its 12th-century UNESCO world heritage old town within close vicinity of the Swiss Alps, and is consistently ranked as one of the world's best city for quality of living (e.g. Top 15 in Mercer survey).     Applications      The following application materials should be sent as a single pdf file to jonas.kuehn@unibe.ch:               A motivation letter including contact details, information on skills and previous experience, and the names of 2-3 references/referees (max. 3 pages).    Curriculum vitae (max. 2 pages), plus a list of publications (not included in page count).    Academic transcripts of PhD and MSc grades.       Two to three letters of recommendation should be sent directly to Prof. Kuhn by the referees themselves, and it is the responsibility of the applicant to ensure that the letters are sent on due date.        Deadline to apply: August 15, 2024, for full consideration, then until the position is filled.        www.space.unibe.ch                         www.karriere.unibe.ch              Rechtliche Hinweise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIGENTEC is a young, dynamic and strongly growing company, headquartered in Lausanne, Switzerland, near EPFL, close to the shore of Lake Geneva. We are developing Photonic Integrated Circuits (PICs) to world-leading performance with our customers for applications in Quantum Technologies, LiDAR, Space, Biosensors and more.    To support our growth, we are looking for a:  Process Engineer  Heterogeneous Integration    Tasks    Within LIGENTEC’s engineering team, our mission is to bring our integrated photonics platform to the next level, building on its world-class passive photonics and extending the functionality with active component integration.    Role and Responsibilities    You are part of an interdisciplinary project team that integrates active functionalities such as modulators, photodiodes and amplifiers onto LIGENTEC’s state-of-the art passives platform.        Develop new processes for new electro-optic modulators, including thin-film lithium niobate integration or other materials on SiN. To this end, you:   Define and execute Design of Experiments at the clean-room facilities.   Contribute to the project technology roadmap from a process development perspective.   Stay up to date with state-of-the art process technology development on active components.   Increase the maturity level of developed processes in order to release them for early customer engagements. To this end, you:   Implement statistical process control and physical model fitting of opto-electrical device properties.   Execute fabrication runs for photonic integrated circuits for internal and external customers.   Documentation of results with strong emphasis on correlations between optical and electrical properties of integrated actives.   Contribute to the R&amp;D and Process teams in all aspects, especially process integration topics.   Requirements        Master’s degree in electrical, chemical, physical or nano engineering.   Min of 3 years experience in relevant environments (MEMS, Semiconductors, Nano-Optics) with hands-on experience on clean room processes such as wafer bonding, lithography, etching, metallization, different material deposition and characterisation techniques.   Experience with heterogeneous integration techniques like wafer bonding, micro-transfer printing or flip-chip assembly is a plus.   Understanding of photonic devices like modulators, photodiodes and lasers is a plus.   Knowledge of python for statistical data analysis is a plus.   Excellent technical problem-solving skills   Open minded, critical, and innovative.   Ability to work independently and with remote teams.   Working proficiency in English.   Benefits        A flexible and dynamic start-up work environment.   Be a member of an international, diverse, customer-focused and highly motivated team.   Personal responsibility in your job and the chance to grow with us   Our passion to bring PICs to everyday life.   We look forward to receiving your full application, including 1) your CV, 2) a statement of interest (relating the position to your skills) and 3) grade or work certificates. Non-complete applications may not be considered.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job Introduction    Serco has made significant contributions at ESA's European Space Research and Technology Centre (ESTEC) in the Netherlands, supporting a wide range of space missions and projects. Serco has provided essential engineering, technical, and management services, playing a key role in logistics and operational support for missions. Serco's expertise in spacecraft management, ground systems and data processing has earned them recognition, including 'Best in Domain' awards from ESA. Their long-standing partnership with ESA reflects their commitment to excellence and innovation in the space sector.   On behalf of our client, the European Space Agency, we are looking for a Microsoft Software Engineer to join our team in the Netherlands.   We are looking for someone skilled with Microsoft tools such as Power User, Power Pivot and Power Query to provide maintenance support and assist the ESA Cyber Internal Audit team in conducting Cybersecurity for the Galileo Program. Main Responsibilities    As Microsoft Software Engineer you will concentrate your activities on the following:      Upgrade and maintain the current ESA GNSS CAATS (computer-assisted Audit techniques) a set of MS excel based applications using Macros and MS Virtual Basic    Develop a new set of tools to improve the current ESA GNSS CAATS.    Support for the maintenance of the ESA GNSS CIA Evidence Database, currently based on Microsoft Excel.    Integrate the inputs provided by the industry into the ESA GNSS CAATS and develop the associated tools to perform this integration. Note that some of these inputs are classified.    Develop and maintain a database with all the data inputs as the main repository of the Auditor knowledge base.    Develop the tools to validate and verify the data provided by ESA.    Develop the tools to maintain records of software Audit activities (evaluation logs, status reports) provided by ESA.    Support to the ESA GNSS CIA team for the development of specific software and scripts during the execution of the Audits.   Successful Candidate    Do you think you are the person we are looking for? See below what experience or knowledge you should bring:      Minimum a Bachelor´s degree or equivalent, preferably in the field of software engineering.    Expertise, at least, 2 years in software development    Experience in conducting projects reviews (document and SW development processes).    Experience on Generalised Audit software (GAS) or Business Intelligence tools.    Knowledge about add-ins, plugins and apps for Microsoft Office as Power User, Power Pivot, Power Query, ParallelDots, Office Tab, Tableau or other similar tools to increase the productivity of the Microsoft Office products.    Comfortable with working in a diverse and multinational team environment.    Excellent interpersonal skills are needed, together with a high degree organizational and communication abilities.    Proficient in the English language, both written and spoken.    Knowledge of another EU member state language is an asset.    Candidates must be eligible to work in the EU.   About The Company   Why should you join Serco ?   At Serco not only is the nature of the work we do important, everyone has an important role to play.   Meaningful and vital work - You’ll contribute to methodologically intercepting challenges whilst achievements will also be recognised and celebrated.   A world of opportunity - You’ll be wholeheartedly supported with development and career progression   Great people - You’ll become an integral member of a well-defined and supportive team who believe passionately in the value of our work. We are a company passionate about diversity and inclusion.   About Serco   Serco Europe has operated in the Netherlands and Spain over the past 30 years, mainly in the field of Space. Serco Netherlands and Spain have a long history of partnership and trust with the European Space Agency (ESA).   In both countries, Serco is proud to deliver the highest calibre of people and services at ESTEC (ESA’s technology and engineering hub) and ESAC (ESA’s Astronomy and Science centre).   At the heart of its business, Serco Netherlands and Spain source, train, care and support employees, enabling them to better pursue their dreams of working in the Space industry in excelling in the delivery of essential public services.        We are diverse and inclusive organisation.   At Serco, we see people first and foremost for their performance and potential and we are committed to supporting the needs of all our colleagues. It’s a mix of people from different backgrounds, experiences and opinion that keeps our culture strong and vibrant.   We believe in equity so we strongly encourage applications from a diverse range of candidates. Disabled applicants who meet the minimum criteria for the job are encouraged to apply and demonstrate their abilities in an interview. We also welcome a conversation about any adjustments that would make the interview process more accessible for you. Wherever possible we are open to discussions around flexible working and we operate a hybrid work structure in many of our business areas.   In the UK we are proud to be a Disability Confident Leader in the government’s scheme and hold the Gold Inclusive Employer Standard; in Belgium we are partner of Diversicom and member of Charter der Vielfalt in Germany.   If you have any questions please do not hesitate to reach out to The Serco Europe Recruitment Team        Important:   Any offer of employment is contingent upon you providing documents to verify your identity and employment eligibility, as required by law.   Applicants are reminded that they will be requested to produce such documentation during the recruitment process.   Please contact a member of the recruitment team if you require further details of acceptable types of documentation required for verification of identity and work authorization.   Data Protection:   For more information on how the personal data in your application is process, please see the link Data Protection policy here. Package Description    What we offer if you join our amazing team:      Flexible working policy (hybrid working)    Comprehensive and competitive benefits plan    A range of wellness activities and employee assistance programs    Casual dress code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job Description        Fugro Norway AS - Satellite Positioning Service Line is looking for a Senior Project Lead GNSS          Fugro Satellite Positioning manages a global network of reference stations, monitoring signals from GNSS (GPS, GLONASS, BeiDou and Galileo) satellites and generating corrections to significantly improve the accuracy of unaugmented GNSS signals.          Correction messages are transmitted via a robust, fault-tolerant broadcast infrastructure, providing precise, reliable, real-time satellite positioning that is accurate worldwide, 24/7 availability and full redundancy under demanding conditions.        As the leading company in our market, we offers an interesting, international and inspiring career opportunity.          What we offer:                 International work environment                 Flexible work hours                 Subsidized meals in our canteen                 On-site parking                 In-house exercise room                 Company-covered mobile phone and internet expenses                 Secure bike storage and changing/shower facilities                 Great pension and insurance benefits              Essential Duties &amp; Responsibilities:        Contribute with defining scope, goals and deliverables for projects    Manage own projects and coordinate with other project managers to deliver on business roadmap    Take initiative for and contribute to the improvement of existing Fugro Satellite Positioning products and tools    Contribute to research, development and testing of new solutions for precise GNSS applications    Stay oriented about new research and leading-edge developments in GNSS and other relevant technologies    Create and maintain good relations with suppliers, partners and clients          Desired background and preferred skills:        Deep understanding of GNSS principles like Precise Orbit Determination and Precise Point Positioning technology    Have an ability to see new possibilities and solutions and a desire to undertake challenging tasks    Familiar with Agile project management principles and the Scrum methodology    Be able to work independently, as well as being a good team member and have an open personality    Experience in multi-site multinational development organizations with matrix management          Qualifications required:        MSc candidate with education within GNSS / Geodesy    At least 3 years relevant work experience within the GNSS/Space industry    Good communication skills in both written and spoken English          Ready to take your career to the next level? Join us at Fugro Satellite Positioning and be part of something extraordinary! If you're passionate about GNSS technology and want to make a real impact in a dynamic global environment we encourage you to apply!          Disclaimer for recruitment agencies:        Fugro does not accept any unsolicited applications from recruitment agencies. Acquisition to Fugro Recruitment or any Fugro employee is not appreciated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you searching for a Postdoc position at an internationally important geodetic fundamental station and work for the benefit of the scientific community as well as your own research and society at large? At Onsala Space Observatory we are now looking for a highly motivated colleague to work with us as a Postdoctoral researcher on GNSS-related research in geodesy and geodynamics.    Project description Possible GNSS-related research topics can include, e.g., reference frames, crustal motion, glacial isostatic adjustment, atmospheric signal delays, ionospheric research, LEO-augmented GNSS, new space missions, etc. The Postdoc position is in the research group for Space Geodesy and Geodynamics. It is restricted to three years (2+1) with a review after the second year. Together we work to increase knowledge on how to best achieve a long-term sustainable planet. Our main working places are the Onsala Space Observatory, 40 km south of Gothenburg, and Chalmers University of Technology in Gothenburg.    Information about the department At the department of Space, Earth and Environment we search for answers to the really big questions. In a long time perspective, the lifecycles of stars and galaxies provide an insight into the origin and future of the universe, earth and life. We also observe our planet and the interaction between society, technology and nature in order to develop technologies, models and tools that can meet global challenges regarding natural resources, climate impact and energy supply.      Major responsibilities Your major responsibilities as a Postdoc is to perform your own and innovative research in the field of GNSS for geodesy and geodynamics. You are expected to develop and conduct your own research in close collaboration with your colleagues in the Space Geodesy and Geodynamics research group. In addition it might be beneficial for your future career to participate in teaching and outreach activities on a level of 10 per cent.    Qualifications      Relevant PhD degree in Geodesy/Geophysics/Geodynamics/Aerospace/Physics or an equivalent education, including a GNSS-related PhD thesis and experience.        Fluency in both written and spoken English.        Experience in/knowledge of computer programming in e.g. C/C++, Python, Matlab, Fortran        To qualify for the position of postdoc, you must hold a doctoral degree awarded no more than three years prior to the application deadline (according to the current agreement with the Swedish Agency for Government Employers). Exceptions from the 3-year limit can be made for longer periods resulting from parental leave, sick leave or military service. The date shown in your doctoral degree certificate is the date we use, as this is the date you have met all requirements for the doctoral degree.      Meritorious      Educational background in space geodesy, geodynamics, atmospheric sciences, computer sciences, statistics and probability        Experience in/knowledge of data analysis, computer science, parallel programming, statistics         Swedish is not a requirement but Chalmers offers Swedish courses.        Contract terms    This postdoc position is a full-time temporary employment for two/three years.        We offer     Chalmers offers a cultivating and inspiring working environment in the coastal city of Gothenburg.    Read more about working at Chalmers and our benefits for employees.        Chalmers aims to actively improve our gender balance. We work broadly with equality projects, for example the GENIE Initiative on gender equality for excellence. Equality and diversity are substantial foundations in all activities at Chalmers.        Application procedure    The application should be marked with 20240433 and written in English. The application should be sent electronically and be attached as PDF-files, as below. Maximum size for each file is 40 MB. Please note that the system does not support Zip files.        CV: (Please name the document as: CV, Surname, Ref. number) including:           CV, include complete list of publications    Previous teaching and pedagogical experiences    Two references that we can contact.        Personal letter: (Please name the document as: Personal letter, Family name, Ref. number)    1-3 pages where you:           Introduce yourself     Describe your previous research fields and main research results    Describe your future goals and future research focus, including a detailed reserch plan for the Postdoc position        Other documents:           Please provide a digital copy of your PhD thesis, as well as attested copies and transcripts of completed education, grades, etc.       Use the button at the foot of the page to reach the application form.      Please note: The applicant is responsible for ensuring that the application is complete. Incomplete applications and applications sent by email will not be considered.  Application deadline: 2024-09-30   For questions regarding the recruitment process and research, please contact: Prof. Dr. Rüdiger Haas, rudiger.haas@chalmers.se    *** Chalmers declines to consider all offers of further announcement publishing or other types of support for the recruiting process in connection with this position. ***         Chalmers University of Technology in Gothenburg conducts research and education in technology and natural sciences at a high international level. The university has 3100 employees and 10,000 students, and offers education in engineering, science, shipping and architecture. With scientific excellence as a basis, Chalmers promotes knowledge and technical solutions for a sustainable world. Through global commitment and entrepreneurship, we foster an innovative spirit, in close collaboration with wider society. Chalmers was founded in 1829 and has the same motto today as it did then: Avancez – forward.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Satellite Navigation      We are looking for a person who is excellent in understanding technical requirements and developing and improving software products, considering the existing technology stack within OHB Digital Solutions.      Your Challenge:          Perform research and development for interdisciplinary projects in the field of satellite navigation and related      Design and implement algorithms for specific problems related to GNSS      Prototype software components and modules for concept demonstration      Define and execute test plans to ensure compliance with the requirements      Document research and development results      Comply with project plans, industry standards and OHB Digital Solutions design principles and workfloww      Work within an interdisciplinary and diverse development team         Your Qualification:          Formal education (graduated or in final semesters) in Geodesy, Telematics, Physics, Software engineering, Informatics, or similar, or equivalent work experience      Experience in research related to the field of positioning, navigation and/or timing      Ability to work with cross-function and geographically distributed teams      Soft skills such as analytic thinking and result orientation      Fluent in German and/or English         …and nice to have:      Good communication skills           Experience in project management and/or working on projects with the European Space Agency      Technically proficient / conversant in GNSS Technologies      Good communication skills         We offer:          A friendly and pleasant working environment in a varied and exciting field of work in the area of precise positioning and navigation      The opportunity to learn new skills and face new challenges every day      A permanent contract in a young, well-coordinated team with flexible working hours and the opportunity to partially work in home-office      Thorough induction phase      For legal reasons, we refer to a minimum salary according to the current Collective Agreement. The actual payment is of course higher and depends on your qualifications and experience          Location: Graz or Vienna      We are looking forward to receive your application (cover letter, resume, references and certificates) including your availability and salary expectations either in German or in English.      office@ohb-digital.at            We are hiring:          Research Engineer (full-stack)      Software Engineer (full-stack)      Software Engineer (C++)      Product Manager (GNSS Signal Simulation)                   TOGETHER AGAINST JAMMING + SPOOFING</t>
   </si>
 </sst>
 </file>
@@ -354,7 +505,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -398,6 +549,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -450,8 +607,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -459,11 +620,19 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -590,620 +759,1198 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:B147"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="62" zoomScaleNormal="62" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="62" zoomScaleNormal="62" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D154" activeCellId="0" sqref="D154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B41" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="0" t="n">
+      <c r="B43" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="0" t="n">
+      <c r="B44" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="0" t="n">
+      <c r="B47" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B48" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="0" t="n">
+      <c r="B49" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="0" t="n">
+      <c r="B50" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="0" t="n">
+      <c r="B51" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="0" t="n">
+      <c r="B52" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="0" t="n">
+      <c r="B53" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="0" t="n">
+      <c r="B54" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="0" t="n">
+      <c r="B55" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="673.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="s">
+      <c r="B56" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="594.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2" t="s">
+      <c r="B57" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="0" t="n">
+      <c r="B58" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="0" t="n">
+      <c r="B59" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="0" t="n">
+      <c r="B60" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="0" t="n">
+      <c r="B61" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="0" t="n">
+      <c r="B62" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="0" t="n">
+      <c r="B63" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="0" t="n">
+      <c r="B64" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="0" t="n">
+      <c r="B65" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="326.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2" t="s">
+      <c r="B66" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="0" t="n">
+      <c r="B67" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="0" t="n">
+      <c r="B68" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="0" t="n">
+      <c r="B69" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="0" t="n">
+      <c r="B70" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="0" t="n">
+      <c r="B71" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="0" t="n">
+      <c r="B72" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="0" t="n">
+      <c r="B73" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="0" t="n">
+      <c r="B74" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="0" t="n">
+      <c r="B75" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B88" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B89" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B90" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B92" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B94" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B95" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B96" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B97" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B99" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B101" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B102" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B103" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B105" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B109" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B110" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B111" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B112" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B113" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B114" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B117" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B119" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B121" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B122" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B123" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B124" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B125" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B126" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B127" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B128" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B129" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B130" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B131" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B132" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B133" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B134" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B135" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B136" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B137" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B138" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B139" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B140" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B141" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B142" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B143" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B144" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B145" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B146" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B147" s="0" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A55" r:id="rId1" display="dpynor@bostonhale.com"/>
+    <hyperlink ref="A55" r:id="rId1" display="Business Intelligence Director Ref: BBBH4772              Location. London     Salary. Bonus, Pension     Type. Permanent           Job Description.    Global BI Director:    We are seeking a Global Business Intelligence Director to shape our future strategy and lead the design and development of core data and reporting applications. Collaborating with the Head of Systems and Integration and the Enterprise Architect, you will identify company needs, build fully automated dashboards, create our first Enterprise Data Warehouse, and execute the full strategy. You will oversee data standards and repositories to support business needs.            5 Days a week on-site in Victoria     up to 20% bonus     £7 a day contributory lunch allowance          Key Responsibilities:            Define solution architecture and delivery for data standards across all company applications, systems, and platforms.     Ensure application software aligns with data standards and reporting strategy.     Understand business processes, systems, tools, regulations, and structure to provide valuable intelligence and reporting services.     Oversee information design for application software and continuous improvement initiatives.     Manage design, coding, verification, testing, documentation, amendments, and refactoring of programs/scripts.     Approve database specifications, maintaining standards and data integrity.     Install and test complex databases and products to meet internal and customer requirements.     Design and select critical storage, data center, and client/server environments in line with industry best practices, and provide third-line escalation for global infrastructure solutions.     Redesign complex software applications or components using agreed standards, patterns, and tools.     Produce specifications for cloud-based or on-premise components for detailed design.     Support change programs or projects with technical plans adhering to enterprise and solution architecture standards, including security.     Evaluate alternative architectures for cost, performance, and scalability.     Monitor emerging technologies to assess potential impacts, threats, and opportunities.     Document and present solutions to stakeholders, including business and technical design authorities.     Evaluate potential risks and defects, analyze specifications, and customize applications.     Define and manage technology governance processes for the Information and Data landscape.     Produce documentation for application architecture, design steps, integration processes, and testing procedures.           Technical Experience required:            Strong knowledge of architecture and data methodologies, principles and frameworks.     A strong familiarity working with data platforms especially SQL server and PowerBI are a must have.           Diversity, equity and inclusion are at the heart of what we value as an organisation. Boston Hale is an equal opportunities employer and all qualified applicants will receive consideration for employment without regard to race, religion, sex, sexual orientation, age, disability or any other status protected by law.    If you are able to operate across the top-level of an organisation, have an enthusiastic and positive attitude and can explain the complicated in simple terms whilst driving a Global Organisation's BI environment towards best in class technologies and Best Practices, then please get in touch ASAP                      David Pynor      Head of Data &amp; Technology      +44 (0)20 3587 7905      dpynor@bostonhale.com"/>
+    <hyperlink ref="A115" r:id="rId2" display="elke.ebner@emtensor.com"/>
+    <hyperlink ref="A123" r:id="rId3" display="jobs@caeleste.be"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>